<commit_message>
- More work on unit conversion - Fixed AutoMatch to redraw Flowables - Updated webinars_plus_issues_... Excel sheet with todo list.
</commit_message>
<xml_diff>
--- a/HarmonizationTool/notes/webinars_plus_issues_prior_to_2015-08-01.xlsx
+++ b/HarmonizationTool/notes/webinars_plus_issues_prior_to_2015-08-01.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\lca\new_exec\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="7-21" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="7-24" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Summary" sheetId="4" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="1" r:id="rId2"/>
+    <sheet name="7-21" sheetId="2" r:id="rId3"/>
+    <sheet name="7-24" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="397">
   <si>
     <t>URLs</t>
   </si>
@@ -166,7 +171,7 @@
     <t>Change "User Preferences" to "User Metadata" or "Annotation IDs"?</t>
   </si>
   <si>
-    <t>If I click OK but not Apply, are my changes saved? </t>
+    <t>If I click OK but not Apply, are my changes saved?</t>
   </si>
   <si>
     <t>11:08</t>
@@ -187,10 +192,10 @@
     <t>13:52</t>
   </si>
   <si>
-    <t>Logger </t>
-  </si>
-  <si>
-    <t>Change Logger to Log File? Or just Log? </t>
+    <t>Logger</t>
+  </si>
+  <si>
+    <t>Change Logger to Log File? Or just Log?</t>
   </si>
   <si>
     <t>14:00</t>
@@ -303,7 +308,7 @@
   <si>
     <t>Change menu name to Dataset. 
 Change Edit Metadata to Edit Properties. (I'm focused on Properties nomenclature since I'm working in Windows, but Metadata could work here too.) 
-Change Load Data Set to Load New Dataset. </t>
+Change Load Data Set to Load New Dataset.</t>
   </si>
   <si>
     <t>0</t>
@@ -460,7 +465,7 @@
     <t>42:37</t>
   </si>
   <si>
-    <t>User should go through them because there won't be many. 4-15, typically. Can be done quickly by clicking Next and selecting resource. When done, they should see 8 of 8. </t>
+    <t>User should go through them because there won't be many. 4-15, typically. Can be done quickly by clicking Next and selecting resource. When done, they should see 8 of 8.</t>
   </si>
   <si>
     <t>43:43</t>
@@ -517,7 +522,7 @@
     <t>48:49</t>
   </si>
   <si>
-    <t>Focus on flowables tab. Green = match, yellow = no information, orange = some information but not a definitive match. </t>
+    <t>Focus on flowables tab. Green = match, yellow = no information, orange = some information but not a definitive match.</t>
   </si>
   <si>
     <t>49:50</t>
@@ -548,7 +553,7 @@
   </si>
   <si>
     <t>Nitrous Oxide. No match. User needs to know: Click on the row (in User Data or in Flowables tab?) and the HT does a second check that is slower, looking for name or CAS matching. Logic: do what's fastest first to get a match, and do the slower match (1 sec) for problem matches.
-* Enter a search. LOGGER feeds back search transaction </t>
+* Enter a search. LOGGER feeds back search transaction</t>
   </si>
   <si>
     <t>54:20</t>
@@ -635,7 +640,7 @@
     <t>1:01:45</t>
   </si>
   <si>
-    <t>Tom muses: ensure the Rename and Delete work or just remove them? I'd say remove them and put enhancements into v2.0, unless you consider dataset mgmt to be core functionality. I think flow matching and harmonization functions are more important. Let the users know in the UG how to rename or delete OUTSIDE of lcaht? </t>
+    <t>Tom muses: ensure the Rename and Delete work or just remove them? I'd say remove them and put enhancements into v2.0, unless you consider dataset mgmt to be core functionality. I think flow matching and harmonization functions are more important. Let the users know in the UG how to rename or delete OUTSIDE of lcaht?</t>
   </si>
   <si>
     <t>1:02:15</t>
@@ -656,7 +661,7 @@
     <t>Dataset menu</t>
   </si>
   <si>
-    <t>Rename Load Data Set to Reload Dataset? </t>
+    <t>Rename Load Data Set to Reload Dataset?</t>
   </si>
   <si>
     <t>1:03:20</t>
@@ -747,7 +752,7 @@
     <t>1:11:36</t>
   </si>
   <si>
-    <t>Document the choices and what they are: json, jsonld (same as json), turtle (mainly for development use), zip (prepping for openLCA - runs a separate algorithm). The zipped json choice </t>
+    <t>Document the choices and what they are: json, jsonld (same as json), turtle (mainly for development use), zip (prepping for openLCA - runs a separate algorithm). The zipped json choice</t>
   </si>
   <si>
     <t>1:12:30</t>
@@ -827,10 +832,7 @@
     <t>Add checkbox that says, "Do not show this again." it could be checked by default. Or they could uncheck it in the preferences.  (Wes)</t>
   </si>
   <si>
-    <t>Verify if this functionality works. </t>
-  </si>
-  <si>
-    <t>fixed</t>
+    <t>Verify if this functionality works.</t>
   </si>
   <si>
     <t>20:00</t>
@@ -852,7 +854,7 @@
     <t>File Menu</t>
   </si>
   <si>
-    <t>Add "Show Dataset Contents" query to File Menu </t>
+    <t>Add "Show Dataset Contents" query to File Menu</t>
   </si>
   <si>
     <t>22:57</t>
@@ -1005,14 +1007,14 @@
     <t>44:36</t>
   </si>
   <si>
-    <t>Fix coloring on flowables: water should be green.  water,fresh should be yellow. Water, salt ocean should be green. </t>
+    <t>Fix coloring on flowables: water should be green.  water,fresh should be yellow. Water, salt ocean should be green.</t>
   </si>
   <si>
     <t>46:00</t>
   </si>
   <si>
     <t>Prescribe that users match contexts and properties first. Provide justification for that (Wes). 
-TT: if you're trying to pick a flowable, you could be guided by the flowable in context and the property in other flows. You want to find the most common and accurate match. </t>
+TT: if you're trying to pick a flowable, you could be guided by the flowable in context and the property in other flows. You want to find the most common and accurate match.</t>
   </si>
   <si>
     <t>48:12</t>
@@ -1178,7 +1180,7 @@
     <t>1:12:47</t>
   </si>
   <si>
-    <t>Fix "1 rows" so it says "1 row" when there is only 1 row. </t>
+    <t>Fix "1 rows" so it says "1 row" when there is only 1 row.</t>
   </si>
   <si>
     <t>1:14:20</t>
@@ -1211,7 +1213,7 @@
     <t>Export Dialog</t>
   </si>
   <si>
-    <t> Dialog should ask you to both choose the dataset and output format</t>
+    <t>Dialog should ask you to both choose the dataset and output format</t>
   </si>
   <si>
     <t>1:18:00</t>
@@ -1227,18 +1229,113 @@
     <t>TDB should be Database
 Database is a more normal term to hear
 Put it in UI</t>
+  </si>
+  <si>
+    <t>Items to finalize prior to August 1st release</t>
+  </si>
+  <si>
+    <t>Export zipped .json can be imported to openLCA with Flows, FlowCategory, and FlowProperties mapped to master values</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Executables </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>do</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> work with the following caveats: 1) automatic loading of master files is problematic 2) export zipped .json fails due to dependency on the olca conversion tool.</t>
+    </r>
+  </si>
+  <si>
+    <t>Vector graphic created to allow sizing</t>
+  </si>
+  <si>
+    <t>User guide updated</t>
+  </si>
+  <si>
+    <t>Work on punch list</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Export of zipped .json file must adjust Exchange </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>amount</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and ImpactFactor </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">according to user data Units  </t>
+    </r>
+  </si>
+  <si>
+    <t>Tony and Tom working steadily</t>
+  </si>
+  <si>
+    <t>Executables must function on Windows.      Specs: 32-bit plus 64-bit with 1024 MB.    Users may bump up to 2048 MB JVM size.  Document which to choose and how to increase mem.</t>
+  </si>
+  <si>
+    <t>Graphical identifier to add</t>
+  </si>
+  <si>
+    <t>Mike Brown working -- in progress.  Goal is to have text in place on Wed. 7/29.  Screenshots to follow on 7/30 and 7/31.</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="H:MM:SS"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1247,22 +1344,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1270,7 +1352,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
@@ -1278,15 +1360,29 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1317,16 +1413,34 @@
         <bgColor rgb="FFC9C9C9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1335,219 +1449,188 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFC9C9C9"/>
       </left>
-      <right style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top style="thin">
         <color rgb="FFC9C9C9"/>
       </top>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top style="thin">
         <color rgb="FFC9C9C9"/>
       </top>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="44">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="33">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="21" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="21" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1606,106 +1689,466 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.85714285714286"/>
+    <col min="1" max="1" width="52.7109375" style="38" customWidth="1"/>
+    <col min="2" max="2" width="1.5703125" style="42" customWidth="1"/>
+    <col min="3" max="3" width="52.7109375" style="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>8</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>385</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="33" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="41"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="41"/>
+    </row>
+    <row r="3" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>391</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="33" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="40"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="40"/>
+    </row>
+    <row r="5" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
+        <v>393</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="33" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="40"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="40"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="38" t="s">
+        <v>394</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="33" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="40"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="40"/>
+    </row>
+    <row r="9" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="38" t="s">
+        <v>389</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="33" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="40"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="40"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="38" t="s">
+        <v>390</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>392</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://epa.connectsolutions.com/p737zn4ooqr/"/>
-    <hyperlink ref="C3" r:id="rId2" display="https://epa.connectsolutions.com/p6zbmbobl7c/?launcher=false&amp;fcsContent=true&amp;pbMode=normal"/>
-  </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1025" width="8.85546875"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D91" activeCellId="0" sqref="D91"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="11.8622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="17.8571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="28.8622448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="75"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="13.8571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.8571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.85714285714286"/>
+    <col min="1" max="1" width="11.85546875" style="3"/>
+    <col min="2" max="2" width="17.85546875" style="4"/>
+    <col min="3" max="3" width="28.85546875" style="4"/>
+    <col min="4" max="4" width="75" style="5"/>
+    <col min="5" max="5" width="13.85546875" style="5"/>
+    <col min="6" max="6" width="15.85546875"/>
+    <col min="7" max="1025" width="8.85546875"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -1724,11 +2167,11 @@
       <c r="F1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>16</v>
       </c>
@@ -1744,7 +2187,7 @@
       <c r="E2" s="14"/>
       <c r="F2" s="15"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>16</v>
       </c>
@@ -1760,7 +2203,7 @@
       <c r="E3" s="14"/>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>21</v>
       </c>
@@ -1776,7 +2219,7 @@
       <c r="E4" s="19"/>
       <c r="F4" s="20"/>
     </row>
-    <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>21</v>
       </c>
@@ -1793,7 +2236,7 @@
       <c r="F5" s="15"/>
       <c r="J5" s="22"/>
     </row>
-    <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>25</v>
       </c>
@@ -1810,7 +2253,7 @@
       <c r="F6" s="20"/>
       <c r="J6" s="22"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>25</v>
       </c>
@@ -1827,7 +2270,7 @@
       <c r="F7" s="15"/>
       <c r="J7" s="23"/>
     </row>
-    <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>25</v>
       </c>
@@ -1844,7 +2287,7 @@
       <c r="F8" s="20"/>
       <c r="J8" s="24"/>
     </row>
-    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>31</v>
       </c>
@@ -1861,7 +2304,7 @@
       <c r="F9" s="15"/>
       <c r="J9" s="22"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>31</v>
       </c>
@@ -1877,7 +2320,7 @@
       <c r="E10" s="14"/>
       <c r="F10" s="20"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>31</v>
       </c>
@@ -1893,7 +2336,7 @@
       <c r="E11" s="14"/>
       <c r="F11" s="15"/>
     </row>
-    <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>31</v>
       </c>
@@ -1909,7 +2352,7 @@
       <c r="E12" s="19"/>
       <c r="F12" s="20"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>37</v>
       </c>
@@ -1925,7 +2368,7 @@
       <c r="E13" s="14"/>
       <c r="F13" s="15"/>
     </row>
-    <row r="14" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>39</v>
       </c>
@@ -1941,7 +2384,7 @@
       <c r="E14" s="19"/>
       <c r="F14" s="20"/>
     </row>
-    <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>41</v>
       </c>
@@ -1957,7 +2400,7 @@
       <c r="E15" s="14"/>
       <c r="F15" s="15"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>44</v>
       </c>
@@ -1973,7 +2416,7 @@
       <c r="E16" s="19"/>
       <c r="F16" s="20"/>
     </row>
-    <row r="17" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>44</v>
       </c>
@@ -1989,7 +2432,7 @@
       <c r="E17" s="19"/>
       <c r="F17" s="15"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>44</v>
       </c>
@@ -2005,7 +2448,7 @@
       <c r="E18" s="19"/>
       <c r="F18" s="20"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>44</v>
       </c>
@@ -2021,7 +2464,7 @@
       <c r="E19" s="19"/>
       <c r="F19" s="15"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>50</v>
       </c>
@@ -2037,7 +2480,7 @@
       <c r="E20" s="19"/>
       <c r="F20" s="20"/>
     </row>
-    <row r="21" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>53</v>
       </c>
@@ -2053,7 +2496,7 @@
       <c r="E21" s="14"/>
       <c r="F21" s="15"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>55</v>
       </c>
@@ -2069,7 +2512,7 @@
       <c r="E22" s="19"/>
       <c r="F22" s="20"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>58</v>
       </c>
@@ -2085,7 +2528,7 @@
       <c r="E23" s="14"/>
       <c r="F23" s="15"/>
     </row>
-    <row r="24" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>61</v>
       </c>
@@ -2101,8 +2544,8 @@
       <c r="E24" s="19"/>
       <c r="F24" s="20"/>
     </row>
-    <row r="25" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="11" t="n">
+    <row r="25" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
         <v>0</v>
       </c>
       <c r="B25" s="12" t="s">
@@ -2117,7 +2560,7 @@
       <c r="E25" s="14"/>
       <c r="F25" s="15"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>66</v>
       </c>
@@ -2133,7 +2576,7 @@
       <c r="E26" s="19"/>
       <c r="F26" s="20"/>
     </row>
-    <row r="27" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>69</v>
       </c>
@@ -2149,7 +2592,7 @@
       <c r="E27" s="14"/>
       <c r="F27" s="15"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>72</v>
       </c>
@@ -2165,7 +2608,7 @@
       <c r="E28" s="19"/>
       <c r="F28" s="20"/>
     </row>
-    <row r="29" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>75</v>
       </c>
@@ -2181,7 +2624,7 @@
       <c r="E29" s="14"/>
       <c r="F29" s="15"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>75</v>
       </c>
@@ -2197,7 +2640,7 @@
       <c r="E30" s="14"/>
       <c r="F30" s="20"/>
     </row>
-    <row r="31" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>75</v>
       </c>
@@ -2213,7 +2656,7 @@
       <c r="E31" s="14"/>
       <c r="F31" s="15"/>
     </row>
-    <row r="32" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>75</v>
       </c>
@@ -2229,7 +2672,7 @@
       <c r="E32" s="14"/>
       <c r="F32" s="25"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
         <v>75</v>
       </c>
@@ -2245,7 +2688,7 @@
       <c r="E33" s="19"/>
       <c r="F33" s="20"/>
     </row>
-    <row r="34" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
         <v>82</v>
       </c>
@@ -2261,7 +2704,7 @@
       <c r="E34" s="19"/>
       <c r="F34" s="20"/>
     </row>
-    <row r="35" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
         <v>84</v>
       </c>
@@ -2277,7 +2720,7 @@
       <c r="E35" s="19"/>
       <c r="F35" s="20"/>
     </row>
-    <row r="36" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
         <v>86</v>
       </c>
@@ -2293,7 +2736,7 @@
       <c r="E36" s="19"/>
       <c r="F36" s="20"/>
     </row>
-    <row r="37" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="27" t="s">
         <v>86</v>
       </c>
@@ -2309,7 +2752,7 @@
       <c r="E37" s="19"/>
       <c r="F37" s="20"/>
     </row>
-    <row r="38" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
         <v>89</v>
       </c>
@@ -2325,7 +2768,7 @@
       <c r="E38" s="19"/>
       <c r="F38" s="20"/>
     </row>
-    <row r="39" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
         <v>92</v>
       </c>
@@ -2341,7 +2784,7 @@
       <c r="E39" s="19"/>
       <c r="F39" s="20"/>
     </row>
-    <row r="40" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
         <v>95</v>
       </c>
@@ -2355,7 +2798,7 @@
       <c r="E40" s="19"/>
       <c r="F40" s="20"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
         <v>97</v>
       </c>
@@ -2373,7 +2816,7 @@
       </c>
       <c r="F41" s="20"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
         <v>102</v>
       </c>
@@ -2389,7 +2832,7 @@
       <c r="E42" s="19"/>
       <c r="F42" s="20"/>
     </row>
-    <row r="43" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="27" t="s">
         <v>105</v>
       </c>
@@ -2405,7 +2848,7 @@
       </c>
       <c r="F43" s="20"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
         <v>107</v>
       </c>
@@ -2421,7 +2864,7 @@
       </c>
       <c r="F44" s="20"/>
     </row>
-    <row r="45" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="28" t="s">
         <v>109</v>
       </c>
@@ -2437,7 +2880,7 @@
       <c r="E45" s="19"/>
       <c r="F45" s="20"/>
     </row>
-    <row r="46" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="29" t="s">
         <v>111</v>
       </c>
@@ -2455,7 +2898,7 @@
       </c>
       <c r="F46" s="20"/>
     </row>
-    <row r="47" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="28" t="s">
         <v>113</v>
       </c>
@@ -2471,7 +2914,7 @@
       <c r="E47" s="19"/>
       <c r="F47" s="20"/>
     </row>
-    <row r="48" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="28" t="s">
         <v>115</v>
       </c>
@@ -2489,7 +2932,7 @@
       </c>
       <c r="F48" s="20"/>
     </row>
-    <row r="49" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="28" t="s">
         <v>117</v>
       </c>
@@ -2507,7 +2950,7 @@
       </c>
       <c r="F49" s="20"/>
     </row>
-    <row r="50" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="28" t="s">
         <v>120</v>
       </c>
@@ -2523,7 +2966,7 @@
       <c r="E50" s="19"/>
       <c r="F50" s="20"/>
     </row>
-    <row r="51" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="28" t="s">
         <v>122</v>
       </c>
@@ -2539,7 +2982,7 @@
       <c r="E51" s="19"/>
       <c r="F51" s="20"/>
     </row>
-    <row r="52" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="28" t="s">
         <v>125</v>
       </c>
@@ -2557,7 +3000,7 @@
       </c>
       <c r="F52" s="20"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="28" t="s">
         <v>128</v>
       </c>
@@ -2573,7 +3016,7 @@
       <c r="E53" s="19"/>
       <c r="F53" s="20"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="28" t="s">
         <v>130</v>
       </c>
@@ -2591,7 +3034,7 @@
       </c>
       <c r="F54" s="20"/>
     </row>
-    <row r="55" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="28" t="s">
         <v>132</v>
       </c>
@@ -2609,7 +3052,7 @@
       </c>
       <c r="F55" s="20"/>
     </row>
-    <row r="56" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="28" t="s">
         <v>134</v>
       </c>
@@ -2627,7 +3070,7 @@
       </c>
       <c r="F56" s="20"/>
     </row>
-    <row r="57" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="28" t="s">
         <v>136</v>
       </c>
@@ -2643,7 +3086,7 @@
       <c r="E57" s="19"/>
       <c r="F57" s="20"/>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="28" t="s">
         <v>138</v>
       </c>
@@ -2661,7 +3104,7 @@
       </c>
       <c r="F58" s="20"/>
     </row>
-    <row r="59" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="29" t="s">
         <v>95</v>
       </c>
@@ -2677,7 +3120,7 @@
       </c>
       <c r="F59" s="20"/>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="29" t="s">
         <v>141</v>
       </c>
@@ -2695,7 +3138,7 @@
       </c>
       <c r="F60" s="20"/>
     </row>
-    <row r="61" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="29" t="s">
         <v>143</v>
       </c>
@@ -2711,7 +3154,7 @@
       <c r="E61" s="19"/>
       <c r="F61" s="20"/>
     </row>
-    <row r="62" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="29" t="s">
         <v>145</v>
       </c>
@@ -2729,7 +3172,7 @@
       </c>
       <c r="F62" s="20"/>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="29" t="s">
         <v>147</v>
       </c>
@@ -2747,7 +3190,7 @@
       </c>
       <c r="F63" s="20"/>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="29" t="s">
         <v>150</v>
       </c>
@@ -2763,7 +3206,7 @@
       <c r="E64" s="19"/>
       <c r="F64" s="20"/>
     </row>
-    <row r="65" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="29" t="s">
         <v>152</v>
       </c>
@@ -2779,7 +3222,7 @@
       <c r="E65" s="19"/>
       <c r="F65" s="20"/>
     </row>
-    <row r="66" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="29" t="s">
         <v>154</v>
       </c>
@@ -2797,7 +3240,7 @@
       </c>
       <c r="F66" s="20"/>
     </row>
-    <row r="67" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="29" t="s">
         <v>156</v>
       </c>
@@ -2815,7 +3258,7 @@
       </c>
       <c r="F67" s="20"/>
     </row>
-    <row r="68" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="29" t="s">
         <v>158</v>
       </c>
@@ -2831,7 +3274,7 @@
       <c r="E68" s="19"/>
       <c r="F68" s="20"/>
     </row>
-    <row r="69" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" s="29" t="s">
         <v>160</v>
       </c>
@@ -2849,7 +3292,7 @@
       </c>
       <c r="F69" s="20"/>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="29" t="s">
         <v>162</v>
       </c>
@@ -2865,7 +3308,7 @@
       <c r="E70" s="19"/>
       <c r="F70" s="20"/>
     </row>
-    <row r="71" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="29" t="s">
         <v>164</v>
       </c>
@@ -2883,7 +3326,7 @@
       </c>
       <c r="F71" s="20"/>
     </row>
-    <row r="72" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="29" t="s">
         <v>166</v>
       </c>
@@ -2899,7 +3342,7 @@
       <c r="E72" s="19"/>
       <c r="F72" s="20"/>
     </row>
-    <row r="73" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="29" t="s">
         <v>168</v>
       </c>
@@ -2917,7 +3360,7 @@
       </c>
       <c r="F73" s="20"/>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="29" t="s">
         <v>170</v>
       </c>
@@ -2933,7 +3376,7 @@
       <c r="E74" s="19"/>
       <c r="F74" s="20"/>
     </row>
-    <row r="75" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="29" t="s">
         <v>172</v>
       </c>
@@ -2951,7 +3394,7 @@
       </c>
       <c r="F75" s="20"/>
     </row>
-    <row r="76" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A76" s="29" t="s">
         <v>174</v>
       </c>
@@ -2969,7 +3412,7 @@
       </c>
       <c r="F76" s="20"/>
     </row>
-    <row r="77" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="29" t="s">
         <v>176</v>
       </c>
@@ -2987,7 +3430,7 @@
       </c>
       <c r="F77" s="20"/>
     </row>
-    <row r="78" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="29" t="s">
         <v>178</v>
       </c>
@@ -3005,7 +3448,7 @@
       </c>
       <c r="F78" s="20"/>
     </row>
-    <row r="79" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="29" t="s">
         <v>180</v>
       </c>
@@ -3023,7 +3466,7 @@
       </c>
       <c r="F79" s="20"/>
     </row>
-    <row r="80" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="29" t="s">
         <v>182</v>
       </c>
@@ -3039,7 +3482,7 @@
       <c r="E80" s="19"/>
       <c r="F80" s="20"/>
     </row>
-    <row r="81" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="29" t="s">
         <v>184</v>
       </c>
@@ -3055,7 +3498,7 @@
       <c r="E81" s="19"/>
       <c r="F81" s="20"/>
     </row>
-    <row r="82" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A82" s="29" t="s">
         <v>186</v>
       </c>
@@ -3073,7 +3516,7 @@
       </c>
       <c r="F82" s="20"/>
     </row>
-    <row r="83" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="29" t="s">
         <v>188</v>
       </c>
@@ -3091,7 +3534,7 @@
       </c>
       <c r="F83" s="20"/>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="29" t="s">
         <v>190</v>
       </c>
@@ -3109,7 +3552,7 @@
       </c>
       <c r="F84" s="20"/>
     </row>
-    <row r="85" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="29" t="s">
         <v>190</v>
       </c>
@@ -3125,7 +3568,7 @@
       <c r="E85" s="19"/>
       <c r="F85" s="20"/>
     </row>
-    <row r="86" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A86" s="29" t="s">
         <v>194</v>
       </c>
@@ -3141,7 +3584,7 @@
       <c r="E86" s="19"/>
       <c r="F86" s="20"/>
     </row>
-    <row r="87" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A87" s="29" t="s">
         <v>197</v>
       </c>
@@ -3157,7 +3600,7 @@
       <c r="E87" s="19"/>
       <c r="F87" s="20"/>
     </row>
-    <row r="88" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" s="29" t="s">
         <v>200</v>
       </c>
@@ -3173,7 +3616,7 @@
       <c r="E88" s="19"/>
       <c r="F88" s="20"/>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="29" t="s">
         <v>202</v>
       </c>
@@ -3189,7 +3632,7 @@
       </c>
       <c r="F89" s="20"/>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="29" t="s">
         <v>204</v>
       </c>
@@ -3205,7 +3648,7 @@
       <c r="E90" s="19"/>
       <c r="F90" s="20"/>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="29" t="s">
         <v>206</v>
       </c>
@@ -3221,7 +3664,7 @@
       <c r="E91" s="19"/>
       <c r="F91" s="20"/>
     </row>
-    <row r="92" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="29" t="s">
         <v>209</v>
       </c>
@@ -3237,7 +3680,7 @@
       <c r="E92" s="19"/>
       <c r="F92" s="20"/>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="29" t="s">
         <v>212</v>
       </c>
@@ -3253,7 +3696,7 @@
       <c r="E93" s="19"/>
       <c r="F93" s="20"/>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="29" t="s">
         <v>215</v>
       </c>
@@ -3269,7 +3712,7 @@
       <c r="E94" s="19"/>
       <c r="F94" s="20"/>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="29" t="s">
         <v>215</v>
       </c>
@@ -3285,7 +3728,7 @@
       <c r="E95" s="19"/>
       <c r="F95" s="20"/>
     </row>
-    <row r="96" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A96" s="29" t="s">
         <v>219</v>
       </c>
@@ -3301,7 +3744,7 @@
       <c r="E96" s="19"/>
       <c r="F96" s="20"/>
     </row>
-    <row r="97" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="29" t="s">
         <v>222</v>
       </c>
@@ -3317,7 +3760,7 @@
       <c r="E97" s="19"/>
       <c r="F97" s="20"/>
     </row>
-    <row r="98" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A98" s="29" t="s">
         <v>222</v>
       </c>
@@ -3331,7 +3774,7 @@
       <c r="E98" s="19"/>
       <c r="F98" s="20"/>
     </row>
-    <row r="99" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="29" t="s">
         <v>226</v>
       </c>
@@ -3349,7 +3792,7 @@
       </c>
       <c r="F99" s="20"/>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="29" t="s">
         <v>229</v>
       </c>
@@ -3367,7 +3810,7 @@
       </c>
       <c r="F100" s="20"/>
     </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="29" t="s">
         <v>232</v>
       </c>
@@ -3383,7 +3826,7 @@
       </c>
       <c r="F101" s="20"/>
     </row>
-    <row r="102" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" s="29" t="s">
         <v>232</v>
       </c>
@@ -3399,7 +3842,7 @@
       <c r="E102" s="19"/>
       <c r="F102" s="20"/>
     </row>
-    <row r="103" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" s="29" t="s">
         <v>235</v>
       </c>
@@ -3417,7 +3860,7 @@
       </c>
       <c r="F103" s="20"/>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="29" t="s">
         <v>237</v>
       </c>
@@ -3433,7 +3876,7 @@
       <c r="E104" s="19"/>
       <c r="F104" s="20"/>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="29" t="s">
         <v>240</v>
       </c>
@@ -3449,7 +3892,7 @@
       <c r="E105" s="19"/>
       <c r="F105" s="20"/>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="29" t="s">
         <v>237</v>
       </c>
@@ -3465,7 +3908,7 @@
       <c r="E106" s="19"/>
       <c r="F106" s="20"/>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="29"/>
       <c r="B107" s="18"/>
       <c r="C107" s="18"/>
@@ -3473,7 +3916,7 @@
       <c r="E107" s="19"/>
       <c r="F107" s="20"/>
     </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="29"/>
       <c r="B108" s="18"/>
       <c r="C108" s="18"/>
@@ -3481,7 +3924,7 @@
       <c r="E108" s="19"/>
       <c r="F108" s="20"/>
     </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="29"/>
       <c r="B109" s="18"/>
       <c r="C109" s="18"/>
@@ -3490,38 +3933,30 @@
       <c r="F109" s="20"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:G64"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK64"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="B56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="4" width="14.7040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="24.8571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="67.2908163265306"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="14.7040816326531"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="15.8571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="4" width="14.7040816326531"/>
+    <col min="1" max="2" width="14.7109375" style="4"/>
+    <col min="3" max="3" width="24.85546875" style="4"/>
+    <col min="4" max="4" width="67.28515625" style="5"/>
+    <col min="5" max="5" width="14.7109375" style="4"/>
+    <col min="6" max="6" width="15.85546875" style="4"/>
+    <col min="7" max="1025" width="14.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3544,21 +3979,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
+      <c r="B2"/>
+      <c r="C2"/>
       <c r="D2" s="32" t="s">
         <v>244</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>246</v>
       </c>
@@ -3574,9 +4009,9 @@
       <c r="E3" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="F3" s="0"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>246</v>
       </c>
@@ -3592,9 +4027,12 @@
       <c r="E4" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="135" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F4"/>
+      <c r="G4" s="43" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>251</v>
       </c>
@@ -3610,9 +4048,9 @@
       <c r="E5" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>254</v>
       </c>
@@ -3628,9 +4066,9 @@
       <c r="E6" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F6"/>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
       <c r="B7" s="4" t="s">
         <v>26</v>
@@ -3644,9 +4082,9 @@
       <c r="E7" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F7" s="0"/>
-    </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F7"/>
+    </row>
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="31"/>
       <c r="B8" s="4" t="s">
         <v>26</v>
@@ -3660,9 +4098,9 @@
       <c r="E8" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F8" s="0"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
       <c r="B9" s="4" t="s">
         <v>26</v>
@@ -3676,9 +4114,9 @@
       <c r="E9" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F9" s="0"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="31"/>
       <c r="B10" s="4" t="s">
         <v>98</v>
@@ -3692,9 +4130,9 @@
       <c r="E10" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="F10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F10"/>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>260</v>
       </c>
@@ -3710,9 +4148,9 @@
       <c r="E11" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F11"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="31"/>
       <c r="B12" s="4" t="s">
         <v>103</v>
@@ -3726,68 +4164,68 @@
       <c r="E12" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F12" s="0"/>
-      <c r="G12" s="4" t="s">
+      <c r="F12"/>
+      <c r="G12" s="43" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="31" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="31" t="s">
+      <c r="B13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="E13" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
         <v>267</v>
       </c>
-      <c r="F13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="31" t="s">
+      <c r="B14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="32" t="s">
         <v>269</v>
-      </c>
-      <c r="D14" s="32" t="s">
-        <v>270</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F14"/>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="D15" s="32" t="s">
         <v>272</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>273</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="F15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F15"/>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>103</v>
@@ -3796,16 +4234,16 @@
         <v>198</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F16"/>
+    </row>
+    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>26</v>
@@ -3814,14 +4252,14 @@
         <v>191</v>
       </c>
       <c r="D17" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="F17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F17"/>
+    </row>
+    <row r="18" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>95</v>
       </c>
@@ -3832,66 +4270,66 @@
         <v>191</v>
       </c>
       <c r="D18" s="32" t="s">
+        <v>278</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="F18"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="s">
         <v>280</v>
       </c>
-      <c r="F18" s="0"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="31" t="s">
+      <c r="B19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="D19" s="32" t="s">
         <v>282</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>283</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F19" s="0"/>
-    </row>
-    <row r="20" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F19"/>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D20" s="32" t="s">
         <v>285</v>
       </c>
-      <c r="D20" s="32" t="s">
+      <c r="E20" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="F20"/>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="31" t="s">
         <v>286</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="F20" s="0"/>
-    </row>
-    <row r="21" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="31" t="s">
-        <v>287</v>
-      </c>
-      <c r="B21" s="0"/>
+      <c r="B21"/>
       <c r="C21" s="4" t="s">
         <v>90</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="F21" s="0"/>
-    </row>
-    <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+      <c r="F21"/>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="31"/>
       <c r="B22" s="4" t="s">
         <v>26</v>
@@ -3900,140 +4338,140 @@
         <v>90</v>
       </c>
       <c r="D22" s="32" t="s">
+        <v>288</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="F22"/>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="31" t="s">
         <v>289</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="F22" s="0"/>
-    </row>
-    <row r="23" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="31" t="s">
+      <c r="B23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="32" t="s">
         <v>291</v>
-      </c>
-      <c r="D23" s="32" t="s">
-        <v>292</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F23" s="0"/>
-    </row>
-    <row r="24" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F23"/>
+    </row>
+    <row r="24" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
+        <v>292</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="D24" s="32" t="s">
         <v>293</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="D24" s="32" t="s">
-        <v>294</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F24" s="0"/>
-    </row>
-    <row r="25" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D25" s="32" t="s">
         <v>295</v>
-      </c>
-      <c r="D25" s="32" t="s">
-        <v>296</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F25" s="0"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F25"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
+        <v>296</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="D26" s="32" t="s">
         <v>298</v>
       </c>
-      <c r="D26" s="32" t="s">
+      <c r="E26" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="F26"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="31" t="s">
         <v>299</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="F26" s="0"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="31" t="s">
-        <v>300</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>103</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="D27" s="32" t="s">
         <v>301</v>
       </c>
-      <c r="D27" s="32" t="s">
+      <c r="E27" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="F27"/>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="31" t="s">
         <v>302</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="F27" s="0"/>
-    </row>
-    <row r="28" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="31" t="s">
+      <c r="B28" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="4" t="s">
+      <c r="D28" s="32" t="s">
         <v>304</v>
-      </c>
-      <c r="D28" s="32" t="s">
-        <v>305</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F28" s="0"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F28"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
+        <v>305</v>
+      </c>
+      <c r="B29"/>
+      <c r="C29" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="D29" s="32" t="s">
         <v>306</v>
       </c>
-      <c r="B29" s="0"/>
-      <c r="C29" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="D29" s="32" t="s">
+      <c r="E29" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="F29"/>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="31" t="s">
         <v>307</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="F29" s="0"/>
-    </row>
-    <row r="30" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="31" t="s">
-        <v>308</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>26</v>
@@ -4042,16 +4480,16 @@
         <v>90</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F30" s="0"/>
-    </row>
-    <row r="31" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F30"/>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>26</v>
@@ -4060,14 +4498,14 @@
         <v>90</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F31" s="0"/>
-    </row>
-    <row r="32" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F31"/>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
         <v>143</v>
       </c>
@@ -4075,55 +4513,58 @@
         <v>26</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F32" s="0"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F32"/>
+    </row>
+    <row r="33" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
+        <v>312</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D33" s="32" t="s">
         <v>313</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="D33" s="32" t="s">
-        <v>314</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F33" s="0"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F33"/>
+    </row>
+    <row r="34" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
+        <v>314</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="D34" s="32" t="s">
         <v>315</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="D34" s="32" t="s">
-        <v>316</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F34" s="0"/>
-    </row>
-    <row r="35" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F34"/>
+      <c r="G34" s="43" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>103</v>
@@ -4132,16 +4573,16 @@
         <v>70</v>
       </c>
       <c r="D35" s="32" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F35" s="0"/>
-    </row>
-    <row r="36" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F35"/>
+    </row>
+    <row r="36" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>98</v>
@@ -4150,16 +4591,16 @@
         <v>90</v>
       </c>
       <c r="D36" s="32" t="s">
+        <v>319</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="F36"/>
+    </row>
+    <row r="37" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
+      <c r="A37" s="31" t="s">
         <v>320</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="F36" s="0"/>
-    </row>
-    <row r="37" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="31" t="s">
-        <v>321</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>103</v>
@@ -4168,178 +4609,1199 @@
         <v>90</v>
       </c>
       <c r="D37" s="32" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F37" s="0"/>
-    </row>
-    <row r="38" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F37"/>
+    </row>
+    <row r="38" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>103</v>
       </c>
       <c r="C38" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="D38" s="32" t="s">
         <v>324</v>
-      </c>
-      <c r="D38" s="32" t="s">
-        <v>325</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F38" s="0"/>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F38"/>
+    </row>
+    <row r="39" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>103</v>
       </c>
       <c r="C39" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="D39" s="32" t="s">
         <v>327</v>
-      </c>
-      <c r="D39" s="32" t="s">
-        <v>328</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F39" s="0"/>
-    </row>
-    <row r="40" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F39"/>
+      <c r="G39" s="43" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1025" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
+        <v>328</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="4" t="s">
+      <c r="D40" s="32" t="s">
         <v>330</v>
-      </c>
-      <c r="D40" s="32" t="s">
-        <v>331</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F40" s="0"/>
-    </row>
-    <row r="41" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F40"/>
+    </row>
+    <row r="41" spans="1:1025" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C41" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="D41" s="32" t="s">
         <v>332</v>
       </c>
-      <c r="D41" s="32" t="s">
+      <c r="E41" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="F41"/>
+    </row>
+    <row r="42" spans="1:1025" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="34" t="s">
         <v>333</v>
       </c>
-      <c r="E41" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="F41" s="0"/>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="31" t="s">
+      <c r="B42" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="D42" s="36" t="s">
         <v>334</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="D42" s="32" t="s">
+      <c r="E42" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="G42" s="35"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="35"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="35"/>
+      <c r="L42" s="35"/>
+      <c r="M42" s="35"/>
+      <c r="N42" s="35"/>
+      <c r="O42" s="35"/>
+      <c r="P42" s="35"/>
+      <c r="Q42" s="35"/>
+      <c r="R42" s="35"/>
+      <c r="S42" s="35"/>
+      <c r="T42" s="35"/>
+      <c r="U42" s="35"/>
+      <c r="V42" s="35"/>
+      <c r="W42" s="35"/>
+      <c r="X42" s="35"/>
+      <c r="Y42" s="35"/>
+      <c r="Z42" s="35"/>
+      <c r="AA42" s="35"/>
+      <c r="AB42" s="35"/>
+      <c r="AC42" s="35"/>
+      <c r="AD42" s="35"/>
+      <c r="AE42" s="35"/>
+      <c r="AF42" s="35"/>
+      <c r="AG42" s="35"/>
+      <c r="AH42" s="35"/>
+      <c r="AI42" s="35"/>
+      <c r="AJ42" s="35"/>
+      <c r="AK42" s="35"/>
+      <c r="AL42" s="35"/>
+      <c r="AM42" s="35"/>
+      <c r="AN42" s="35"/>
+      <c r="AO42" s="35"/>
+      <c r="AP42" s="35"/>
+      <c r="AQ42" s="35"/>
+      <c r="AR42" s="35"/>
+      <c r="AS42" s="35"/>
+      <c r="AT42" s="35"/>
+      <c r="AU42" s="35"/>
+      <c r="AV42" s="35"/>
+      <c r="AW42" s="35"/>
+      <c r="AX42" s="35"/>
+      <c r="AY42" s="35"/>
+      <c r="AZ42" s="35"/>
+      <c r="BA42" s="35"/>
+      <c r="BB42" s="35"/>
+      <c r="BC42" s="35"/>
+      <c r="BD42" s="35"/>
+      <c r="BE42" s="35"/>
+      <c r="BF42" s="35"/>
+      <c r="BG42" s="35"/>
+      <c r="BH42" s="35"/>
+      <c r="BI42" s="35"/>
+      <c r="BJ42" s="35"/>
+      <c r="BK42" s="35"/>
+      <c r="BL42" s="35"/>
+      <c r="BM42" s="35"/>
+      <c r="BN42" s="35"/>
+      <c r="BO42" s="35"/>
+      <c r="BP42" s="35"/>
+      <c r="BQ42" s="35"/>
+      <c r="BR42" s="35"/>
+      <c r="BS42" s="35"/>
+      <c r="BT42" s="35"/>
+      <c r="BU42" s="35"/>
+      <c r="BV42" s="35"/>
+      <c r="BW42" s="35"/>
+      <c r="BX42" s="35"/>
+      <c r="BY42" s="35"/>
+      <c r="BZ42" s="35"/>
+      <c r="CA42" s="35"/>
+      <c r="CB42" s="35"/>
+      <c r="CC42" s="35"/>
+      <c r="CD42" s="35"/>
+      <c r="CE42" s="35"/>
+      <c r="CF42" s="35"/>
+      <c r="CG42" s="35"/>
+      <c r="CH42" s="35"/>
+      <c r="CI42" s="35"/>
+      <c r="CJ42" s="35"/>
+      <c r="CK42" s="35"/>
+      <c r="CL42" s="35"/>
+      <c r="CM42" s="35"/>
+      <c r="CN42" s="35"/>
+      <c r="CO42" s="35"/>
+      <c r="CP42" s="35"/>
+      <c r="CQ42" s="35"/>
+      <c r="CR42" s="35"/>
+      <c r="CS42" s="35"/>
+      <c r="CT42" s="35"/>
+      <c r="CU42" s="35"/>
+      <c r="CV42" s="35"/>
+      <c r="CW42" s="35"/>
+      <c r="CX42" s="35"/>
+      <c r="CY42" s="35"/>
+      <c r="CZ42" s="35"/>
+      <c r="DA42" s="35"/>
+      <c r="DB42" s="35"/>
+      <c r="DC42" s="35"/>
+      <c r="DD42" s="35"/>
+      <c r="DE42" s="35"/>
+      <c r="DF42" s="35"/>
+      <c r="DG42" s="35"/>
+      <c r="DH42" s="35"/>
+      <c r="DI42" s="35"/>
+      <c r="DJ42" s="35"/>
+      <c r="DK42" s="35"/>
+      <c r="DL42" s="35"/>
+      <c r="DM42" s="35"/>
+      <c r="DN42" s="35"/>
+      <c r="DO42" s="35"/>
+      <c r="DP42" s="35"/>
+      <c r="DQ42" s="35"/>
+      <c r="DR42" s="35"/>
+      <c r="DS42" s="35"/>
+      <c r="DT42" s="35"/>
+      <c r="DU42" s="35"/>
+      <c r="DV42" s="35"/>
+      <c r="DW42" s="35"/>
+      <c r="DX42" s="35"/>
+      <c r="DY42" s="35"/>
+      <c r="DZ42" s="35"/>
+      <c r="EA42" s="35"/>
+      <c r="EB42" s="35"/>
+      <c r="EC42" s="35"/>
+      <c r="ED42" s="35"/>
+      <c r="EE42" s="35"/>
+      <c r="EF42" s="35"/>
+      <c r="EG42" s="35"/>
+      <c r="EH42" s="35"/>
+      <c r="EI42" s="35"/>
+      <c r="EJ42" s="35"/>
+      <c r="EK42" s="35"/>
+      <c r="EL42" s="35"/>
+      <c r="EM42" s="35"/>
+      <c r="EN42" s="35"/>
+      <c r="EO42" s="35"/>
+      <c r="EP42" s="35"/>
+      <c r="EQ42" s="35"/>
+      <c r="ER42" s="35"/>
+      <c r="ES42" s="35"/>
+      <c r="ET42" s="35"/>
+      <c r="EU42" s="35"/>
+      <c r="EV42" s="35"/>
+      <c r="EW42" s="35"/>
+      <c r="EX42" s="35"/>
+      <c r="EY42" s="35"/>
+      <c r="EZ42" s="35"/>
+      <c r="FA42" s="35"/>
+      <c r="FB42" s="35"/>
+      <c r="FC42" s="35"/>
+      <c r="FD42" s="35"/>
+      <c r="FE42" s="35"/>
+      <c r="FF42" s="35"/>
+      <c r="FG42" s="35"/>
+      <c r="FH42" s="35"/>
+      <c r="FI42" s="35"/>
+      <c r="FJ42" s="35"/>
+      <c r="FK42" s="35"/>
+      <c r="FL42" s="35"/>
+      <c r="FM42" s="35"/>
+      <c r="FN42" s="35"/>
+      <c r="FO42" s="35"/>
+      <c r="FP42" s="35"/>
+      <c r="FQ42" s="35"/>
+      <c r="FR42" s="35"/>
+      <c r="FS42" s="35"/>
+      <c r="FT42" s="35"/>
+      <c r="FU42" s="35"/>
+      <c r="FV42" s="35"/>
+      <c r="FW42" s="35"/>
+      <c r="FX42" s="35"/>
+      <c r="FY42" s="35"/>
+      <c r="FZ42" s="35"/>
+      <c r="GA42" s="35"/>
+      <c r="GB42" s="35"/>
+      <c r="GC42" s="35"/>
+      <c r="GD42" s="35"/>
+      <c r="GE42" s="35"/>
+      <c r="GF42" s="35"/>
+      <c r="GG42" s="35"/>
+      <c r="GH42" s="35"/>
+      <c r="GI42" s="35"/>
+      <c r="GJ42" s="35"/>
+      <c r="GK42" s="35"/>
+      <c r="GL42" s="35"/>
+      <c r="GM42" s="35"/>
+      <c r="GN42" s="35"/>
+      <c r="GO42" s="35"/>
+      <c r="GP42" s="35"/>
+      <c r="GQ42" s="35"/>
+      <c r="GR42" s="35"/>
+      <c r="GS42" s="35"/>
+      <c r="GT42" s="35"/>
+      <c r="GU42" s="35"/>
+      <c r="GV42" s="35"/>
+      <c r="GW42" s="35"/>
+      <c r="GX42" s="35"/>
+      <c r="GY42" s="35"/>
+      <c r="GZ42" s="35"/>
+      <c r="HA42" s="35"/>
+      <c r="HB42" s="35"/>
+      <c r="HC42" s="35"/>
+      <c r="HD42" s="35"/>
+      <c r="HE42" s="35"/>
+      <c r="HF42" s="35"/>
+      <c r="HG42" s="35"/>
+      <c r="HH42" s="35"/>
+      <c r="HI42" s="35"/>
+      <c r="HJ42" s="35"/>
+      <c r="HK42" s="35"/>
+      <c r="HL42" s="35"/>
+      <c r="HM42" s="35"/>
+      <c r="HN42" s="35"/>
+      <c r="HO42" s="35"/>
+      <c r="HP42" s="35"/>
+      <c r="HQ42" s="35"/>
+      <c r="HR42" s="35"/>
+      <c r="HS42" s="35"/>
+      <c r="HT42" s="35"/>
+      <c r="HU42" s="35"/>
+      <c r="HV42" s="35"/>
+      <c r="HW42" s="35"/>
+      <c r="HX42" s="35"/>
+      <c r="HY42" s="35"/>
+      <c r="HZ42" s="35"/>
+      <c r="IA42" s="35"/>
+      <c r="IB42" s="35"/>
+      <c r="IC42" s="35"/>
+      <c r="ID42" s="35"/>
+      <c r="IE42" s="35"/>
+      <c r="IF42" s="35"/>
+      <c r="IG42" s="35"/>
+      <c r="IH42" s="35"/>
+      <c r="II42" s="35"/>
+      <c r="IJ42" s="35"/>
+      <c r="IK42" s="35"/>
+      <c r="IL42" s="35"/>
+      <c r="IM42" s="35"/>
+      <c r="IN42" s="35"/>
+      <c r="IO42" s="35"/>
+      <c r="IP42" s="35"/>
+      <c r="IQ42" s="35"/>
+      <c r="IR42" s="35"/>
+      <c r="IS42" s="35"/>
+      <c r="IT42" s="35"/>
+      <c r="IU42" s="35"/>
+      <c r="IV42" s="35"/>
+      <c r="IW42" s="35"/>
+      <c r="IX42" s="35"/>
+      <c r="IY42" s="35"/>
+      <c r="IZ42" s="35"/>
+      <c r="JA42" s="35"/>
+      <c r="JB42" s="35"/>
+      <c r="JC42" s="35"/>
+      <c r="JD42" s="35"/>
+      <c r="JE42" s="35"/>
+      <c r="JF42" s="35"/>
+      <c r="JG42" s="35"/>
+      <c r="JH42" s="35"/>
+      <c r="JI42" s="35"/>
+      <c r="JJ42" s="35"/>
+      <c r="JK42" s="35"/>
+      <c r="JL42" s="35"/>
+      <c r="JM42" s="35"/>
+      <c r="JN42" s="35"/>
+      <c r="JO42" s="35"/>
+      <c r="JP42" s="35"/>
+      <c r="JQ42" s="35"/>
+      <c r="JR42" s="35"/>
+      <c r="JS42" s="35"/>
+      <c r="JT42" s="35"/>
+      <c r="JU42" s="35"/>
+      <c r="JV42" s="35"/>
+      <c r="JW42" s="35"/>
+      <c r="JX42" s="35"/>
+      <c r="JY42" s="35"/>
+      <c r="JZ42" s="35"/>
+      <c r="KA42" s="35"/>
+      <c r="KB42" s="35"/>
+      <c r="KC42" s="35"/>
+      <c r="KD42" s="35"/>
+      <c r="KE42" s="35"/>
+      <c r="KF42" s="35"/>
+      <c r="KG42" s="35"/>
+      <c r="KH42" s="35"/>
+      <c r="KI42" s="35"/>
+      <c r="KJ42" s="35"/>
+      <c r="KK42" s="35"/>
+      <c r="KL42" s="35"/>
+      <c r="KM42" s="35"/>
+      <c r="KN42" s="35"/>
+      <c r="KO42" s="35"/>
+      <c r="KP42" s="35"/>
+      <c r="KQ42" s="35"/>
+      <c r="KR42" s="35"/>
+      <c r="KS42" s="35"/>
+      <c r="KT42" s="35"/>
+      <c r="KU42" s="35"/>
+      <c r="KV42" s="35"/>
+      <c r="KW42" s="35"/>
+      <c r="KX42" s="35"/>
+      <c r="KY42" s="35"/>
+      <c r="KZ42" s="35"/>
+      <c r="LA42" s="35"/>
+      <c r="LB42" s="35"/>
+      <c r="LC42" s="35"/>
+      <c r="LD42" s="35"/>
+      <c r="LE42" s="35"/>
+      <c r="LF42" s="35"/>
+      <c r="LG42" s="35"/>
+      <c r="LH42" s="35"/>
+      <c r="LI42" s="35"/>
+      <c r="LJ42" s="35"/>
+      <c r="LK42" s="35"/>
+      <c r="LL42" s="35"/>
+      <c r="LM42" s="35"/>
+      <c r="LN42" s="35"/>
+      <c r="LO42" s="35"/>
+      <c r="LP42" s="35"/>
+      <c r="LQ42" s="35"/>
+      <c r="LR42" s="35"/>
+      <c r="LS42" s="35"/>
+      <c r="LT42" s="35"/>
+      <c r="LU42" s="35"/>
+      <c r="LV42" s="35"/>
+      <c r="LW42" s="35"/>
+      <c r="LX42" s="35"/>
+      <c r="LY42" s="35"/>
+      <c r="LZ42" s="35"/>
+      <c r="MA42" s="35"/>
+      <c r="MB42" s="35"/>
+      <c r="MC42" s="35"/>
+      <c r="MD42" s="35"/>
+      <c r="ME42" s="35"/>
+      <c r="MF42" s="35"/>
+      <c r="MG42" s="35"/>
+      <c r="MH42" s="35"/>
+      <c r="MI42" s="35"/>
+      <c r="MJ42" s="35"/>
+      <c r="MK42" s="35"/>
+      <c r="ML42" s="35"/>
+      <c r="MM42" s="35"/>
+      <c r="MN42" s="35"/>
+      <c r="MO42" s="35"/>
+      <c r="MP42" s="35"/>
+      <c r="MQ42" s="35"/>
+      <c r="MR42" s="35"/>
+      <c r="MS42" s="35"/>
+      <c r="MT42" s="35"/>
+      <c r="MU42" s="35"/>
+      <c r="MV42" s="35"/>
+      <c r="MW42" s="35"/>
+      <c r="MX42" s="35"/>
+      <c r="MY42" s="35"/>
+      <c r="MZ42" s="35"/>
+      <c r="NA42" s="35"/>
+      <c r="NB42" s="35"/>
+      <c r="NC42" s="35"/>
+      <c r="ND42" s="35"/>
+      <c r="NE42" s="35"/>
+      <c r="NF42" s="35"/>
+      <c r="NG42" s="35"/>
+      <c r="NH42" s="35"/>
+      <c r="NI42" s="35"/>
+      <c r="NJ42" s="35"/>
+      <c r="NK42" s="35"/>
+      <c r="NL42" s="35"/>
+      <c r="NM42" s="35"/>
+      <c r="NN42" s="35"/>
+      <c r="NO42" s="35"/>
+      <c r="NP42" s="35"/>
+      <c r="NQ42" s="35"/>
+      <c r="NR42" s="35"/>
+      <c r="NS42" s="35"/>
+      <c r="NT42" s="35"/>
+      <c r="NU42" s="35"/>
+      <c r="NV42" s="35"/>
+      <c r="NW42" s="35"/>
+      <c r="NX42" s="35"/>
+      <c r="NY42" s="35"/>
+      <c r="NZ42" s="35"/>
+      <c r="OA42" s="35"/>
+      <c r="OB42" s="35"/>
+      <c r="OC42" s="35"/>
+      <c r="OD42" s="35"/>
+      <c r="OE42" s="35"/>
+      <c r="OF42" s="35"/>
+      <c r="OG42" s="35"/>
+      <c r="OH42" s="35"/>
+      <c r="OI42" s="35"/>
+      <c r="OJ42" s="35"/>
+      <c r="OK42" s="35"/>
+      <c r="OL42" s="35"/>
+      <c r="OM42" s="35"/>
+      <c r="ON42" s="35"/>
+      <c r="OO42" s="35"/>
+      <c r="OP42" s="35"/>
+      <c r="OQ42" s="35"/>
+      <c r="OR42" s="35"/>
+      <c r="OS42" s="35"/>
+      <c r="OT42" s="35"/>
+      <c r="OU42" s="35"/>
+      <c r="OV42" s="35"/>
+      <c r="OW42" s="35"/>
+      <c r="OX42" s="35"/>
+      <c r="OY42" s="35"/>
+      <c r="OZ42" s="35"/>
+      <c r="PA42" s="35"/>
+      <c r="PB42" s="35"/>
+      <c r="PC42" s="35"/>
+      <c r="PD42" s="35"/>
+      <c r="PE42" s="35"/>
+      <c r="PF42" s="35"/>
+      <c r="PG42" s="35"/>
+      <c r="PH42" s="35"/>
+      <c r="PI42" s="35"/>
+      <c r="PJ42" s="35"/>
+      <c r="PK42" s="35"/>
+      <c r="PL42" s="35"/>
+      <c r="PM42" s="35"/>
+      <c r="PN42" s="35"/>
+      <c r="PO42" s="35"/>
+      <c r="PP42" s="35"/>
+      <c r="PQ42" s="35"/>
+      <c r="PR42" s="35"/>
+      <c r="PS42" s="35"/>
+      <c r="PT42" s="35"/>
+      <c r="PU42" s="35"/>
+      <c r="PV42" s="35"/>
+      <c r="PW42" s="35"/>
+      <c r="PX42" s="35"/>
+      <c r="PY42" s="35"/>
+      <c r="PZ42" s="35"/>
+      <c r="QA42" s="35"/>
+      <c r="QB42" s="35"/>
+      <c r="QC42" s="35"/>
+      <c r="QD42" s="35"/>
+      <c r="QE42" s="35"/>
+      <c r="QF42" s="35"/>
+      <c r="QG42" s="35"/>
+      <c r="QH42" s="35"/>
+      <c r="QI42" s="35"/>
+      <c r="QJ42" s="35"/>
+      <c r="QK42" s="35"/>
+      <c r="QL42" s="35"/>
+      <c r="QM42" s="35"/>
+      <c r="QN42" s="35"/>
+      <c r="QO42" s="35"/>
+      <c r="QP42" s="35"/>
+      <c r="QQ42" s="35"/>
+      <c r="QR42" s="35"/>
+      <c r="QS42" s="35"/>
+      <c r="QT42" s="35"/>
+      <c r="QU42" s="35"/>
+      <c r="QV42" s="35"/>
+      <c r="QW42" s="35"/>
+      <c r="QX42" s="35"/>
+      <c r="QY42" s="35"/>
+      <c r="QZ42" s="35"/>
+      <c r="RA42" s="35"/>
+      <c r="RB42" s="35"/>
+      <c r="RC42" s="35"/>
+      <c r="RD42" s="35"/>
+      <c r="RE42" s="35"/>
+      <c r="RF42" s="35"/>
+      <c r="RG42" s="35"/>
+      <c r="RH42" s="35"/>
+      <c r="RI42" s="35"/>
+      <c r="RJ42" s="35"/>
+      <c r="RK42" s="35"/>
+      <c r="RL42" s="35"/>
+      <c r="RM42" s="35"/>
+      <c r="RN42" s="35"/>
+      <c r="RO42" s="35"/>
+      <c r="RP42" s="35"/>
+      <c r="RQ42" s="35"/>
+      <c r="RR42" s="35"/>
+      <c r="RS42" s="35"/>
+      <c r="RT42" s="35"/>
+      <c r="RU42" s="35"/>
+      <c r="RV42" s="35"/>
+      <c r="RW42" s="35"/>
+      <c r="RX42" s="35"/>
+      <c r="RY42" s="35"/>
+      <c r="RZ42" s="35"/>
+      <c r="SA42" s="35"/>
+      <c r="SB42" s="35"/>
+      <c r="SC42" s="35"/>
+      <c r="SD42" s="35"/>
+      <c r="SE42" s="35"/>
+      <c r="SF42" s="35"/>
+      <c r="SG42" s="35"/>
+      <c r="SH42" s="35"/>
+      <c r="SI42" s="35"/>
+      <c r="SJ42" s="35"/>
+      <c r="SK42" s="35"/>
+      <c r="SL42" s="35"/>
+      <c r="SM42" s="35"/>
+      <c r="SN42" s="35"/>
+      <c r="SO42" s="35"/>
+      <c r="SP42" s="35"/>
+      <c r="SQ42" s="35"/>
+      <c r="SR42" s="35"/>
+      <c r="SS42" s="35"/>
+      <c r="ST42" s="35"/>
+      <c r="SU42" s="35"/>
+      <c r="SV42" s="35"/>
+      <c r="SW42" s="35"/>
+      <c r="SX42" s="35"/>
+      <c r="SY42" s="35"/>
+      <c r="SZ42" s="35"/>
+      <c r="TA42" s="35"/>
+      <c r="TB42" s="35"/>
+      <c r="TC42" s="35"/>
+      <c r="TD42" s="35"/>
+      <c r="TE42" s="35"/>
+      <c r="TF42" s="35"/>
+      <c r="TG42" s="35"/>
+      <c r="TH42" s="35"/>
+      <c r="TI42" s="35"/>
+      <c r="TJ42" s="35"/>
+      <c r="TK42" s="35"/>
+      <c r="TL42" s="35"/>
+      <c r="TM42" s="35"/>
+      <c r="TN42" s="35"/>
+      <c r="TO42" s="35"/>
+      <c r="TP42" s="35"/>
+      <c r="TQ42" s="35"/>
+      <c r="TR42" s="35"/>
+      <c r="TS42" s="35"/>
+      <c r="TT42" s="35"/>
+      <c r="TU42" s="35"/>
+      <c r="TV42" s="35"/>
+      <c r="TW42" s="35"/>
+      <c r="TX42" s="35"/>
+      <c r="TY42" s="35"/>
+      <c r="TZ42" s="35"/>
+      <c r="UA42" s="35"/>
+      <c r="UB42" s="35"/>
+      <c r="UC42" s="35"/>
+      <c r="UD42" s="35"/>
+      <c r="UE42" s="35"/>
+      <c r="UF42" s="35"/>
+      <c r="UG42" s="35"/>
+      <c r="UH42" s="35"/>
+      <c r="UI42" s="35"/>
+      <c r="UJ42" s="35"/>
+      <c r="UK42" s="35"/>
+      <c r="UL42" s="35"/>
+      <c r="UM42" s="35"/>
+      <c r="UN42" s="35"/>
+      <c r="UO42" s="35"/>
+      <c r="UP42" s="35"/>
+      <c r="UQ42" s="35"/>
+      <c r="UR42" s="35"/>
+      <c r="US42" s="35"/>
+      <c r="UT42" s="35"/>
+      <c r="UU42" s="35"/>
+      <c r="UV42" s="35"/>
+      <c r="UW42" s="35"/>
+      <c r="UX42" s="35"/>
+      <c r="UY42" s="35"/>
+      <c r="UZ42" s="35"/>
+      <c r="VA42" s="35"/>
+      <c r="VB42" s="35"/>
+      <c r="VC42" s="35"/>
+      <c r="VD42" s="35"/>
+      <c r="VE42" s="35"/>
+      <c r="VF42" s="35"/>
+      <c r="VG42" s="35"/>
+      <c r="VH42" s="35"/>
+      <c r="VI42" s="35"/>
+      <c r="VJ42" s="35"/>
+      <c r="VK42" s="35"/>
+      <c r="VL42" s="35"/>
+      <c r="VM42" s="35"/>
+      <c r="VN42" s="35"/>
+      <c r="VO42" s="35"/>
+      <c r="VP42" s="35"/>
+      <c r="VQ42" s="35"/>
+      <c r="VR42" s="35"/>
+      <c r="VS42" s="35"/>
+      <c r="VT42" s="35"/>
+      <c r="VU42" s="35"/>
+      <c r="VV42" s="35"/>
+      <c r="VW42" s="35"/>
+      <c r="VX42" s="35"/>
+      <c r="VY42" s="35"/>
+      <c r="VZ42" s="35"/>
+      <c r="WA42" s="35"/>
+      <c r="WB42" s="35"/>
+      <c r="WC42" s="35"/>
+      <c r="WD42" s="35"/>
+      <c r="WE42" s="35"/>
+      <c r="WF42" s="35"/>
+      <c r="WG42" s="35"/>
+      <c r="WH42" s="35"/>
+      <c r="WI42" s="35"/>
+      <c r="WJ42" s="35"/>
+      <c r="WK42" s="35"/>
+      <c r="WL42" s="35"/>
+      <c r="WM42" s="35"/>
+      <c r="WN42" s="35"/>
+      <c r="WO42" s="35"/>
+      <c r="WP42" s="35"/>
+      <c r="WQ42" s="35"/>
+      <c r="WR42" s="35"/>
+      <c r="WS42" s="35"/>
+      <c r="WT42" s="35"/>
+      <c r="WU42" s="35"/>
+      <c r="WV42" s="35"/>
+      <c r="WW42" s="35"/>
+      <c r="WX42" s="35"/>
+      <c r="WY42" s="35"/>
+      <c r="WZ42" s="35"/>
+      <c r="XA42" s="35"/>
+      <c r="XB42" s="35"/>
+      <c r="XC42" s="35"/>
+      <c r="XD42" s="35"/>
+      <c r="XE42" s="35"/>
+      <c r="XF42" s="35"/>
+      <c r="XG42" s="35"/>
+      <c r="XH42" s="35"/>
+      <c r="XI42" s="35"/>
+      <c r="XJ42" s="35"/>
+      <c r="XK42" s="35"/>
+      <c r="XL42" s="35"/>
+      <c r="XM42" s="35"/>
+      <c r="XN42" s="35"/>
+      <c r="XO42" s="35"/>
+      <c r="XP42" s="35"/>
+      <c r="XQ42" s="35"/>
+      <c r="XR42" s="35"/>
+      <c r="XS42" s="35"/>
+      <c r="XT42" s="35"/>
+      <c r="XU42" s="35"/>
+      <c r="XV42" s="35"/>
+      <c r="XW42" s="35"/>
+      <c r="XX42" s="35"/>
+      <c r="XY42" s="35"/>
+      <c r="XZ42" s="35"/>
+      <c r="YA42" s="35"/>
+      <c r="YB42" s="35"/>
+      <c r="YC42" s="35"/>
+      <c r="YD42" s="35"/>
+      <c r="YE42" s="35"/>
+      <c r="YF42" s="35"/>
+      <c r="YG42" s="35"/>
+      <c r="YH42" s="35"/>
+      <c r="YI42" s="35"/>
+      <c r="YJ42" s="35"/>
+      <c r="YK42" s="35"/>
+      <c r="YL42" s="35"/>
+      <c r="YM42" s="35"/>
+      <c r="YN42" s="35"/>
+      <c r="YO42" s="35"/>
+      <c r="YP42" s="35"/>
+      <c r="YQ42" s="35"/>
+      <c r="YR42" s="35"/>
+      <c r="YS42" s="35"/>
+      <c r="YT42" s="35"/>
+      <c r="YU42" s="35"/>
+      <c r="YV42" s="35"/>
+      <c r="YW42" s="35"/>
+      <c r="YX42" s="35"/>
+      <c r="YY42" s="35"/>
+      <c r="YZ42" s="35"/>
+      <c r="ZA42" s="35"/>
+      <c r="ZB42" s="35"/>
+      <c r="ZC42" s="35"/>
+      <c r="ZD42" s="35"/>
+      <c r="ZE42" s="35"/>
+      <c r="ZF42" s="35"/>
+      <c r="ZG42" s="35"/>
+      <c r="ZH42" s="35"/>
+      <c r="ZI42" s="35"/>
+      <c r="ZJ42" s="35"/>
+      <c r="ZK42" s="35"/>
+      <c r="ZL42" s="35"/>
+      <c r="ZM42" s="35"/>
+      <c r="ZN42" s="35"/>
+      <c r="ZO42" s="35"/>
+      <c r="ZP42" s="35"/>
+      <c r="ZQ42" s="35"/>
+      <c r="ZR42" s="35"/>
+      <c r="ZS42" s="35"/>
+      <c r="ZT42" s="35"/>
+      <c r="ZU42" s="35"/>
+      <c r="ZV42" s="35"/>
+      <c r="ZW42" s="35"/>
+      <c r="ZX42" s="35"/>
+      <c r="ZY42" s="35"/>
+      <c r="ZZ42" s="35"/>
+      <c r="AAA42" s="35"/>
+      <c r="AAB42" s="35"/>
+      <c r="AAC42" s="35"/>
+      <c r="AAD42" s="35"/>
+      <c r="AAE42" s="35"/>
+      <c r="AAF42" s="35"/>
+      <c r="AAG42" s="35"/>
+      <c r="AAH42" s="35"/>
+      <c r="AAI42" s="35"/>
+      <c r="AAJ42" s="35"/>
+      <c r="AAK42" s="35"/>
+      <c r="AAL42" s="35"/>
+      <c r="AAM42" s="35"/>
+      <c r="AAN42" s="35"/>
+      <c r="AAO42" s="35"/>
+      <c r="AAP42" s="35"/>
+      <c r="AAQ42" s="35"/>
+      <c r="AAR42" s="35"/>
+      <c r="AAS42" s="35"/>
+      <c r="AAT42" s="35"/>
+      <c r="AAU42" s="35"/>
+      <c r="AAV42" s="35"/>
+      <c r="AAW42" s="35"/>
+      <c r="AAX42" s="35"/>
+      <c r="AAY42" s="35"/>
+      <c r="AAZ42" s="35"/>
+      <c r="ABA42" s="35"/>
+      <c r="ABB42" s="35"/>
+      <c r="ABC42" s="35"/>
+      <c r="ABD42" s="35"/>
+      <c r="ABE42" s="35"/>
+      <c r="ABF42" s="35"/>
+      <c r="ABG42" s="35"/>
+      <c r="ABH42" s="35"/>
+      <c r="ABI42" s="35"/>
+      <c r="ABJ42" s="35"/>
+      <c r="ABK42" s="35"/>
+      <c r="ABL42" s="35"/>
+      <c r="ABM42" s="35"/>
+      <c r="ABN42" s="35"/>
+      <c r="ABO42" s="35"/>
+      <c r="ABP42" s="35"/>
+      <c r="ABQ42" s="35"/>
+      <c r="ABR42" s="35"/>
+      <c r="ABS42" s="35"/>
+      <c r="ABT42" s="35"/>
+      <c r="ABU42" s="35"/>
+      <c r="ABV42" s="35"/>
+      <c r="ABW42" s="35"/>
+      <c r="ABX42" s="35"/>
+      <c r="ABY42" s="35"/>
+      <c r="ABZ42" s="35"/>
+      <c r="ACA42" s="35"/>
+      <c r="ACB42" s="35"/>
+      <c r="ACC42" s="35"/>
+      <c r="ACD42" s="35"/>
+      <c r="ACE42" s="35"/>
+      <c r="ACF42" s="35"/>
+      <c r="ACG42" s="35"/>
+      <c r="ACH42" s="35"/>
+      <c r="ACI42" s="35"/>
+      <c r="ACJ42" s="35"/>
+      <c r="ACK42" s="35"/>
+      <c r="ACL42" s="35"/>
+      <c r="ACM42" s="35"/>
+      <c r="ACN42" s="35"/>
+      <c r="ACO42" s="35"/>
+      <c r="ACP42" s="35"/>
+      <c r="ACQ42" s="35"/>
+      <c r="ACR42" s="35"/>
+      <c r="ACS42" s="35"/>
+      <c r="ACT42" s="35"/>
+      <c r="ACU42" s="35"/>
+      <c r="ACV42" s="35"/>
+      <c r="ACW42" s="35"/>
+      <c r="ACX42" s="35"/>
+      <c r="ACY42" s="35"/>
+      <c r="ACZ42" s="35"/>
+      <c r="ADA42" s="35"/>
+      <c r="ADB42" s="35"/>
+      <c r="ADC42" s="35"/>
+      <c r="ADD42" s="35"/>
+      <c r="ADE42" s="35"/>
+      <c r="ADF42" s="35"/>
+      <c r="ADG42" s="35"/>
+      <c r="ADH42" s="35"/>
+      <c r="ADI42" s="35"/>
+      <c r="ADJ42" s="35"/>
+      <c r="ADK42" s="35"/>
+      <c r="ADL42" s="35"/>
+      <c r="ADM42" s="35"/>
+      <c r="ADN42" s="35"/>
+      <c r="ADO42" s="35"/>
+      <c r="ADP42" s="35"/>
+      <c r="ADQ42" s="35"/>
+      <c r="ADR42" s="35"/>
+      <c r="ADS42" s="35"/>
+      <c r="ADT42" s="35"/>
+      <c r="ADU42" s="35"/>
+      <c r="ADV42" s="35"/>
+      <c r="ADW42" s="35"/>
+      <c r="ADX42" s="35"/>
+      <c r="ADY42" s="35"/>
+      <c r="ADZ42" s="35"/>
+      <c r="AEA42" s="35"/>
+      <c r="AEB42" s="35"/>
+      <c r="AEC42" s="35"/>
+      <c r="AED42" s="35"/>
+      <c r="AEE42" s="35"/>
+      <c r="AEF42" s="35"/>
+      <c r="AEG42" s="35"/>
+      <c r="AEH42" s="35"/>
+      <c r="AEI42" s="35"/>
+      <c r="AEJ42" s="35"/>
+      <c r="AEK42" s="35"/>
+      <c r="AEL42" s="35"/>
+      <c r="AEM42" s="35"/>
+      <c r="AEN42" s="35"/>
+      <c r="AEO42" s="35"/>
+      <c r="AEP42" s="35"/>
+      <c r="AEQ42" s="35"/>
+      <c r="AER42" s="35"/>
+      <c r="AES42" s="35"/>
+      <c r="AET42" s="35"/>
+      <c r="AEU42" s="35"/>
+      <c r="AEV42" s="35"/>
+      <c r="AEW42" s="35"/>
+      <c r="AEX42" s="35"/>
+      <c r="AEY42" s="35"/>
+      <c r="AEZ42" s="35"/>
+      <c r="AFA42" s="35"/>
+      <c r="AFB42" s="35"/>
+      <c r="AFC42" s="35"/>
+      <c r="AFD42" s="35"/>
+      <c r="AFE42" s="35"/>
+      <c r="AFF42" s="35"/>
+      <c r="AFG42" s="35"/>
+      <c r="AFH42" s="35"/>
+      <c r="AFI42" s="35"/>
+      <c r="AFJ42" s="35"/>
+      <c r="AFK42" s="35"/>
+      <c r="AFL42" s="35"/>
+      <c r="AFM42" s="35"/>
+      <c r="AFN42" s="35"/>
+      <c r="AFO42" s="35"/>
+      <c r="AFP42" s="35"/>
+      <c r="AFQ42" s="35"/>
+      <c r="AFR42" s="35"/>
+      <c r="AFS42" s="35"/>
+      <c r="AFT42" s="35"/>
+      <c r="AFU42" s="35"/>
+      <c r="AFV42" s="35"/>
+      <c r="AFW42" s="35"/>
+      <c r="AFX42" s="35"/>
+      <c r="AFY42" s="35"/>
+      <c r="AFZ42" s="35"/>
+      <c r="AGA42" s="35"/>
+      <c r="AGB42" s="35"/>
+      <c r="AGC42" s="35"/>
+      <c r="AGD42" s="35"/>
+      <c r="AGE42" s="35"/>
+      <c r="AGF42" s="35"/>
+      <c r="AGG42" s="35"/>
+      <c r="AGH42" s="35"/>
+      <c r="AGI42" s="35"/>
+      <c r="AGJ42" s="35"/>
+      <c r="AGK42" s="35"/>
+      <c r="AGL42" s="35"/>
+      <c r="AGM42" s="35"/>
+      <c r="AGN42" s="35"/>
+      <c r="AGO42" s="35"/>
+      <c r="AGP42" s="35"/>
+      <c r="AGQ42" s="35"/>
+      <c r="AGR42" s="35"/>
+      <c r="AGS42" s="35"/>
+      <c r="AGT42" s="35"/>
+      <c r="AGU42" s="35"/>
+      <c r="AGV42" s="35"/>
+      <c r="AGW42" s="35"/>
+      <c r="AGX42" s="35"/>
+      <c r="AGY42" s="35"/>
+      <c r="AGZ42" s="35"/>
+      <c r="AHA42" s="35"/>
+      <c r="AHB42" s="35"/>
+      <c r="AHC42" s="35"/>
+      <c r="AHD42" s="35"/>
+      <c r="AHE42" s="35"/>
+      <c r="AHF42" s="35"/>
+      <c r="AHG42" s="35"/>
+      <c r="AHH42" s="35"/>
+      <c r="AHI42" s="35"/>
+      <c r="AHJ42" s="35"/>
+      <c r="AHK42" s="35"/>
+      <c r="AHL42" s="35"/>
+      <c r="AHM42" s="35"/>
+      <c r="AHN42" s="35"/>
+      <c r="AHO42" s="35"/>
+      <c r="AHP42" s="35"/>
+      <c r="AHQ42" s="35"/>
+      <c r="AHR42" s="35"/>
+      <c r="AHS42" s="35"/>
+      <c r="AHT42" s="35"/>
+      <c r="AHU42" s="35"/>
+      <c r="AHV42" s="35"/>
+      <c r="AHW42" s="35"/>
+      <c r="AHX42" s="35"/>
+      <c r="AHY42" s="35"/>
+      <c r="AHZ42" s="35"/>
+      <c r="AIA42" s="35"/>
+      <c r="AIB42" s="35"/>
+      <c r="AIC42" s="35"/>
+      <c r="AID42" s="35"/>
+      <c r="AIE42" s="35"/>
+      <c r="AIF42" s="35"/>
+      <c r="AIG42" s="35"/>
+      <c r="AIH42" s="35"/>
+      <c r="AII42" s="35"/>
+      <c r="AIJ42" s="35"/>
+      <c r="AIK42" s="35"/>
+      <c r="AIL42" s="35"/>
+      <c r="AIM42" s="35"/>
+      <c r="AIN42" s="35"/>
+      <c r="AIO42" s="35"/>
+      <c r="AIP42" s="35"/>
+      <c r="AIQ42" s="35"/>
+      <c r="AIR42" s="35"/>
+      <c r="AIS42" s="35"/>
+      <c r="AIT42" s="35"/>
+      <c r="AIU42" s="35"/>
+      <c r="AIV42" s="35"/>
+      <c r="AIW42" s="35"/>
+      <c r="AIX42" s="35"/>
+      <c r="AIY42" s="35"/>
+      <c r="AIZ42" s="35"/>
+      <c r="AJA42" s="35"/>
+      <c r="AJB42" s="35"/>
+      <c r="AJC42" s="35"/>
+      <c r="AJD42" s="35"/>
+      <c r="AJE42" s="35"/>
+      <c r="AJF42" s="35"/>
+      <c r="AJG42" s="35"/>
+      <c r="AJH42" s="35"/>
+      <c r="AJI42" s="35"/>
+      <c r="AJJ42" s="35"/>
+      <c r="AJK42" s="35"/>
+      <c r="AJL42" s="35"/>
+      <c r="AJM42" s="35"/>
+      <c r="AJN42" s="35"/>
+      <c r="AJO42" s="35"/>
+      <c r="AJP42" s="35"/>
+      <c r="AJQ42" s="35"/>
+      <c r="AJR42" s="35"/>
+      <c r="AJS42" s="35"/>
+      <c r="AJT42" s="35"/>
+      <c r="AJU42" s="35"/>
+      <c r="AJV42" s="35"/>
+      <c r="AJW42" s="35"/>
+      <c r="AJX42" s="35"/>
+      <c r="AJY42" s="35"/>
+      <c r="AJZ42" s="35"/>
+      <c r="AKA42" s="35"/>
+      <c r="AKB42" s="35"/>
+      <c r="AKC42" s="35"/>
+      <c r="AKD42" s="35"/>
+      <c r="AKE42" s="35"/>
+      <c r="AKF42" s="35"/>
+      <c r="AKG42" s="35"/>
+      <c r="AKH42" s="35"/>
+      <c r="AKI42" s="35"/>
+      <c r="AKJ42" s="35"/>
+      <c r="AKK42" s="35"/>
+      <c r="AKL42" s="35"/>
+      <c r="AKM42" s="35"/>
+      <c r="AKN42" s="35"/>
+      <c r="AKO42" s="35"/>
+      <c r="AKP42" s="35"/>
+      <c r="AKQ42" s="35"/>
+      <c r="AKR42" s="35"/>
+      <c r="AKS42" s="35"/>
+      <c r="AKT42" s="35"/>
+      <c r="AKU42" s="35"/>
+      <c r="AKV42" s="35"/>
+      <c r="AKW42" s="35"/>
+      <c r="AKX42" s="35"/>
+      <c r="AKY42" s="35"/>
+      <c r="AKZ42" s="35"/>
+      <c r="ALA42" s="35"/>
+      <c r="ALB42" s="35"/>
+      <c r="ALC42" s="35"/>
+      <c r="ALD42" s="35"/>
+      <c r="ALE42" s="35"/>
+      <c r="ALF42" s="35"/>
+      <c r="ALG42" s="35"/>
+      <c r="ALH42" s="35"/>
+      <c r="ALI42" s="35"/>
+      <c r="ALJ42" s="35"/>
+      <c r="ALK42" s="35"/>
+      <c r="ALL42" s="35"/>
+      <c r="ALM42" s="35"/>
+      <c r="ALN42" s="35"/>
+      <c r="ALO42" s="35"/>
+      <c r="ALP42" s="35"/>
+      <c r="ALQ42" s="35"/>
+      <c r="ALR42" s="35"/>
+      <c r="ALS42" s="35"/>
+      <c r="ALT42" s="35"/>
+      <c r="ALU42" s="35"/>
+      <c r="ALV42" s="35"/>
+      <c r="ALW42" s="35"/>
+      <c r="ALX42" s="35"/>
+      <c r="ALY42" s="35"/>
+      <c r="ALZ42" s="35"/>
+      <c r="AMA42" s="35"/>
+      <c r="AMB42" s="35"/>
+      <c r="AMC42" s="35"/>
+      <c r="AMD42" s="35"/>
+      <c r="AME42" s="35"/>
+      <c r="AMF42" s="35"/>
+      <c r="AMG42" s="35"/>
+      <c r="AMH42" s="35"/>
+      <c r="AMI42" s="35"/>
+      <c r="AMJ42" s="35"/>
+      <c r="AMK42" s="35"/>
+    </row>
+    <row r="43" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
+      <c r="A43" s="31" t="s">
         <v>335</v>
       </c>
-      <c r="E42" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F42" s="0"/>
-    </row>
-    <row r="43" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="31" t="s">
+      <c r="B43" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="C43" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="D43" s="32" t="s">
         <v>338</v>
       </c>
-      <c r="D43" s="32" t="s">
+      <c r="E43" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="F43"/>
+    </row>
+    <row r="44" spans="1:1025" x14ac:dyDescent="0.25">
+      <c r="A44" s="31" t="s">
         <v>339</v>
       </c>
-      <c r="E43" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="F43" s="0"/>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="31" t="s">
+      <c r="B44" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="D44" s="32" t="s">
         <v>340</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="D44" s="32" t="s">
-        <v>341</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F44" s="0"/>
-    </row>
-    <row r="45" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F44"/>
+    </row>
+    <row r="45" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C45" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="D45" s="32" t="s">
         <v>343</v>
       </c>
-      <c r="D45" s="32" t="s">
+      <c r="E45" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="F45"/>
+    </row>
+    <row r="46" spans="1:1025" x14ac:dyDescent="0.25">
+      <c r="A46" s="31" t="s">
         <v>344</v>
       </c>
-      <c r="E45" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="F45" s="0"/>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="31" t="s">
+      <c r="B46" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C46" s="4" t="s">
+      <c r="D46" s="32" t="s">
         <v>346</v>
-      </c>
-      <c r="D46" s="32" t="s">
-        <v>347</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F46" s="0"/>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F46"/>
+    </row>
+    <row r="47" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A47" s="31" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>26</v>
@@ -4348,66 +5810,66 @@
         <v>148</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F47" s="0"/>
-    </row>
-    <row r="48" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F47"/>
+    </row>
+    <row r="48" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="31" t="s">
+        <v>349</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48"/>
+      <c r="D48" s="32" t="s">
         <v>350</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C48" s="0"/>
-      <c r="D48" s="32" t="s">
-        <v>351</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F48" s="0"/>
-    </row>
-    <row r="49" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F48"/>
+    </row>
+    <row r="49" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A49" s="31" t="s">
+        <v>351</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C49" s="4" t="s">
+      <c r="D49" s="32" t="s">
         <v>353</v>
-      </c>
-      <c r="D49" s="32" t="s">
-        <v>354</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F49" s="0"/>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F49"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="31" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C50" s="0"/>
+      <c r="C50"/>
       <c r="D50" s="32" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F50" s="0"/>
-    </row>
-    <row r="51" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F50"/>
+    </row>
+    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="31" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>26</v>
@@ -4416,16 +5878,16 @@
         <v>70</v>
       </c>
       <c r="D51" s="32" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F51" s="0"/>
-    </row>
-    <row r="52" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F51"/>
+    </row>
+    <row r="52" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="31" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>26</v>
@@ -4434,16 +5896,16 @@
         <v>70</v>
       </c>
       <c r="D52" s="32" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F52" s="0"/>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F52"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="31" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>26</v>
@@ -4452,18 +5914,18 @@
         <v>70</v>
       </c>
       <c r="D53" s="32" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F53" s="4" t="n">
+      <c r="F53" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="31" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>26</v>
@@ -4472,15 +5934,15 @@
         <v>70</v>
       </c>
       <c r="D54" s="32" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="31" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>98</v>
@@ -4489,15 +5951,15 @@
         <v>70</v>
       </c>
       <c r="D55" s="32" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="31" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>26</v>
@@ -4506,15 +5968,15 @@
         <v>70</v>
       </c>
       <c r="D56" s="32" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="31" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>26</v>
@@ -4523,15 +5985,15 @@
         <v>70</v>
       </c>
       <c r="D57" s="32" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="31" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>26</v>
@@ -4540,15 +6002,15 @@
         <v>70</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="31" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>103</v>
@@ -4557,66 +6019,66 @@
         <v>70</v>
       </c>
       <c r="D59" s="32" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="31" t="s">
+        <v>372</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="B60" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C60" s="4" t="s">
+      <c r="D60" s="32" t="s">
         <v>374</v>
-      </c>
-      <c r="D60" s="32" t="s">
-        <v>375</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="31" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>103</v>
       </c>
       <c r="C61" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D61" s="32" t="s">
         <v>377</v>
-      </c>
-      <c r="D61" s="32" t="s">
-        <v>378</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="31" t="s">
+        <v>378</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="B62" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C62" s="4" t="s">
+      <c r="D62" s="32" t="s">
         <v>380</v>
-      </c>
-      <c r="D62" s="32" t="s">
-        <v>381</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="31" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>17</v>
@@ -4625,15 +6087,15 @@
         <v>64</v>
       </c>
       <c r="D63" s="32" t="s">
+        <v>382</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A64" s="31" t="s">
         <v>383</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="31" t="s">
-        <v>384</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>17</v>
@@ -4642,19 +6104,14 @@
         <v>64</v>
       </c>
       <c r="D64" s="32" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Updated Excel "webinars_plus_issues_prior..." in notes folder - Removed System.out.println items in zipped .json export
</commit_message>
<xml_diff>
--- a/HarmonizationTool/notes/webinars_plus_issues_prior_to_2015-08-01.xlsx
+++ b/HarmonizationTool/notes/webinars_plus_issues_prior_to_2015-08-01.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="422">
   <si>
     <t>URLs</t>
   </si>
@@ -803,11 +803,6 @@
     <t>Choose Storage Location</t>
   </si>
   <si>
-    <t>Display a message if running LCA-HT the first time? Ie,
-"Choose your workspace." Where will the TDb live? And your workspace? Where would you like to store your projects? What is the project name? Do you want to work on an existing project or create a new one? "Choose a database storage location." "Choose a project and project directories."
-- Choose a database location. Then, where do you want to store yr project and what is your project called? Then, when you log in again, you can select from an existing list of projects.</t>
-  </si>
-  <si>
     <t>14:30</t>
   </si>
   <si>
@@ -978,9 +973,6 @@
   </si>
   <si>
     <t>41:44</t>
-  </si>
-  <si>
-    <t>Wes-Status boxes should feed back percentages; a single number, rather than 1/4, 2/4, etc.</t>
   </si>
   <si>
     <t>42:07</t>
@@ -1172,9 +1164,6 @@
   </si>
   <si>
     <t>1:12:20</t>
-  </si>
-  <si>
-    <t>Add NEXT UNMATCHED button to echo similar NEXT/NEXT UNMATCHED in Contexts and Properties</t>
   </si>
   <si>
     <t>1:12:47</t>
@@ -1330,12 +1319,98 @@
   <si>
     <t>Done</t>
   </si>
+  <si>
+    <t>Ready for testing</t>
+  </si>
+  <si>
+    <t>Priority (H,M,L)</t>
+  </si>
+  <si>
+    <t>Exists, but incomplete</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Difficulty (5 = hard 1 = Easy)</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Wes-Status boxes should feed back percentages; a single number, rather than 1/4, 2/4, etc.  Note: same as Row 19</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Add NEXT UNMATCHED button to echo similar NEXT/NEXT UNMATCHED in Contexts and Properties (like Row 46)</t>
+  </si>
+  <si>
+    <t>Display a message if running LCA-HT the first time? Ie,
+"Choose your workspace." Where will the TDb live? And your workspace? Where would you like to store your projects? What is the project name? Do you want to work on an existing project or create a new one? "Choose a database storage location." "Choose a project and project directories."
+- Choose a database location. Then, where do you want to store yr project and what is your project called? Then, when you log in again, you can select from an existing list of projects. See details in e-mail on 7-30-2015!</t>
+  </si>
+  <si>
+    <t>Discussion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very first run: 1) save logger info until Workspace can be defined.  2) TDB space is initialized in a folder named "TDB Database" which is a sibling  of executable file.  3) First run dialog says, "Welcome... Documentation... Credits... Please choose a workspace directory where LCA Harmonization Tool input, output, and log files may be placed."  The default is a folder called "Harmonization Tool Workspace", and it is located in the same folder with the executable, configuration, p2, TDB Database, and other files are.  Once selected, the workspace folder will get three subfolders only:  log, input, and output -- no projects for now.  The new log file will be placed in the log folder.  People can just use Datasets as projects.  Also, they don't get to choose the subfolders of the workspace, just the workspace location and name.  So, there is only one choice: workspace folder name and path.  4) If possible, update the progress bar that is inside the splash graphic with info like the fact that master flowables is being loaded. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subsequent runs: 1) Don't let a person run two concurrent runs.  2) Collect TDB and workspace info from preferences (stored automatically in configuration files).  3) Direct the new log file, 4) Show dialog with workspace directory and a "Don't show this dialog again" checkbox -- which is linked to a preferences checkbox.  5)    If possible, update the progress bar that is inside the splash graphic with things like the syncing from TDB </t>
+  </si>
+  <si>
+    <t>Bug? Click Next in Contexts tab takes me to the last row but does not cycle back to the top of the User Data tab</t>
+  </si>
+  <si>
+    <t>e-mail of 7-29 5:18p</t>
+  </si>
+  <si>
+    <t>Change the “View/Edit Meta Data” dialog to “Edit Metadata.” Metadata should be one word.</t>
+  </si>
+  <si>
+    <t>e-mail of 7-29 2:55p</t>
+  </si>
+  <si>
+    <t>Style: Change Name Data Set dialog box name to Rename Dataset</t>
+  </si>
+  <si>
+    <t>FlowContext, FlowProperty</t>
+  </si>
+  <si>
+    <t>e-mail of 7-29 3:05p</t>
+  </si>
+  <si>
+    <t>e-mail of 7-29 4:30p</t>
+  </si>
+  <si>
+    <t>Bug: Contexts and Properties tabs do not show summary detail nor highlighted unit/context.  Show "loading…" in Dialog prior to completion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question for Wes: What to do with "Length*area" and "Length*area/time" which are Land Transformations, but measure with physical hybrid props. </t>
+  </si>
+  <si>
+    <t>e-mail of 7-29 7:49p</t>
+  </si>
+  <si>
+    <t>FlowProperty</t>
+  </si>
+  <si>
+    <t>Question for PI</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1381,8 +1456,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1428,6 +1509,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1511,7 +1598,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1604,9 +1691,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1623,6 +1707,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1981,82 +2080,82 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.7109375" style="38" customWidth="1"/>
-    <col min="2" max="2" width="1.5703125" style="42" customWidth="1"/>
-    <col min="3" max="3" width="52.7109375" style="38" customWidth="1"/>
+    <col min="1" max="1" width="52.7109375" style="37" customWidth="1"/>
+    <col min="2" max="2" width="1.5703125" style="41" customWidth="1"/>
+    <col min="3" max="3" width="52.7109375" style="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
+        <v>382</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="33" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="40"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="40"/>
+    </row>
+    <row r="3" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
+        <v>388</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="33" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="39"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="39"/>
+    </row>
+    <row r="5" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="37" t="s">
+        <v>390</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="33" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="39"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="39"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
+        <v>391</v>
+      </c>
+      <c r="C7" s="37" t="s">
         <v>385</v>
       </c>
-      <c r="C1" s="39" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="33" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="41"/>
-    </row>
-    <row r="3" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
-        <v>391</v>
-      </c>
-      <c r="C3" s="38" t="s">
+    </row>
+    <row r="8" spans="1:3" s="33" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="39"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="39"/>
+    </row>
+    <row r="9" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" s="33" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="40"/>
-    </row>
-    <row r="5" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
-        <v>393</v>
-      </c>
-      <c r="C5" s="38" t="s">
+      <c r="C9" s="37" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="33" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="39"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="39"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="37" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" s="33" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="40"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
-        <v>394</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="33" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="40"/>
-    </row>
-    <row r="9" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="C11" s="37" t="s">
         <v>389</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="33" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="40"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
-        <v>390</v>
-      </c>
-      <c r="C11" s="38" t="s">
-        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -3940,10 +4039,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK64"/>
+  <dimension ref="A1:AML71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3952,11 +4053,14 @@
     <col min="3" max="3" width="24.85546875" style="4"/>
     <col min="4" max="4" width="67.28515625" style="5"/>
     <col min="5" max="5" width="14.7109375" style="4"/>
-    <col min="6" max="6" width="15.85546875" style="4"/>
-    <col min="7" max="1025" width="14.7109375" style="4"/>
+    <col min="6" max="6" width="7.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="4"/>
+    <col min="9" max="9" width="114.5703125" style="4" customWidth="1"/>
+    <col min="10" max="1026" width="14.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3972,14 +4076,20 @@
       <c r="E1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I1" s="4" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>25</v>
       </c>
@@ -3991,9 +4101,12 @@
       <c r="E2" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2"/>
+      <c r="H2" s="42" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>246</v>
       </c>
@@ -4009,9 +4122,17 @@
       <c r="E3" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="F3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>246</v>
       </c>
@@ -4027,12 +4148,12 @@
       <c r="E4" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F4"/>
-      <c r="G4" s="43" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="G4"/>
+      <c r="H4" s="42" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>251</v>
       </c>
@@ -4043,16 +4164,24 @@
         <v>252</v>
       </c>
       <c r="D5" s="32" t="s">
+        <v>405</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="31" t="s">
         <v>253</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F5"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
-        <v>254</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>26</v>
@@ -4061,14 +4190,22 @@
         <v>252</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F6"/>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="I6" s="46" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
       <c r="B7" s="4" t="s">
         <v>26</v>
@@ -4077,14 +4214,20 @@
         <v>252</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F7"/>
-    </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="I7" s="46"/>
+    </row>
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="31"/>
       <c r="B8" s="4" t="s">
         <v>26</v>
@@ -4093,14 +4236,15 @@
         <v>29</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F8"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+      <c r="G8"/>
+      <c r="I8" s="46"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
       <c r="B9" s="4" t="s">
         <v>26</v>
@@ -4109,14 +4253,20 @@
         <v>252</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F9"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="I9" s="46"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="31"/>
       <c r="B10" s="4" t="s">
         <v>98</v>
@@ -4125,16 +4275,16 @@
         <v>22</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="F10"/>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G10"/>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>26</v>
@@ -4143,14 +4293,19 @@
         <v>252</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F11"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="31"/>
       <c r="B12" s="4" t="s">
         <v>103</v>
@@ -4159,73 +4314,83 @@
         <v>198</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F12"/>
-      <c r="G12" s="43" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="G12"/>
+      <c r="H12" s="42" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
+        <v>262</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="32" t="s">
         <v>264</v>
       </c>
-      <c r="D13" s="32" t="s">
-        <v>265</v>
-      </c>
       <c r="E13" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
         <v>266</v>
       </c>
-      <c r="F13"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+      <c r="B14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="32" t="s">
         <v>268</v>
-      </c>
-      <c r="D14" s="32" t="s">
-        <v>269</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F14"/>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F14" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D15" s="32" t="s">
         <v>271</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>272</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="F15"/>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>103</v>
@@ -4234,16 +4399,21 @@
         <v>198</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F16"/>
-    </row>
-    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="F16" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>26</v>
@@ -4252,14 +4422,17 @@
         <v>191</v>
       </c>
       <c r="D17" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="F17"/>
-    </row>
-    <row r="18" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="F17" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>95</v>
       </c>
@@ -4270,66 +4443,79 @@
         <v>191</v>
       </c>
       <c r="D18" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="F18" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="s">
         <v>279</v>
       </c>
-      <c r="F18"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="B19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="D19" s="32" t="s">
         <v>281</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>282</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F19"/>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F19" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="D20" s="32" t="s">
         <v>284</v>
       </c>
-      <c r="D20" s="32" t="s">
+      <c r="E20" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="31" t="s">
         <v>285</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="F20"/>
-    </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
-        <v>286</v>
       </c>
       <c r="B21"/>
       <c r="C21" s="4" t="s">
         <v>90</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="F21"/>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="31"/>
       <c r="B22" s="4" t="s">
         <v>26</v>
@@ -4338,140 +4524,140 @@
         <v>90</v>
       </c>
       <c r="D22" s="32" t="s">
+        <v>287</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="G22"/>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="31" t="s">
         <v>288</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="F22"/>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="B23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="32" t="s">
         <v>290</v>
-      </c>
-      <c r="D23" s="32" t="s">
-        <v>291</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F23"/>
-    </row>
-    <row r="24" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="G23"/>
+    </row>
+    <row r="24" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
+        <v>291</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="D24" s="32" t="s">
         <v>292</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="D24" s="32" t="s">
-        <v>293</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F24"/>
-    </row>
-    <row r="25" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="G24"/>
+    </row>
+    <row r="25" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="D25" s="32" t="s">
         <v>294</v>
-      </c>
-      <c r="D25" s="32" t="s">
-        <v>295</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F25"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
+        <v>295</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="D26" s="32" t="s">
         <v>297</v>
       </c>
-      <c r="D26" s="32" t="s">
+      <c r="E26" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="G26"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="31" t="s">
         <v>298</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="F26"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
-        <v>299</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>103</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="D27" s="32" t="s">
         <v>300</v>
       </c>
-      <c r="D27" s="32" t="s">
+      <c r="E27" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="G27"/>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="31" t="s">
         <v>301</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="F27"/>
-    </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
+      <c r="B28" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="4" t="s">
+      <c r="D28" s="32" t="s">
         <v>303</v>
-      </c>
-      <c r="D28" s="32" t="s">
-        <v>304</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F28"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B29"/>
       <c r="C29" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D29" s="32" t="s">
+        <v>305</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="G29"/>
+    </row>
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="31" t="s">
         <v>306</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="F29"/>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="31" t="s">
-        <v>307</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>26</v>
@@ -4480,16 +4666,21 @@
         <v>90</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>308</v>
+        <v>402</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F30"/>
-    </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>26</v>
@@ -4498,14 +4689,14 @@
         <v>90</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F31"/>
-    </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G31"/>
+    </row>
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
         <v>143</v>
       </c>
@@ -4513,58 +4704,63 @@
         <v>26</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F32"/>
-    </row>
-    <row r="33" spans="1:1025" x14ac:dyDescent="0.25">
+      <c r="G32"/>
+    </row>
+    <row r="33" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D33" s="32" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F33"/>
-    </row>
-    <row r="34" spans="1:1025" x14ac:dyDescent="0.25">
+      <c r="F33" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F34"/>
-      <c r="G34" s="43" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+      <c r="G34"/>
+      <c r="H34" s="42" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1026" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>103</v>
@@ -4573,16 +4769,21 @@
         <v>70</v>
       </c>
       <c r="D35" s="32" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F35"/>
-    </row>
-    <row r="36" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
+      <c r="F35" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1026" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>98</v>
@@ -4591,16 +4792,16 @@
         <v>90</v>
       </c>
       <c r="D36" s="32" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="F36"/>
-    </row>
-    <row r="37" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+      <c r="G36"/>
+    </row>
+    <row r="37" spans="1:1026" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>103</v>
@@ -4609,106 +4810,131 @@
         <v>90</v>
       </c>
       <c r="D37" s="32" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F37"/>
-    </row>
-    <row r="38" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+      <c r="F37" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="G37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1026" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>103</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D38" s="32" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F38"/>
-    </row>
-    <row r="39" spans="1:1025" x14ac:dyDescent="0.25">
+      <c r="F38" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>103</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D39" s="32" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F39"/>
-      <c r="G39" s="43" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1025" ht="60" x14ac:dyDescent="0.25">
+      <c r="G39"/>
+      <c r="H39" s="42" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1026" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
+        <v>326</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="D40" s="32" t="s">
         <v>328</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="D40" s="32" t="s">
-        <v>330</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F40"/>
-    </row>
-    <row r="41" spans="1:1025" ht="60" x14ac:dyDescent="0.25">
+      <c r="F40" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1026" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C41" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="D41" s="32" t="s">
+        <v>330</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="G41"/>
+    </row>
+    <row r="42" spans="1:1026" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="34" t="s">
         <v>331</v>
       </c>
-      <c r="D41" s="32" t="s">
+      <c r="B42" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="D42" s="45" t="s">
         <v>332</v>
       </c>
-      <c r="E41" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="F41"/>
-    </row>
-    <row r="42" spans="1:1025" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="34" t="s">
-        <v>333</v>
-      </c>
-      <c r="B42" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="C42" s="35" t="s">
-        <v>148</v>
-      </c>
-      <c r="D42" s="36" t="s">
-        <v>334</v>
-      </c>
-      <c r="E42" s="35" t="s">
+      <c r="E42" s="44" t="s">
         <v>245</v>
       </c>
-      <c r="G42" s="35"/>
-      <c r="H42" s="35"/>
+      <c r="F42" s="35" t="s">
+        <v>403</v>
+      </c>
+      <c r="G42" s="36">
+        <v>5</v>
+      </c>
+      <c r="H42" s="43" t="s">
+        <v>394</v>
+      </c>
       <c r="I42" s="35"/>
       <c r="J42" s="35"/>
       <c r="K42" s="35"/>
@@ -5726,82 +5952,101 @@
       <c r="AMI42" s="35"/>
       <c r="AMJ42" s="35"/>
       <c r="AMK42" s="35"/>
-    </row>
-    <row r="43" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
+      <c r="AML42" s="35"/>
+    </row>
+    <row r="43" spans="1:1026" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
+        <v>333</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="D43" s="32" t="s">
         <v>336</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="E43" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A44" s="31" t="s">
         <v>337</v>
       </c>
-      <c r="D43" s="32" t="s">
+      <c r="B44" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="D44" s="32" t="s">
         <v>338</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="F43"/>
-    </row>
-    <row r="44" spans="1:1025" x14ac:dyDescent="0.25">
-      <c r="A44" s="31" t="s">
-        <v>339</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="D44" s="32" t="s">
-        <v>340</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F44"/>
-    </row>
-    <row r="45" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+      <c r="F44" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1026" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C45" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="D45" s="32" t="s">
+        <v>341</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G45"/>
+    </row>
+    <row r="46" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A46" s="31" t="s">
         <v>342</v>
       </c>
-      <c r="D45" s="32" t="s">
+      <c r="B46" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="E45" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="F45"/>
-    </row>
-    <row r="46" spans="1:1025" x14ac:dyDescent="0.25">
-      <c r="A46" s="31" t="s">
+      <c r="D46" s="32" t="s">
         <v>344</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="D46" s="32" t="s">
-        <v>346</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F46"/>
-    </row>
-    <row r="47" spans="1:1025" x14ac:dyDescent="0.25">
+      <c r="F46" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A47" s="31" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>26</v>
@@ -5810,66 +6055,81 @@
         <v>148</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F47"/>
-    </row>
-    <row r="48" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+      <c r="F47" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1026" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="31" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C48"/>
       <c r="D48" s="32" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F48"/>
-    </row>
-    <row r="49" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="G48"/>
+    </row>
+    <row r="49" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A49" s="31" t="s">
+        <v>349</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="D49" s="32" t="s">
         <v>351</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="D49" s="32" t="s">
-        <v>353</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F49"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F49" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="G49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="31" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C50"/>
       <c r="D50" s="32" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F50"/>
-    </row>
-    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F50" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="G50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="31" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>26</v>
@@ -5878,16 +6138,21 @@
         <v>70</v>
       </c>
       <c r="D51" s="32" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F51"/>
-    </row>
-    <row r="52" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="F51" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="G51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="31" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>26</v>
@@ -5896,16 +6161,21 @@
         <v>70</v>
       </c>
       <c r="D52" s="32" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F52"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F52" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="G52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="31" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>26</v>
@@ -5914,18 +6184,21 @@
         <v>70</v>
       </c>
       <c r="D53" s="32" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F53" s="4">
+      <c r="F53" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="G53" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="31" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>26</v>
@@ -5934,15 +6207,21 @@
         <v>70</v>
       </c>
       <c r="D54" s="32" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F54" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G54" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="31" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>98</v>
@@ -5951,15 +6230,15 @@
         <v>70</v>
       </c>
       <c r="D55" s="32" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="31" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>26</v>
@@ -5968,15 +6247,21 @@
         <v>70</v>
       </c>
       <c r="D56" s="32" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F56" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G56" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="31" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>26</v>
@@ -5985,15 +6270,21 @@
         <v>70</v>
       </c>
       <c r="D57" s="32" t="s">
-        <v>367</v>
+        <v>404</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F57" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G57" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="31" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>26</v>
@@ -6002,15 +6293,21 @@
         <v>70</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F58" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="G58" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="31" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>103</v>
@@ -6019,66 +6316,87 @@
         <v>70</v>
       </c>
       <c r="D59" s="32" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F59" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="G59" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="31" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D60" s="32" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F60" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="G60" s="4">
+        <v>3</v>
+      </c>
+      <c r="H60" s="42" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="31" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>103</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D61" s="32" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H61" s="42" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="31" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D62" s="32" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H62" s="42" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="31" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>17</v>
@@ -6087,15 +6405,15 @@
         <v>64</v>
       </c>
       <c r="D63" s="32" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="31" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>17</v>
@@ -6104,14 +6422,137 @@
         <v>64</v>
       </c>
       <c r="D64" s="32" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D65" s="47" t="s">
+        <v>411</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G65" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D66" s="47" t="s">
+        <v>413</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G66" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="G67" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="G68" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="G69" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D71" s="5" t="s">
+        <v>400</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I6:I9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Updated webinars_plus... spreadsheet / todo list.
</commit_message>
<xml_diff>
--- a/HarmonizationTool/notes/webinars_plus_issues_prior_to_2015-08-01.xlsx
+++ b/HarmonizationTool/notes/webinars_plus_issues_prior_to_2015-08-01.xlsx
@@ -16,13 +16,15 @@
     <sheet name="Instructions" sheetId="1" r:id="rId2"/>
     <sheet name="7-21" sheetId="2" r:id="rId3"/>
     <sheet name="7-24" sheetId="3" r:id="rId4"/>
+    <sheet name="Text choices" sheetId="5" r:id="rId5"/>
+    <sheet name="Workflow states" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="523">
   <si>
     <t>URLs</t>
   </si>
@@ -1405,12 +1407,315 @@
   <si>
     <t>Question for PI</t>
   </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Current Name</t>
+  </si>
+  <si>
+    <t>Proposed New</t>
+  </si>
+  <si>
+    <t>Windows folder</t>
+  </si>
+  <si>
+    <t>Name of folder containing the LCA-HT executable and files</t>
+  </si>
+  <si>
+    <t>LCA-HarmonizationTool</t>
+  </si>
+  <si>
+    <t>Name of the LCA executable file</t>
+  </si>
+  <si>
+    <t>LCA-HT.exe</t>
+  </si>
+  <si>
+    <t>Mouseover Taskbar icon for LCA-HT; Window title of LCA-HT; Task Manager Application Name</t>
+  </si>
+  <si>
+    <t>Name of the LCA-HT Application</t>
+  </si>
+  <si>
+    <t>LCA-Harmonization Tool</t>
+  </si>
+  <si>
+    <t>1. User Data</t>
+  </si>
+  <si>
+    <t>2. Format</t>
+  </si>
+  <si>
+    <t>3. Save+Match</t>
+  </si>
+  <si>
+    <t>4. Flow Context</t>
+  </si>
+  <si>
+    <t>5. Flow Unit</t>
+  </si>
+  <si>
+    <t>7. Finish</t>
+  </si>
+  <si>
+    <t>6. Flowable</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Load…</t>
+  </si>
+  <si>
+    <t>Check Data</t>
+  </si>
+  <si>
+    <t>Begin</t>
+  </si>
+  <si>
+    <t>Show Unique</t>
+  </si>
+  <si>
+    <t>22% (loading)</t>
+  </si>
+  <si>
+    <t>electricity.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ... checking data ...</t>
+  </si>
+  <si>
+    <t>Tooltip Action</t>
+  </si>
+  <si>
+    <t>Tooltip Status</t>
+  </si>
+  <si>
+    <t>Click to load user data.  To load reference (master) data, see Advanced -&gt; Load Reference Data List...</t>
+  </si>
+  <si>
+    <t>User data includes any dataset the user wishes to harmonize.</t>
+  </si>
+  <si>
+    <t>Prior to saving and matching LCA data, data formats are checked for common errors.</t>
+  </si>
+  <si>
+    <t>In this step, user data is written to the database and matched against master data.  Canceling prior to the completion of this set means that user data is not saved.</t>
+  </si>
+  <si>
+    <t>The Flow Unit and its corresponding Flow Property must be matched for an LCA Flow to match.</t>
+  </si>
+  <si>
+    <t>The LCA-Harmonization Tool chooses the term "Flow Context" to represent a term often called category or compartment.  The Flow Context must match for a user Flow to match a master Flow.</t>
+  </si>
+  <si>
+    <t>In the LCA-Harmonization Tool, Flowables are matched indendently of Flows so that like Flowables can be scrutinized as a group.</t>
+  </si>
+  <si>
+    <t>In this step, users may export harmonized data or cancel if prior to completing step 3.</t>
+  </si>
+  <si>
+    <t>Load in progress…</t>
+  </si>
+  <si>
+    <t>[File path]</t>
+  </si>
+  <si>
+    <t>Click to run format checks.</t>
+  </si>
+  <si>
+    <t>1. Opening</t>
+  </si>
+  <si>
+    <t>2. Running step 1</t>
+  </si>
+  <si>
+    <t>3. End of step 1</t>
+  </si>
+  <si>
+    <t>4. During step 2</t>
+  </si>
+  <si>
+    <t>Checking…</t>
+  </si>
+  <si>
+    <t>0 issues, 8 columns checked</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>To see info about issues [more..]</t>
+  </si>
+  <si>
+    <t>5. Following step 2 (if  issues)</t>
+  </si>
+  <si>
+    <t>3 issues, 8 columns checked</t>
+  </si>
+  <si>
+    <t>Issues must be resolved prior to Save+Match</t>
+  </si>
+  <si>
+    <t>Click to begin saving to database and matching data</t>
+  </si>
+  <si>
+    <t>6. Following step 2 (if no issues)</t>
+  </si>
+  <si>
+    <t>7. During step 3</t>
+  </si>
+  <si>
+    <t>Cancel…</t>
+  </si>
+  <si>
+    <t>Click to cancel the Save &amp; Match process.</t>
+  </si>
+  <si>
+    <t>14% (matching components)</t>
+  </si>
+  <si>
+    <t>3 matched, 4 found</t>
+  </si>
+  <si>
+    <t>2 matched, 2 found</t>
+  </si>
+  <si>
+    <t>8. Following step 3</t>
+  </si>
+  <si>
+    <t>Click to cancel working with this dataset.  Nothing will be saved to the database.</t>
+  </si>
+  <si>
+    <t>Suggestion</t>
+  </si>
+  <si>
+    <t>Allow for cancel loading?</t>
+  </si>
+  <si>
+    <t>Export…</t>
+  </si>
+  <si>
+    <t>Click to export this dataset to any of several formats.</t>
+  </si>
+  <si>
+    <t>23 matched, 25 found</t>
+  </si>
+  <si>
+    <t>8 matched, 8 found</t>
+  </si>
+  <si>
+    <t>7 matched, 8 found</t>
+  </si>
+  <si>
+    <t>6 matched, 6 found</t>
+  </si>
+  <si>
+    <t>14 matched, 15 found</t>
+  </si>
+  <si>
+    <t>A total of 8 distinct Flow Contexts were found, and 7 have been matched to master Flow Contexts</t>
+  </si>
+  <si>
+    <t>A total of 6 distinct Flow Units were found, and 6 have been matched to master Flow Units</t>
+  </si>
+  <si>
+    <t>Show All</t>
+  </si>
+  <si>
+    <t>You must click "Show All" next to "5. Flow Unit" to use this function.</t>
+  </si>
+  <si>
+    <t>Click to show all rows in the User Data table.</t>
+  </si>
+  <si>
+    <t>Click to show only the first row with each of the 8 distinct Flow Contexts in the User Data table.</t>
+  </si>
+  <si>
+    <t>Click to show only the first row with each of the 6 distinct Flow Units in the User Data table.</t>
+  </si>
+  <si>
+    <t>Click to show only the first row with each of the 25 distinct Flowables in the User Data table.</t>
+  </si>
+  <si>
+    <t>User data has been saved to the database and matched against master data.  Results are shown below.</t>
+  </si>
+  <si>
+    <t>A total of 8 distinct Flow Contexts were found, and 8 have been matched to master Flow Contexts</t>
+  </si>
+  <si>
+    <t>25 matched, 25 found</t>
+  </si>
+  <si>
+    <t>A total of 25 distinct Flowables were found, and 25 have been matched to master Flowables</t>
+  </si>
+  <si>
+    <t>A total of 25 distinct Flowables were found, and 23 have been matched to master Flowables</t>
+  </si>
+  <si>
+    <t>Click to cancel the export process.</t>
+  </si>
+  <si>
+    <t>23% (oragnizing components)</t>
+  </si>
+  <si>
+    <t>Click to load a new user dataset.  Current data may be reloaded in the future to continue harmonization.  To re-load a previously laoded dataset, use the menu item "DataSet -&gt; Reload dataset". To load reference (master) data, see Advanced -&gt; Load Reference Data List...</t>
+  </si>
+  <si>
+    <t>9. Following step 3, if 4 is toggled</t>
+  </si>
+  <si>
+    <t>You must click "Show All" next to "4. Flow Context" to use this function.</t>
+  </si>
+  <si>
+    <t>10. Following step 3, if 5 is toggled</t>
+  </si>
+  <si>
+    <t>11. Following step 3, if 6 is toggled</t>
+  </si>
+  <si>
+    <t>You must click "Show All" next to "6. Flowable" to use this function.</t>
+  </si>
+  <si>
+    <t>12. During step 7 (following dialogs)</t>
+  </si>
+  <si>
+    <t>Examples of what may be show in the Status window</t>
+  </si>
+  <si>
+    <t>Boolean for action enabled and not grayed</t>
+  </si>
+  <si>
+    <t>Tooltip for field to left</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Load new data…</t>
+  </si>
+  <si>
+    <t>done for step 1</t>
+  </si>
+  <si>
+    <t>some in tooltips.  See the new Workflow states Worksheet in this Excel workbook.</t>
+  </si>
+  <si>
+    <t>some</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1461,6 +1766,26 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1519,7 +1844,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1593,12 +1918,107 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1718,10 +2138,98 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4041,10 +4549,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C70" sqref="C70"/>
+      <selection pane="bottomLeft" activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4053,14 +4561,14 @@
     <col min="3" max="3" width="24.85546875" style="4"/>
     <col min="4" max="4" width="67.28515625" style="5"/>
     <col min="5" max="5" width="14.7109375" style="4"/>
-    <col min="6" max="6" width="7.28515625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="46" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="46" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" style="4"/>
     <col min="9" max="9" width="114.5703125" style="4" customWidth="1"/>
     <col min="10" max="1026" width="14.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -4076,10 +4584,10 @@
       <c r="E1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="47" t="s">
         <v>395</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="47" t="s">
         <v>398</v>
       </c>
       <c r="H1" s="4" t="s">
@@ -4101,7 +4609,6 @@
       <c r="E2" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="G2"/>
       <c r="H2" s="42" t="s">
         <v>393</v>
       </c>
@@ -4122,10 +4629,10 @@
       <c r="E3" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="46" t="s">
         <v>397</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="46">
         <v>2</v>
       </c>
       <c r="H3" s="4" t="s">
@@ -4148,7 +4655,6 @@
       <c r="E4" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="G4"/>
       <c r="H4" s="42" t="s">
         <v>393</v>
       </c>
@@ -4169,10 +4675,10 @@
       <c r="E5" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="46">
         <v>3</v>
       </c>
       <c r="I5" s="5" t="s">
@@ -4195,13 +4701,13 @@
       <c r="E6" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="46">
         <v>2</v>
       </c>
-      <c r="I6" s="46" t="s">
+      <c r="I6" s="85" t="s">
         <v>408</v>
       </c>
     </row>
@@ -4219,13 +4725,13 @@
       <c r="E7" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="46" t="s">
         <v>397</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="46">
         <v>3</v>
       </c>
-      <c r="I7" s="46"/>
+      <c r="I7" s="85"/>
     </row>
     <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="31"/>
@@ -4241,8 +4747,7 @@
       <c r="E8" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="G8"/>
-      <c r="I8" s="46"/>
+      <c r="I8" s="85"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
@@ -4258,13 +4763,13 @@
       <c r="E9" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="46" t="s">
         <v>397</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="46">
         <v>3</v>
       </c>
-      <c r="I9" s="46"/>
+      <c r="I9" s="85"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="31"/>
@@ -4280,7 +4785,6 @@
       <c r="E10" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="G10"/>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
@@ -4298,10 +4802,10 @@
       <c r="E11" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="46">
         <v>2</v>
       </c>
     </row>
@@ -4319,7 +4823,6 @@
       <c r="E12" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="G12"/>
       <c r="H12" s="42" t="s">
         <v>393</v>
       </c>
@@ -4340,10 +4843,10 @@
       <c r="E13" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="46">
         <v>1</v>
       </c>
     </row>
@@ -4363,10 +4866,10 @@
       <c r="E14" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="46">
         <v>2</v>
       </c>
     </row>
@@ -4386,7 +4889,6 @@
       <c r="E15" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="G15"/>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
@@ -4404,14 +4906,14 @@
       <c r="E16" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="46">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
         <v>274</v>
       </c>
@@ -4427,12 +4929,11 @@
       <c r="E17" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="46" t="s">
         <v>397</v>
       </c>
-      <c r="G17"/>
-    </row>
-    <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>95</v>
       </c>
@@ -4448,12 +4949,14 @@
       <c r="E18" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="G18"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18" s="4" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>279</v>
       </c>
@@ -4469,14 +4972,17 @@
       <c r="E19" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="46">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H19" s="4" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>282</v>
       </c>
@@ -4492,14 +4998,17 @@
       <c r="E20" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="46">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I20" s="4" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
         <v>285</v>
       </c>
@@ -4513,9 +5022,11 @@
       <c r="E21" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="G21"/>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I21" s="4" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="31"/>
       <c r="B22" s="4" t="s">
         <v>26</v>
@@ -4529,9 +5040,11 @@
       <c r="E22" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="G22"/>
-    </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H22" s="42" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
         <v>288</v>
       </c>
@@ -4547,9 +5060,8 @@
       <c r="E23" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="G23"/>
-    </row>
-    <row r="24" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
         <v>291</v>
       </c>
@@ -4565,9 +5077,8 @@
       <c r="E24" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="G24"/>
-    </row>
-    <row r="25" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
         <v>291</v>
       </c>
@@ -4583,9 +5094,8 @@
       <c r="E25" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="G25"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
         <v>295</v>
       </c>
@@ -4601,9 +5111,8 @@
       <c r="E26" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="G26"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
         <v>298</v>
       </c>
@@ -4619,9 +5128,8 @@
       <c r="E27" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="G27"/>
-    </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
         <v>301</v>
       </c>
@@ -4637,9 +5145,8 @@
       <c r="E28" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="G28"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
         <v>304</v>
       </c>
@@ -4653,9 +5160,8 @@
       <c r="E29" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="G29"/>
-    </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
         <v>306</v>
       </c>
@@ -4671,14 +5177,14 @@
       <c r="E30" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="46">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>307</v>
       </c>
@@ -4694,9 +5200,8 @@
       <c r="E31" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="G31"/>
-    </row>
-    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
         <v>143</v>
       </c>
@@ -4712,7 +5217,6 @@
       <c r="E32" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="G32"/>
     </row>
     <row r="33" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
@@ -4730,10 +5234,10 @@
       <c r="E33" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="F33" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="46">
         <v>1</v>
       </c>
     </row>
@@ -4753,7 +5257,6 @@
       <c r="E34" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="G34"/>
       <c r="H34" s="42" t="s">
         <v>393</v>
       </c>
@@ -4774,10 +5277,10 @@
       <c r="E35" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F35" s="46" t="s">
         <v>403</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="46">
         <v>2</v>
       </c>
     </row>
@@ -4797,7 +5300,6 @@
       <c r="E36" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="G36"/>
     </row>
     <row r="37" spans="1:1026" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
@@ -4815,10 +5317,10 @@
       <c r="E37" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="F37" s="46" t="s">
         <v>403</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="46">
         <v>3</v>
       </c>
     </row>
@@ -4838,10 +5340,10 @@
       <c r="E38" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F38" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="46">
         <v>1</v>
       </c>
     </row>
@@ -4861,7 +5363,6 @@
       <c r="E39" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="G39"/>
       <c r="H39" s="42" t="s">
         <v>393</v>
       </c>
@@ -4882,10 +5383,10 @@
       <c r="E40" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F40" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="46">
         <v>3</v>
       </c>
     </row>
@@ -4905,10 +5406,9 @@
       <c r="E41" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="F41" s="46" t="s">
         <v>403</v>
       </c>
-      <c r="G41"/>
     </row>
     <row r="42" spans="1:1026" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="34" t="s">
@@ -4926,10 +5426,10 @@
       <c r="E42" s="44" t="s">
         <v>245</v>
       </c>
-      <c r="F42" s="35" t="s">
+      <c r="F42" s="49" t="s">
         <v>403</v>
       </c>
-      <c r="G42" s="36">
+      <c r="G42" s="49">
         <v>5</v>
       </c>
       <c r="H42" s="43" t="s">
@@ -5970,10 +6470,10 @@
       <c r="E43" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F43" s="46" t="s">
         <v>403</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="46">
         <v>3</v>
       </c>
     </row>
@@ -5993,10 +6493,10 @@
       <c r="E44" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F44" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="46">
         <v>1</v>
       </c>
     </row>
@@ -6016,10 +6516,9 @@
       <c r="E45" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="F45" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="G45"/>
     </row>
     <row r="46" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A46" s="31" t="s">
@@ -6037,10 +6536,10 @@
       <c r="E46" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="F46" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="46">
         <v>2</v>
       </c>
     </row>
@@ -6060,11 +6559,14 @@
       <c r="E47" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F47" s="4" t="s">
+      <c r="F47" s="46" t="s">
         <v>403</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="46">
         <v>1</v>
+      </c>
+      <c r="H47" s="42" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="48" spans="1:1026" ht="30" x14ac:dyDescent="0.25">
@@ -6081,7 +6583,9 @@
       <c r="E48" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="G48"/>
+      <c r="H48" s="42" t="s">
+        <v>393</v>
+      </c>
     </row>
     <row r="49" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A49" s="31" t="s">
@@ -6099,11 +6603,14 @@
       <c r="E49" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F49" s="4" t="s">
+      <c r="F49" s="46" t="s">
         <v>403</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="46">
         <v>4</v>
+      </c>
+      <c r="H49" s="42" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -6118,12 +6625,12 @@
         <v>353</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="F50" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="F50" s="46" t="s">
         <v>403</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="46">
         <v>3</v>
       </c>
     </row>
@@ -6143,10 +6650,10 @@
       <c r="E51" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F51" s="4" t="s">
+      <c r="F51" s="46" t="s">
         <v>397</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="46">
         <v>2</v>
       </c>
     </row>
@@ -6166,10 +6673,10 @@
       <c r="E52" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F52" s="4" t="s">
+      <c r="F52" s="46" t="s">
         <v>403</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="46">
         <v>3</v>
       </c>
     </row>
@@ -6189,10 +6696,10 @@
       <c r="E53" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F53" s="4" t="s">
+      <c r="F53" s="46" t="s">
         <v>397</v>
       </c>
-      <c r="G53" s="4">
+      <c r="G53" s="46">
         <v>1</v>
       </c>
     </row>
@@ -6212,10 +6719,10 @@
       <c r="E54" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F54" s="4" t="s">
+      <c r="F54" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="G54" s="4">
+      <c r="G54" s="46">
         <v>1</v>
       </c>
     </row>
@@ -6252,10 +6759,10 @@
       <c r="E56" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F56" s="4" t="s">
+      <c r="F56" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="G56" s="4">
+      <c r="G56" s="46">
         <v>1</v>
       </c>
     </row>
@@ -6275,10 +6782,10 @@
       <c r="E57" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F57" s="4" t="s">
+      <c r="F57" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="G57" s="4">
+      <c r="G57" s="46">
         <v>2</v>
       </c>
     </row>
@@ -6298,10 +6805,10 @@
       <c r="E58" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F58" s="4" t="s">
+      <c r="F58" s="46" t="s">
         <v>397</v>
       </c>
-      <c r="G58" s="4">
+      <c r="G58" s="46">
         <v>2</v>
       </c>
     </row>
@@ -6321,10 +6828,10 @@
       <c r="E59" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F59" s="4" t="s">
+      <c r="F59" s="46" t="s">
         <v>403</v>
       </c>
-      <c r="G59" s="4">
+      <c r="G59" s="46">
         <v>3</v>
       </c>
     </row>
@@ -6344,10 +6851,10 @@
       <c r="E60" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F60" s="4" t="s">
+      <c r="F60" s="46" t="s">
         <v>403</v>
       </c>
-      <c r="G60" s="4">
+      <c r="G60" s="46">
         <v>3</v>
       </c>
       <c r="H60" s="42" t="s">
@@ -6410,6 +6917,9 @@
       <c r="E63" s="4" t="s">
         <v>278</v>
       </c>
+      <c r="H63" s="4" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="31" t="s">
@@ -6428,7 +6938,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>412</v>
       </c>
@@ -6438,20 +6948,23 @@
       <c r="C65" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D65" s="47" t="s">
+      <c r="D65" s="48" t="s">
         <v>411</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="F65" s="4" t="s">
+      <c r="F65" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="G65" s="4">
+      <c r="G65" s="46">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H65" s="42" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>415</v>
       </c>
@@ -6461,20 +6974,20 @@
       <c r="C66" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D66" s="47" t="s">
+      <c r="D66" s="48" t="s">
         <v>413</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="F66" s="4" t="s">
+      <c r="F66" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="G66" s="4">
+      <c r="G66" s="46">
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>410</v>
       </c>
@@ -6490,14 +7003,14 @@
       <c r="E67" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F67" s="4" t="s">
+      <c r="F67" s="46" t="s">
         <v>397</v>
       </c>
-      <c r="G67" s="4">
+      <c r="G67" s="46">
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>416</v>
       </c>
@@ -6513,14 +7026,14 @@
       <c r="E68" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F68" s="4" t="s">
+      <c r="F68" s="46" t="s">
         <v>397</v>
       </c>
-      <c r="G68" s="4">
+      <c r="G68" s="46">
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>419</v>
       </c>
@@ -6536,14 +7049,14 @@
       <c r="E69" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F69" s="4" t="s">
+      <c r="F69" s="46" t="s">
         <v>397</v>
       </c>
-      <c r="G69" s="4">
+      <c r="G69" s="46">
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D71" s="5" t="s">
         <v>400</v>
       </c>
@@ -6555,4 +7068,1948 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25" style="37" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="37" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>422</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>423</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
+        <v>425</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>426</v>
+      </c>
+      <c r="C2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
+        <v>425</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>428</v>
+      </c>
+      <c r="C3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
+        <v>430</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>431</v>
+      </c>
+      <c r="C4" t="s">
+        <v>432</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J123"/>
+  <sheetViews>
+    <sheetView showFormulas="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D74" sqref="D74"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.140625" style="52" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="62" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="54" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" style="52" customWidth="1"/>
+    <col min="5" max="7" width="17.7109375" style="54" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="60" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="52"/>
+    <col min="10" max="10" width="9.140625" style="63"/>
+    <col min="11" max="16384" width="9.140625" style="52"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="66" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="66" t="s">
+        <v>518</v>
+      </c>
+      <c r="B1" s="71" t="s">
+        <v>440</v>
+      </c>
+      <c r="C1" s="68" t="s">
+        <v>441</v>
+      </c>
+      <c r="D1" s="68" t="s">
+        <v>515</v>
+      </c>
+      <c r="E1" s="68" t="s">
+        <v>449</v>
+      </c>
+      <c r="F1" s="68" t="s">
+        <v>514</v>
+      </c>
+      <c r="G1" s="68" t="s">
+        <v>450</v>
+      </c>
+      <c r="H1" s="67" t="s">
+        <v>483</v>
+      </c>
+      <c r="I1" s="76" t="s">
+        <v>517</v>
+      </c>
+      <c r="J1" s="77" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="52">
+        <v>0</v>
+      </c>
+      <c r="B2" s="74" t="s">
+        <v>462</v>
+      </c>
+      <c r="C2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="79"/>
+    </row>
+    <row r="3" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="52">
+        <v>1</v>
+      </c>
+      <c r="B3" s="62" t="s">
+        <v>433</v>
+      </c>
+      <c r="C3" s="54" t="s">
+        <v>442</v>
+      </c>
+      <c r="D3" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="54" t="s">
+        <v>451</v>
+      </c>
+      <c r="I3" s="80" t="s">
+        <v>433</v>
+      </c>
+      <c r="J3" s="81" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="52">
+        <v>2</v>
+      </c>
+      <c r="B4" s="62" t="s">
+        <v>434</v>
+      </c>
+      <c r="C4" s="55" t="s">
+        <v>443</v>
+      </c>
+      <c r="D4" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="80" t="s">
+        <v>434</v>
+      </c>
+      <c r="J4" s="81" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="52">
+        <v>3</v>
+      </c>
+      <c r="B5" s="62" t="s">
+        <v>435</v>
+      </c>
+      <c r="C5" s="55" t="s">
+        <v>444</v>
+      </c>
+      <c r="D5" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="82" t="s">
+        <v>435</v>
+      </c>
+      <c r="J5" s="81" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="52">
+        <v>4</v>
+      </c>
+      <c r="B6" s="62" t="s">
+        <v>436</v>
+      </c>
+      <c r="C6" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D6" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="80" t="s">
+        <v>436</v>
+      </c>
+      <c r="J6" s="81" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="52">
+        <v>5</v>
+      </c>
+      <c r="B7" s="62" t="s">
+        <v>437</v>
+      </c>
+      <c r="C7" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D7" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="80" t="s">
+        <v>437</v>
+      </c>
+      <c r="J7" s="81" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="52">
+        <v>6</v>
+      </c>
+      <c r="B8" s="62" t="s">
+        <v>439</v>
+      </c>
+      <c r="C8" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D8" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="80" t="s">
+        <v>439</v>
+      </c>
+      <c r="J8" s="81" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="66" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="52">
+        <v>7</v>
+      </c>
+      <c r="B9" s="73" t="s">
+        <v>438</v>
+      </c>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="83" t="s">
+        <v>438</v>
+      </c>
+      <c r="J9" s="84" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="52">
+        <v>0</v>
+      </c>
+      <c r="B10" s="74" t="s">
+        <v>463</v>
+      </c>
+      <c r="C10" s="53"/>
+      <c r="D10" s="54"/>
+      <c r="F10" s="53"/>
+      <c r="H10" s="60" t="s">
+        <v>484</v>
+      </c>
+      <c r="J10" s="52"/>
+    </row>
+    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="52">
+        <v>1</v>
+      </c>
+      <c r="B11" s="62" t="s">
+        <v>433</v>
+      </c>
+      <c r="C11" s="55" t="s">
+        <v>442</v>
+      </c>
+      <c r="D11" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="54" t="s">
+        <v>459</v>
+      </c>
+      <c r="F11" s="54" t="s">
+        <v>446</v>
+      </c>
+      <c r="J11" s="52"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="52">
+        <v>2</v>
+      </c>
+      <c r="B12" s="62" t="s">
+        <v>434</v>
+      </c>
+      <c r="C12" s="55" t="s">
+        <v>443</v>
+      </c>
+      <c r="D12" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="52"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="52">
+        <v>3</v>
+      </c>
+      <c r="B13" s="62" t="s">
+        <v>435</v>
+      </c>
+      <c r="C13" s="55" t="s">
+        <v>444</v>
+      </c>
+      <c r="D13" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="52"/>
+    </row>
+    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="52">
+        <v>4</v>
+      </c>
+      <c r="B14" s="62" t="s">
+        <v>436</v>
+      </c>
+      <c r="C14" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D14" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" s="52"/>
+    </row>
+    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="52">
+        <v>5</v>
+      </c>
+      <c r="B15" s="62" t="s">
+        <v>437</v>
+      </c>
+      <c r="C15" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D15" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="52"/>
+    </row>
+    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="52">
+        <v>6</v>
+      </c>
+      <c r="B16" s="62" t="s">
+        <v>439</v>
+      </c>
+      <c r="C16" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D16" s="55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="66" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="52">
+        <v>7</v>
+      </c>
+      <c r="B17" s="73" t="s">
+        <v>438</v>
+      </c>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="69"/>
+      <c r="J17" s="70"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="52">
+        <v>0</v>
+      </c>
+      <c r="B18" s="74" t="s">
+        <v>464</v>
+      </c>
+      <c r="C18" s="53"/>
+      <c r="D18" s="54"/>
+      <c r="F18" s="53"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="52">
+        <v>1</v>
+      </c>
+      <c r="B19" s="62" t="s">
+        <v>433</v>
+      </c>
+      <c r="C19" s="55" t="s">
+        <v>442</v>
+      </c>
+      <c r="D19" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" s="54" t="s">
+        <v>447</v>
+      </c>
+      <c r="G19" s="54" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="52">
+        <v>2</v>
+      </c>
+      <c r="B20" s="62" t="s">
+        <v>434</v>
+      </c>
+      <c r="C20" s="56" t="s">
+        <v>443</v>
+      </c>
+      <c r="D20" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="54" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="52">
+        <v>3</v>
+      </c>
+      <c r="B21" s="62" t="s">
+        <v>435</v>
+      </c>
+      <c r="C21" s="55" t="s">
+        <v>444</v>
+      </c>
+      <c r="D21" s="55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="52">
+        <v>4</v>
+      </c>
+      <c r="B22" s="62" t="s">
+        <v>436</v>
+      </c>
+      <c r="C22" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D22" s="55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="52">
+        <v>5</v>
+      </c>
+      <c r="B23" s="62" t="s">
+        <v>437</v>
+      </c>
+      <c r="C23" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D23" s="55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="52">
+        <v>6</v>
+      </c>
+      <c r="B24" s="62" t="s">
+        <v>439</v>
+      </c>
+      <c r="C24" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D24" s="55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="66" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="52">
+        <v>7</v>
+      </c>
+      <c r="B25" s="73" t="s">
+        <v>438</v>
+      </c>
+      <c r="C25" s="64" t="s">
+        <v>476</v>
+      </c>
+      <c r="D25" s="59" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" s="59" t="s">
+        <v>482</v>
+      </c>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="69"/>
+      <c r="J25" s="70"/>
+    </row>
+    <row r="26" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="52">
+        <v>0</v>
+      </c>
+      <c r="B26" s="74" t="s">
+        <v>465</v>
+      </c>
+      <c r="C26" s="53"/>
+      <c r="D26" s="54"/>
+      <c r="F26" s="53"/>
+    </row>
+    <row r="27" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="52">
+        <v>1</v>
+      </c>
+      <c r="B27" s="62" t="s">
+        <v>433</v>
+      </c>
+      <c r="C27" s="55" t="s">
+        <v>442</v>
+      </c>
+      <c r="D27" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F27" s="54" t="s">
+        <v>447</v>
+      </c>
+      <c r="G27" s="54" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="52">
+        <v>2</v>
+      </c>
+      <c r="B28" s="62" t="s">
+        <v>434</v>
+      </c>
+      <c r="C28" s="55" t="s">
+        <v>443</v>
+      </c>
+      <c r="D28" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" s="54" t="s">
+        <v>466</v>
+      </c>
+      <c r="F28" s="54" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="52">
+        <v>3</v>
+      </c>
+      <c r="B29" s="62" t="s">
+        <v>435</v>
+      </c>
+      <c r="C29" s="55" t="s">
+        <v>444</v>
+      </c>
+      <c r="D29" s="55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="52">
+        <v>4</v>
+      </c>
+      <c r="B30" s="62" t="s">
+        <v>436</v>
+      </c>
+      <c r="C30" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D30" s="55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="52">
+        <v>5</v>
+      </c>
+      <c r="B31" s="62" t="s">
+        <v>437</v>
+      </c>
+      <c r="C31" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D31" s="55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="52">
+        <v>6</v>
+      </c>
+      <c r="B32" s="62" t="s">
+        <v>439</v>
+      </c>
+      <c r="C32" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D32" s="55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="66" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="52">
+        <v>7</v>
+      </c>
+      <c r="B33" s="73" t="s">
+        <v>438</v>
+      </c>
+      <c r="C33" s="58" t="s">
+        <v>476</v>
+      </c>
+      <c r="D33" s="58" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="69"/>
+      <c r="J33" s="70"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="52">
+        <v>0</v>
+      </c>
+      <c r="B34" s="74" t="s">
+        <v>470</v>
+      </c>
+      <c r="C34" s="53"/>
+      <c r="D34" s="54"/>
+      <c r="F34" s="53"/>
+    </row>
+    <row r="35" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="52">
+        <v>1</v>
+      </c>
+      <c r="B35" s="62" t="s">
+        <v>433</v>
+      </c>
+      <c r="C35" s="55" t="s">
+        <v>442</v>
+      </c>
+      <c r="D35" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F35" s="54" t="s">
+        <v>447</v>
+      </c>
+      <c r="G35" s="54" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="52">
+        <v>2</v>
+      </c>
+      <c r="B36" s="62" t="s">
+        <v>434</v>
+      </c>
+      <c r="C36" s="56" t="s">
+        <v>443</v>
+      </c>
+      <c r="D36" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="E36" s="54" t="s">
+        <v>468</v>
+      </c>
+      <c r="F36" s="54" t="s">
+        <v>471</v>
+      </c>
+      <c r="G36" s="54" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="52">
+        <v>3</v>
+      </c>
+      <c r="B37" s="62" t="s">
+        <v>435</v>
+      </c>
+      <c r="C37" s="55" t="s">
+        <v>444</v>
+      </c>
+      <c r="D37" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="54" t="s">
+        <v>472</v>
+      </c>
+      <c r="G37" s="54" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="52">
+        <v>4</v>
+      </c>
+      <c r="B38" s="62" t="s">
+        <v>436</v>
+      </c>
+      <c r="C38" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D38" s="55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="52">
+        <v>5</v>
+      </c>
+      <c r="B39" s="62" t="s">
+        <v>437</v>
+      </c>
+      <c r="C39" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D39" s="55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="52">
+        <v>6</v>
+      </c>
+      <c r="B40" s="62" t="s">
+        <v>439</v>
+      </c>
+      <c r="C40" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D40" s="55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" s="66" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="52">
+        <v>7</v>
+      </c>
+      <c r="B41" s="73" t="s">
+        <v>438</v>
+      </c>
+      <c r="C41" s="64" t="s">
+        <v>476</v>
+      </c>
+      <c r="D41" s="59" t="b">
+        <v>1</v>
+      </c>
+      <c r="E41" s="59" t="s">
+        <v>482</v>
+      </c>
+      <c r="F41" s="59"/>
+      <c r="G41" s="59"/>
+      <c r="H41" s="69"/>
+      <c r="J41" s="70"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="52">
+        <v>0</v>
+      </c>
+      <c r="B42" s="74" t="s">
+        <v>474</v>
+      </c>
+      <c r="C42" s="53"/>
+      <c r="D42" s="54"/>
+      <c r="F42" s="53"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="52">
+        <v>1</v>
+      </c>
+      <c r="B43" s="62" t="s">
+        <v>433</v>
+      </c>
+      <c r="C43" s="55" t="s">
+        <v>442</v>
+      </c>
+      <c r="D43" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F43" s="54" t="s">
+        <v>447</v>
+      </c>
+      <c r="G43" s="54" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="52">
+        <v>2</v>
+      </c>
+      <c r="B44" s="62" t="s">
+        <v>434</v>
+      </c>
+      <c r="C44" s="56" t="s">
+        <v>443</v>
+      </c>
+      <c r="D44" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="E44" s="54" t="s">
+        <v>468</v>
+      </c>
+      <c r="F44" s="54" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="52">
+        <v>3</v>
+      </c>
+      <c r="B45" s="62" t="s">
+        <v>435</v>
+      </c>
+      <c r="C45" s="56" t="s">
+        <v>444</v>
+      </c>
+      <c r="D45" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="E45" s="54" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="52">
+        <v>4</v>
+      </c>
+      <c r="B46" s="62" t="s">
+        <v>436</v>
+      </c>
+      <c r="C46" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D46" s="55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="52">
+        <v>5</v>
+      </c>
+      <c r="B47" s="62" t="s">
+        <v>437</v>
+      </c>
+      <c r="C47" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D47" s="55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="52">
+        <v>6</v>
+      </c>
+      <c r="B48" s="62" t="s">
+        <v>439</v>
+      </c>
+      <c r="C48" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D48" s="55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="66" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="52">
+        <v>7</v>
+      </c>
+      <c r="B49" s="73" t="s">
+        <v>438</v>
+      </c>
+      <c r="C49" s="64" t="s">
+        <v>476</v>
+      </c>
+      <c r="D49" s="59" t="b">
+        <v>1</v>
+      </c>
+      <c r="E49" s="59" t="s">
+        <v>482</v>
+      </c>
+      <c r="F49" s="59"/>
+      <c r="G49" s="59"/>
+      <c r="H49" s="69"/>
+      <c r="J49" s="70"/>
+    </row>
+    <row r="50" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="52">
+        <v>0</v>
+      </c>
+      <c r="B50" s="74" t="s">
+        <v>475</v>
+      </c>
+      <c r="C50" s="53"/>
+      <c r="D50" s="54"/>
+      <c r="F50" s="53"/>
+    </row>
+    <row r="51" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="52">
+        <v>1</v>
+      </c>
+      <c r="B51" s="62" t="s">
+        <v>433</v>
+      </c>
+      <c r="C51" s="55" t="s">
+        <v>442</v>
+      </c>
+      <c r="D51" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F51" s="54" t="s">
+        <v>447</v>
+      </c>
+      <c r="G51" s="54" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="52">
+        <v>2</v>
+      </c>
+      <c r="B52" s="62" t="s">
+        <v>434</v>
+      </c>
+      <c r="C52" s="55" t="s">
+        <v>443</v>
+      </c>
+      <c r="D52" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="E52" s="54" t="s">
+        <v>468</v>
+      </c>
+      <c r="F52" s="54" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="52">
+        <v>3</v>
+      </c>
+      <c r="B53" s="62" t="s">
+        <v>435</v>
+      </c>
+      <c r="C53" s="56" t="s">
+        <v>476</v>
+      </c>
+      <c r="D53" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="E53" s="54" t="s">
+        <v>477</v>
+      </c>
+      <c r="F53" s="54" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="52">
+        <v>4</v>
+      </c>
+      <c r="B54" s="62" t="s">
+        <v>436</v>
+      </c>
+      <c r="C54" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D54" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F54" s="54" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="52">
+        <v>5</v>
+      </c>
+      <c r="B55" s="62" t="s">
+        <v>437</v>
+      </c>
+      <c r="C55" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D55" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F55" s="54" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="52">
+        <v>6</v>
+      </c>
+      <c r="B56" s="62" t="s">
+        <v>439</v>
+      </c>
+      <c r="C56" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D56" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F56" s="54" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" s="66" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="52">
+        <v>7</v>
+      </c>
+      <c r="B57" s="73" t="s">
+        <v>438</v>
+      </c>
+      <c r="C57" s="58" t="s">
+        <v>476</v>
+      </c>
+      <c r="D57" s="58" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="59"/>
+      <c r="F57" s="59"/>
+      <c r="G57" s="59"/>
+      <c r="H57" s="69"/>
+      <c r="J57" s="70"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="52">
+        <v>0</v>
+      </c>
+      <c r="B58" s="74" t="s">
+        <v>481</v>
+      </c>
+      <c r="C58" s="53"/>
+      <c r="D58" s="54"/>
+      <c r="F58" s="53"/>
+    </row>
+    <row r="59" spans="1:10" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="52">
+        <v>1</v>
+      </c>
+      <c r="B59" s="62" t="s">
+        <v>433</v>
+      </c>
+      <c r="C59" s="56" t="s">
+        <v>519</v>
+      </c>
+      <c r="D59" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="E59" s="54" t="s">
+        <v>507</v>
+      </c>
+      <c r="F59" s="54" t="s">
+        <v>447</v>
+      </c>
+      <c r="G59" s="54" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="52">
+        <v>2</v>
+      </c>
+      <c r="B60" s="62" t="s">
+        <v>434</v>
+      </c>
+      <c r="C60" s="55"/>
+      <c r="D60" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="54" t="s">
+        <v>468</v>
+      </c>
+      <c r="F60" s="54" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="52">
+        <v>3</v>
+      </c>
+      <c r="B61" s="62" t="s">
+        <v>435</v>
+      </c>
+      <c r="C61" s="55"/>
+      <c r="D61" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F61" s="54" t="s">
+        <v>468</v>
+      </c>
+      <c r="G61" s="54" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="52">
+        <v>4</v>
+      </c>
+      <c r="B62" s="62" t="s">
+        <v>436</v>
+      </c>
+      <c r="C62" s="56" t="s">
+        <v>445</v>
+      </c>
+      <c r="D62" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="E62" s="54" t="s">
+        <v>497</v>
+      </c>
+      <c r="F62" s="54" t="s">
+        <v>489</v>
+      </c>
+      <c r="G62" s="54" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="52">
+        <v>5</v>
+      </c>
+      <c r="B63" s="62" t="s">
+        <v>437</v>
+      </c>
+      <c r="C63" s="56" t="s">
+        <v>445</v>
+      </c>
+      <c r="D63" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="E63" s="54" t="s">
+        <v>498</v>
+      </c>
+      <c r="F63" s="54" t="s">
+        <v>490</v>
+      </c>
+      <c r="G63" s="54" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="52">
+        <v>6</v>
+      </c>
+      <c r="B64" s="62" t="s">
+        <v>439</v>
+      </c>
+      <c r="C64" s="56" t="s">
+        <v>445</v>
+      </c>
+      <c r="D64" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="E64" s="54" t="s">
+        <v>499</v>
+      </c>
+      <c r="F64" s="54" t="s">
+        <v>487</v>
+      </c>
+      <c r="G64" s="54" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" s="66" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="52">
+        <v>7</v>
+      </c>
+      <c r="B65" s="73" t="s">
+        <v>438</v>
+      </c>
+      <c r="C65" s="64" t="s">
+        <v>485</v>
+      </c>
+      <c r="D65" s="59" t="b">
+        <v>1</v>
+      </c>
+      <c r="E65" s="59" t="s">
+        <v>486</v>
+      </c>
+      <c r="F65" s="59"/>
+      <c r="G65" s="59"/>
+      <c r="H65" s="69"/>
+      <c r="J65" s="70"/>
+    </row>
+    <row r="66" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="52">
+        <v>0</v>
+      </c>
+      <c r="B66" s="75" t="s">
+        <v>508</v>
+      </c>
+      <c r="C66" s="53"/>
+      <c r="D66" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" s="53"/>
+    </row>
+    <row r="67" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="52">
+        <v>1</v>
+      </c>
+      <c r="B67" s="62" t="s">
+        <v>433</v>
+      </c>
+      <c r="C67" s="56" t="s">
+        <v>519</v>
+      </c>
+      <c r="D67" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" s="54" t="s">
+        <v>447</v>
+      </c>
+      <c r="G67" s="54" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="52">
+        <v>2</v>
+      </c>
+      <c r="B68" s="62" t="s">
+        <v>434</v>
+      </c>
+      <c r="C68" s="55"/>
+      <c r="D68" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F68" s="54" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="52">
+        <v>3</v>
+      </c>
+      <c r="B69" s="62" t="s">
+        <v>435</v>
+      </c>
+      <c r="C69" s="55"/>
+      <c r="D69" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F69" s="54" t="s">
+        <v>468</v>
+      </c>
+      <c r="G69" s="54" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="52">
+        <v>4</v>
+      </c>
+      <c r="B70" s="62" t="s">
+        <v>436</v>
+      </c>
+      <c r="C70" s="56" t="s">
+        <v>494</v>
+      </c>
+      <c r="D70" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="E70" s="54" t="s">
+        <v>496</v>
+      </c>
+      <c r="F70" s="54" t="s">
+        <v>489</v>
+      </c>
+      <c r="G70" s="54" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="52">
+        <v>5</v>
+      </c>
+      <c r="B71" s="62" t="s">
+        <v>437</v>
+      </c>
+      <c r="C71" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D71" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" s="54" t="s">
+        <v>509</v>
+      </c>
+      <c r="F71" s="54" t="s">
+        <v>490</v>
+      </c>
+      <c r="G71" s="54" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="52">
+        <v>6</v>
+      </c>
+      <c r="B72" s="62" t="s">
+        <v>439</v>
+      </c>
+      <c r="C72" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D72" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" s="54" t="s">
+        <v>509</v>
+      </c>
+      <c r="F72" s="54" t="s">
+        <v>487</v>
+      </c>
+      <c r="G72" s="54" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" s="66" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="52">
+        <v>7</v>
+      </c>
+      <c r="B73" s="73" t="s">
+        <v>438</v>
+      </c>
+      <c r="C73" s="64" t="s">
+        <v>485</v>
+      </c>
+      <c r="D73" s="59" t="b">
+        <v>1</v>
+      </c>
+      <c r="E73" s="59" t="s">
+        <v>486</v>
+      </c>
+      <c r="F73" s="59"/>
+      <c r="G73" s="59"/>
+      <c r="H73" s="69"/>
+      <c r="J73" s="70"/>
+    </row>
+    <row r="74" spans="1:10" s="54" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="52">
+        <v>0</v>
+      </c>
+      <c r="B74" s="75" t="s">
+        <v>510</v>
+      </c>
+      <c r="C74" s="53"/>
+      <c r="F74" s="53"/>
+      <c r="H74" s="61"/>
+    </row>
+    <row r="75" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="52">
+        <v>1</v>
+      </c>
+      <c r="B75" s="62" t="s">
+        <v>433</v>
+      </c>
+      <c r="C75" s="56" t="s">
+        <v>519</v>
+      </c>
+      <c r="D75" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="F75" s="54" t="s">
+        <v>447</v>
+      </c>
+      <c r="G75" s="54" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="52">
+        <v>2</v>
+      </c>
+      <c r="B76" s="62" t="s">
+        <v>434</v>
+      </c>
+      <c r="C76" s="55"/>
+      <c r="D76" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F76" s="54" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="52">
+        <v>3</v>
+      </c>
+      <c r="B77" s="62" t="s">
+        <v>435</v>
+      </c>
+      <c r="C77" s="55"/>
+      <c r="D77" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F77" s="54" t="s">
+        <v>468</v>
+      </c>
+      <c r="G77" s="54" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="52">
+        <v>4</v>
+      </c>
+      <c r="B78" s="62" t="s">
+        <v>436</v>
+      </c>
+      <c r="C78" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D78" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="E78" s="54" t="s">
+        <v>495</v>
+      </c>
+      <c r="F78" s="54" t="s">
+        <v>489</v>
+      </c>
+      <c r="G78" s="54" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="52">
+        <v>5</v>
+      </c>
+      <c r="B79" s="62" t="s">
+        <v>437</v>
+      </c>
+      <c r="C79" s="56" t="s">
+        <v>494</v>
+      </c>
+      <c r="D79" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="E79" s="54" t="s">
+        <v>496</v>
+      </c>
+      <c r="F79" s="54" t="s">
+        <v>490</v>
+      </c>
+      <c r="G79" s="54" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="52">
+        <v>6</v>
+      </c>
+      <c r="B80" s="62" t="s">
+        <v>439</v>
+      </c>
+      <c r="C80" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D80" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="E80" s="54" t="s">
+        <v>495</v>
+      </c>
+      <c r="F80" s="54" t="s">
+        <v>487</v>
+      </c>
+      <c r="G80" s="54" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" s="66" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="52">
+        <v>7</v>
+      </c>
+      <c r="B81" s="73" t="s">
+        <v>438</v>
+      </c>
+      <c r="C81" s="64" t="s">
+        <v>485</v>
+      </c>
+      <c r="D81" s="59" t="b">
+        <v>1</v>
+      </c>
+      <c r="E81" s="59" t="s">
+        <v>486</v>
+      </c>
+      <c r="F81" s="59"/>
+      <c r="G81" s="59"/>
+      <c r="H81" s="69"/>
+      <c r="J81" s="70"/>
+    </row>
+    <row r="82" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="52">
+        <v>0</v>
+      </c>
+      <c r="B82" s="75" t="s">
+        <v>511</v>
+      </c>
+      <c r="C82" s="53"/>
+      <c r="D82" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82" s="53"/>
+    </row>
+    <row r="83" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="52">
+        <v>1</v>
+      </c>
+      <c r="B83" s="62" t="s">
+        <v>433</v>
+      </c>
+      <c r="C83" s="56" t="s">
+        <v>519</v>
+      </c>
+      <c r="D83" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="F83" s="54" t="s">
+        <v>447</v>
+      </c>
+      <c r="G83" s="54" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="52">
+        <v>2</v>
+      </c>
+      <c r="B84" s="62" t="s">
+        <v>434</v>
+      </c>
+      <c r="C84" s="55"/>
+      <c r="D84" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F84" s="54" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="52">
+        <v>3</v>
+      </c>
+      <c r="B85" s="62" t="s">
+        <v>435</v>
+      </c>
+      <c r="C85" s="55"/>
+      <c r="D85" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F85" s="54" t="s">
+        <v>468</v>
+      </c>
+      <c r="G85" s="54" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="52">
+        <v>4</v>
+      </c>
+      <c r="B86" s="62" t="s">
+        <v>436</v>
+      </c>
+      <c r="C86" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D86" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="E86" s="54" t="s">
+        <v>512</v>
+      </c>
+      <c r="F86" s="54" t="s">
+        <v>489</v>
+      </c>
+      <c r="G86" s="54" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="52">
+        <v>5</v>
+      </c>
+      <c r="B87" s="62" t="s">
+        <v>437</v>
+      </c>
+      <c r="C87" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D87" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" s="54" t="s">
+        <v>512</v>
+      </c>
+      <c r="F87" s="54" t="s">
+        <v>490</v>
+      </c>
+      <c r="G87" s="54" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="52">
+        <v>6</v>
+      </c>
+      <c r="B88" s="62" t="s">
+        <v>439</v>
+      </c>
+      <c r="C88" s="56" t="s">
+        <v>494</v>
+      </c>
+      <c r="D88" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="E88" s="54" t="s">
+        <v>496</v>
+      </c>
+      <c r="F88" s="54" t="s">
+        <v>487</v>
+      </c>
+      <c r="G88" s="54" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" s="66" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="52">
+        <v>7</v>
+      </c>
+      <c r="B89" s="73" t="s">
+        <v>438</v>
+      </c>
+      <c r="C89" s="64" t="s">
+        <v>485</v>
+      </c>
+      <c r="D89" s="59" t="b">
+        <v>1</v>
+      </c>
+      <c r="E89" s="59" t="s">
+        <v>486</v>
+      </c>
+      <c r="F89" s="59"/>
+      <c r="G89" s="59"/>
+      <c r="H89" s="69"/>
+      <c r="J89" s="70"/>
+    </row>
+    <row r="90" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="52">
+        <v>0</v>
+      </c>
+      <c r="B90" s="75" t="s">
+        <v>513</v>
+      </c>
+      <c r="C90" s="53"/>
+      <c r="D90" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" s="53"/>
+    </row>
+    <row r="91" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="52">
+        <v>1</v>
+      </c>
+      <c r="B91" s="62" t="s">
+        <v>433</v>
+      </c>
+      <c r="C91" s="57"/>
+      <c r="D91" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F91" s="54" t="s">
+        <v>447</v>
+      </c>
+      <c r="G91" s="54" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="52">
+        <v>2</v>
+      </c>
+      <c r="B92" s="62" t="s">
+        <v>434</v>
+      </c>
+      <c r="C92" s="55"/>
+      <c r="D92" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F92" s="54" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="52">
+        <v>3</v>
+      </c>
+      <c r="B93" s="62" t="s">
+        <v>435</v>
+      </c>
+      <c r="C93" s="55"/>
+      <c r="D93" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F93" s="54" t="s">
+        <v>468</v>
+      </c>
+      <c r="G93" s="54" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="52">
+        <v>4</v>
+      </c>
+      <c r="B94" s="62" t="s">
+        <v>436</v>
+      </c>
+      <c r="C94" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D94" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F94" s="54" t="s">
+        <v>488</v>
+      </c>
+      <c r="G94" s="54" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="52">
+        <v>5</v>
+      </c>
+      <c r="B95" s="62" t="s">
+        <v>437</v>
+      </c>
+      <c r="C95" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D95" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F95" s="54" t="s">
+        <v>490</v>
+      </c>
+      <c r="G95" s="54" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="52">
+        <v>6</v>
+      </c>
+      <c r="B96" s="62" t="s">
+        <v>439</v>
+      </c>
+      <c r="C96" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="D96" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F96" s="54" t="s">
+        <v>502</v>
+      </c>
+      <c r="G96" s="54" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" s="66" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="52">
+        <v>7</v>
+      </c>
+      <c r="B97" s="73" t="s">
+        <v>438</v>
+      </c>
+      <c r="C97" s="64" t="s">
+        <v>476</v>
+      </c>
+      <c r="D97" s="59" t="b">
+        <v>1</v>
+      </c>
+      <c r="E97" s="59" t="s">
+        <v>505</v>
+      </c>
+      <c r="F97" s="59" t="s">
+        <v>506</v>
+      </c>
+      <c r="G97" s="59"/>
+      <c r="H97" s="69"/>
+      <c r="J97" s="70"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D98" s="54"/>
+    </row>
+    <row r="99" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D99" s="54"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D100" s="54"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D101" s="54"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C107" s="52"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C108" s="52"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C109" s="52"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C110" s="52"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C111" s="52"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C112" s="52"/>
+    </row>
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C113" s="52"/>
+    </row>
+    <row r="117" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B117" s="72"/>
+      <c r="C117" s="51"/>
+      <c r="D117" s="51"/>
+      <c r="E117" s="51"/>
+      <c r="F117" s="51"/>
+      <c r="G117" s="51"/>
+      <c r="H117" s="65"/>
+    </row>
+    <row r="118" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B118" s="72"/>
+      <c r="C118" s="51"/>
+      <c r="D118" s="51"/>
+      <c r="E118" s="51"/>
+      <c r="F118" s="51"/>
+      <c r="G118" s="51"/>
+      <c r="H118" s="65"/>
+    </row>
+    <row r="119" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B119" s="72"/>
+      <c r="C119" s="51"/>
+      <c r="D119" s="51"/>
+      <c r="E119" s="51"/>
+      <c r="F119" s="51"/>
+      <c r="G119" s="51"/>
+      <c r="H119" s="65"/>
+    </row>
+    <row r="120" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B120" s="72"/>
+      <c r="C120" s="51"/>
+      <c r="D120" s="51"/>
+      <c r="E120" s="51"/>
+      <c r="F120" s="51"/>
+      <c r="G120" s="51"/>
+      <c r="H120" s="65"/>
+    </row>
+    <row r="121" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B121" s="72"/>
+      <c r="C121" s="51"/>
+      <c r="D121" s="51"/>
+      <c r="E121" s="51"/>
+      <c r="F121" s="51"/>
+      <c r="G121" s="51"/>
+      <c r="H121" s="65"/>
+    </row>
+    <row r="122" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B122" s="72"/>
+      <c r="C122" s="51"/>
+      <c r="D122" s="51"/>
+      <c r="E122" s="51"/>
+      <c r="F122" s="51"/>
+      <c r="G122" s="51"/>
+      <c r="H122" s="65"/>
+    </row>
+    <row r="123" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B123" s="72"/>
+      <c r="C123" s="51"/>
+      <c r="D123" s="51"/>
+      <c r="E123" s="51"/>
+      <c r="F123" s="51"/>
+      <c r="G123" s="51"/>
+      <c r="H123" s="65"/>
+    </row>
+  </sheetData>
+  <sortState ref="A2:L94">
+    <sortCondition ref="A2:A94"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- More MatchFlowables fixes. - Updated webinars...xlsx file with "ToDo" list
</commit_message>
<xml_diff>
--- a/HarmonizationTool/notes/webinars_plus_issues_prior_to_2015-08-01.xlsx
+++ b/HarmonizationTool/notes/webinars_plus_issues_prior_to_2015-08-01.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="523">
   <si>
     <t>URLs</t>
   </si>
@@ -1708,9 +1708,6 @@
   </si>
   <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>Partial</t>
   </si>
 </sst>
 </file>
@@ -1790,7 +1787,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1842,12 +1839,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2026,7 +2017,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -2238,9 +2229,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4561,9 +4549,9 @@
   <dimension ref="A1:AML71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I69" sqref="I69"/>
+      <selection pane="bottomLeft" activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4721,6 +4709,9 @@
       <c r="G6" s="46">
         <v>2</v>
       </c>
+      <c r="H6" s="42" t="s">
+        <v>392</v>
+      </c>
       <c r="I6" s="85" t="s">
         <v>407</v>
       </c>
@@ -5148,6 +5139,9 @@
       </c>
       <c r="E26" s="4" t="s">
         <v>276</v>
+      </c>
+      <c r="H26" s="42" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -6592,8 +6586,8 @@
       <c r="G46" s="46">
         <v>2</v>
       </c>
-      <c r="H46" s="86" t="s">
-        <v>523</v>
+      <c r="H46" s="42" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="47" spans="1:1026" x14ac:dyDescent="0.25">
@@ -6712,6 +6706,9 @@
       <c r="G51" s="46">
         <v>2</v>
       </c>
+      <c r="H51" s="42" t="s">
+        <v>392</v>
+      </c>
     </row>
     <row r="52" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="31" t="s">
@@ -6735,6 +6732,9 @@
       <c r="G52" s="46">
         <v>3</v>
       </c>
+      <c r="H52" s="42" t="s">
+        <v>392</v>
+      </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="31" t="s">
@@ -6758,6 +6758,9 @@
       <c r="G53" s="46">
         <v>1</v>
       </c>
+      <c r="H53" s="42" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="54" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="31" t="s">
@@ -6781,6 +6784,9 @@
       <c r="G54" s="46">
         <v>1</v>
       </c>
+      <c r="H54" s="42" t="s">
+        <v>392</v>
+      </c>
     </row>
     <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="31" t="s">
@@ -6798,6 +6804,9 @@
       <c r="E55" s="4" t="s">
         <v>245</v>
       </c>
+      <c r="H55" s="42" t="s">
+        <v>392</v>
+      </c>
     </row>
     <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="31" t="s">
@@ -6821,6 +6830,9 @@
       <c r="G56" s="46">
         <v>1</v>
       </c>
+      <c r="H56" s="42" t="s">
+        <v>392</v>
+      </c>
     </row>
     <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="31" t="s">
@@ -6844,8 +6856,8 @@
       <c r="G57" s="46">
         <v>2</v>
       </c>
-      <c r="H57" s="86" t="s">
-        <v>523</v>
+      <c r="H57" s="42" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -6870,8 +6882,8 @@
       <c r="G58" s="46">
         <v>2</v>
       </c>
-      <c r="H58" s="86" t="s">
-        <v>523</v>
+      <c r="H58" s="42" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -7050,6 +7062,9 @@
       </c>
       <c r="G66" s="46">
         <v>1</v>
+      </c>
+      <c r="H66" s="42" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Updated the webinars_plus_issues
</commit_message>
<xml_diff>
--- a/HarmonizationTool/notes/webinars_plus_issues_prior_to_2015-08-01.xlsx
+++ b/HarmonizationTool/notes/webinars_plus_issues_prior_to_2015-08-01.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="537">
   <si>
     <t>URLs</t>
   </si>
@@ -1042,9 +1042,6 @@
     <t>How are reference items in masterlists  flagged? Boldface and mouseover are simple. For the reference item, mousesover would say "Reference (Conversion factor = 1)." For all other items, mouseover gives conversion factor.</t>
   </si>
   <si>
-    <t>Properties, Contexts</t>
-  </si>
-  <si>
     <t>How are reference items in masterlists  flagged? Boldface and mouseover are simple. For the reference item, mousesover would say "Reference (Conversion factor = 1)" For all other items, mouseover gives conversion factor.</t>
   </si>
   <si>
@@ -1061,12 +1058,6 @@
   </si>
   <si>
     <t>CSV issue</t>
-  </si>
-  <si>
-    <t>Wes: if user has amount data with csv data, does that still get shown? Column to assign for amount? 
-Tom - i think so. CHECK THIS.
-Wes will take typical csv data, run it through, and make note of bugs
-Reviewed process of creating csv output</t>
   </si>
   <si>
     <t>58:50</t>
@@ -1701,13 +1692,64 @@
     <t>some in tooltips.  See the new Workflow states Worksheet in this Excel workbook.</t>
   </si>
   <si>
-    <t>some</t>
-  </si>
-  <si>
     <t>When User Data table is scrolled to the right, clicking not detected.  The mouse listener did not allow for a getItem.  Fixed now.</t>
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>started</t>
+  </si>
+  <si>
+    <t>Wes: if user has amount data with csv data, does that still get shown? Column to assign for amount =&gt; Flow Unit -&gt; Conversion Factor
+Users can assign values, and output is mapped in .csv output, but not zipped .json.
+Wes will take typical csv data, run it through, and make note of bugs
+Reviewed process of creating csv output</t>
+  </si>
+  <si>
+    <t>Not done</t>
+  </si>
+  <si>
+    <t>Contexts is quick because data are pre-loaded</t>
+  </si>
+  <si>
+    <t>Tom and Wes should discuss specific requirements</t>
+  </si>
+  <si>
+    <t>Document once Item 40 is done</t>
+  </si>
+  <si>
+    <t>Should be added to Step 5 in UG</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>Several looks at Logger output would be good</t>
+  </si>
+  <si>
+    <t>Requires a little thought, but not too much work</t>
+  </si>
+  <si>
+    <t>See 24, too.</t>
+  </si>
+  <si>
+    <t>Wes should review Appendices C and D</t>
+  </si>
+  <si>
+    <t>Not done yet, but easy</t>
+  </si>
+  <si>
+    <t>Added by Tom: 8-7</t>
+  </si>
+  <si>
+    <t>The FlowsWorkflow tab has many states.  The switching is easy to do, but must be reviewed to ensure that all switches are proper and all parts of the state are set right.</t>
+  </si>
+  <si>
+    <t>Tom and Tony</t>
+  </si>
+  <si>
+    <t>Just lots of cases to look at</t>
   </si>
 </sst>
 </file>
@@ -2017,7 +2059,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -2227,6 +2269,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2594,7 +2639,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C1" s="38" t="s">
         <v>15</v>
@@ -2607,10 +2652,10 @@
     </row>
     <row r="3" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="33" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2620,10 +2665,10 @@
     </row>
     <row r="5" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="33" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2633,10 +2678,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="33" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2646,10 +2691,10 @@
     </row>
     <row r="9" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="33" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2659,10 +2704,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
+        <v>384</v>
+      </c>
+      <c r="C11" s="37" t="s">
         <v>386</v>
-      </c>
-      <c r="C11" s="37" t="s">
-        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -4548,10 +4593,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I64" sqref="I64"/>
+      <selection pane="bottomLeft" activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4584,16 +4629,16 @@
         <v>243</v>
       </c>
       <c r="F1" s="47" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="G1" s="47" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>15</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4609,7 +4654,7 @@
         <v>245</v>
       </c>
       <c r="H2" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -4629,13 +4674,13 @@
         <v>248</v>
       </c>
       <c r="F3" s="46" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G3" s="46">
         <v>2</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4655,7 +4700,7 @@
         <v>250</v>
       </c>
       <c r="H4" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -4669,22 +4714,22 @@
         <v>252</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>248</v>
       </c>
       <c r="F5" s="46" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G5" s="46">
         <v>3</v>
       </c>
       <c r="H5" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -4704,16 +4749,16 @@
         <v>248</v>
       </c>
       <c r="F6" s="46" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G6" s="46">
         <v>2</v>
       </c>
       <c r="H6" s="42" t="s">
-        <v>392</v>
-      </c>
-      <c r="I6" s="85" t="s">
-        <v>407</v>
+        <v>390</v>
+      </c>
+      <c r="I6" s="86" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4731,15 +4776,15 @@
         <v>248</v>
       </c>
       <c r="F7" s="46" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G7" s="46">
         <v>3</v>
       </c>
       <c r="H7" s="42" t="s">
-        <v>392</v>
-      </c>
-      <c r="I7" s="85"/>
+        <v>390</v>
+      </c>
+      <c r="I7" s="86"/>
     </row>
     <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="31"/>
@@ -4756,9 +4801,9 @@
         <v>248</v>
       </c>
       <c r="H8" s="42" t="s">
-        <v>392</v>
-      </c>
-      <c r="I8" s="85"/>
+        <v>390</v>
+      </c>
+      <c r="I8" s="86"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
@@ -4775,15 +4820,15 @@
         <v>248</v>
       </c>
       <c r="F9" s="46" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G9" s="46">
         <v>3</v>
       </c>
       <c r="H9" s="42" t="s">
-        <v>392</v>
-      </c>
-      <c r="I9" s="85"/>
+        <v>390</v>
+      </c>
+      <c r="I9" s="86"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="31"/>
@@ -4800,7 +4845,7 @@
         <v>101</v>
       </c>
       <c r="H10" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4820,13 +4865,13 @@
         <v>248</v>
       </c>
       <c r="F11" s="46" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G11" s="46">
         <v>2</v>
       </c>
       <c r="H11" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -4844,7 +4889,7 @@
         <v>250</v>
       </c>
       <c r="H12" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -4864,16 +4909,16 @@
         <v>245</v>
       </c>
       <c r="F13" s="46" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G13" s="46">
         <v>1</v>
       </c>
       <c r="H13" s="42" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
         <v>266</v>
       </c>
@@ -4890,13 +4935,16 @@
         <v>245</v>
       </c>
       <c r="F14" s="46" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G14" s="46">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H14" s="85" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
         <v>269</v>
       </c>
@@ -4911,6 +4959,9 @@
       </c>
       <c r="E15" s="4" t="s">
         <v>101</v>
+      </c>
+      <c r="H15" s="85" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4930,13 +4981,13 @@
         <v>250</v>
       </c>
       <c r="F16" s="46" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G16" s="46">
         <v>1</v>
       </c>
       <c r="H16" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -4956,10 +5007,10 @@
         <v>276</v>
       </c>
       <c r="F17" s="46" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="H17" s="42" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -4979,10 +5030,10 @@
         <v>278</v>
       </c>
       <c r="F18" s="46" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -5002,13 +5053,13 @@
         <v>250</v>
       </c>
       <c r="F19" s="46" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G19" s="46">
         <v>3</v>
       </c>
       <c r="H19" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5028,13 +5079,13 @@
         <v>278</v>
       </c>
       <c r="F20" s="46" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G20" s="46">
         <v>2</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5052,7 +5103,7 @@
         <v>278</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5070,7 +5121,7 @@
         <v>276</v>
       </c>
       <c r="H22" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5089,6 +5140,15 @@
       <c r="E23" s="4" t="s">
         <v>245</v>
       </c>
+      <c r="F23" s="46" t="s">
+        <v>396</v>
+      </c>
+      <c r="G23" s="46">
+        <v>2</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>530</v>
+      </c>
     </row>
     <row r="24" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
@@ -5106,6 +5166,15 @@
       <c r="E24" s="4" t="s">
         <v>245</v>
       </c>
+      <c r="F24" s="46" t="s">
+        <v>396</v>
+      </c>
+      <c r="G24" s="46">
+        <v>3</v>
+      </c>
+      <c r="H24" s="85" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
@@ -5141,7 +5210,7 @@
         <v>276</v>
       </c>
       <c r="H26" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -5160,8 +5229,11 @@
       <c r="E27" s="4" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H27" s="46" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
         <v>301</v>
       </c>
@@ -5176,6 +5248,15 @@
       </c>
       <c r="E28" s="4" t="s">
         <v>245</v>
+      </c>
+      <c r="F28" s="46" t="s">
+        <v>396</v>
+      </c>
+      <c r="G28" s="46">
+        <v>2</v>
+      </c>
+      <c r="H28" s="85" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -5193,7 +5274,7 @@
         <v>276</v>
       </c>
       <c r="H29" s="42" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5207,19 +5288,19 @@
         <v>90</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>250</v>
       </c>
       <c r="F30" s="46" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G30" s="46">
         <v>3</v>
       </c>
       <c r="H30" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5238,6 +5319,12 @@
       <c r="E31" s="4" t="s">
         <v>245</v>
       </c>
+      <c r="F31" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
@@ -5255,6 +5342,12 @@
       <c r="E32" s="4" t="s">
         <v>250</v>
       </c>
+      <c r="F32" s="46" t="s">
+        <v>400</v>
+      </c>
+      <c r="G32" s="46">
+        <v>2</v>
+      </c>
     </row>
     <row r="33" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
@@ -5273,10 +5366,13 @@
         <v>250</v>
       </c>
       <c r="F33" s="46" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G33" s="46">
         <v>1</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="34" spans="1:1026" x14ac:dyDescent="0.25">
@@ -5296,7 +5392,7 @@
         <v>245</v>
       </c>
       <c r="H34" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="35" spans="1:1026" ht="30" x14ac:dyDescent="0.25">
@@ -5316,10 +5412,13 @@
         <v>245</v>
       </c>
       <c r="F35" s="46" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G35" s="46">
         <v>2</v>
+      </c>
+      <c r="H35" s="42" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="36" spans="1:1026" ht="75" x14ac:dyDescent="0.25">
@@ -5338,6 +5437,15 @@
       <c r="E36" s="4" t="s">
         <v>278</v>
       </c>
+      <c r="F36" s="46" t="s">
+        <v>396</v>
+      </c>
+      <c r="G36" s="46">
+        <v>1</v>
+      </c>
+      <c r="H36" s="85" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="37" spans="1:1026" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
@@ -5350,19 +5458,19 @@
         <v>90</v>
       </c>
       <c r="D37" s="32" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>245</v>
       </c>
       <c r="F37" s="46" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G37" s="46">
         <v>3</v>
       </c>
       <c r="H37" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="38" spans="1:1026" ht="30" x14ac:dyDescent="0.25">
@@ -5382,13 +5490,13 @@
         <v>250</v>
       </c>
       <c r="F38" s="46" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G38" s="46">
         <v>1</v>
       </c>
       <c r="H38" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="39" spans="1:1026" x14ac:dyDescent="0.25">
@@ -5408,7 +5516,7 @@
         <v>245</v>
       </c>
       <c r="H39" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="40" spans="1:1026" ht="60" x14ac:dyDescent="0.25">
@@ -5428,10 +5536,13 @@
         <v>245</v>
       </c>
       <c r="F40" s="46" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G40" s="46">
         <v>3</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="41" spans="1:1026" ht="60" x14ac:dyDescent="0.25">
@@ -5442,21 +5553,24 @@
         <v>98</v>
       </c>
       <c r="C41" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="D41" s="32" t="s">
         <v>328</v>
-      </c>
-      <c r="D41" s="32" t="s">
-        <v>329</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>278</v>
       </c>
       <c r="F41" s="46" t="s">
-        <v>402</v>
+        <v>400</v>
+      </c>
+      <c r="H41" s="85" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="42" spans="1:1026" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="34" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B42" s="44" t="s">
         <v>26</v>
@@ -5465,19 +5579,19 @@
         <v>148</v>
       </c>
       <c r="D42" s="45" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E42" s="44" t="s">
         <v>245</v>
       </c>
       <c r="F42" s="49" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G42" s="49">
         <v>5</v>
       </c>
       <c r="H42" s="43" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I42" s="35"/>
       <c r="J42" s="35"/>
@@ -6498,32 +6612,35 @@
       <c r="AMK42" s="35"/>
       <c r="AML42" s="35"/>
     </row>
-    <row r="43" spans="1:1026" ht="75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1026" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
+        <v>331</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="C43" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>334</v>
-      </c>
       <c r="D43" s="32" t="s">
-        <v>335</v>
+        <v>521</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>265</v>
       </c>
       <c r="F43" s="46" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G43" s="46">
         <v>3</v>
       </c>
+      <c r="H43" s="85" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="44" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>26</v>
@@ -6532,67 +6649,76 @@
         <v>289</v>
       </c>
       <c r="D44" s="32" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>245</v>
       </c>
       <c r="F44" s="46" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G44" s="46">
         <v>1</v>
       </c>
+      <c r="H44" s="42" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="45" spans="1:1026" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D45" s="32" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>278</v>
       </c>
       <c r="F45" s="46" t="s">
-        <v>398</v>
+        <v>394</v>
+      </c>
+      <c r="G45" s="46">
+        <v>1</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="46" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A46" s="31" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D46" s="32" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>245</v>
       </c>
       <c r="F46" s="46" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G46" s="46">
         <v>2</v>
       </c>
       <c r="H46" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="47" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A47" s="31" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>26</v>
@@ -6601,92 +6727,92 @@
         <v>148</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>245</v>
       </c>
       <c r="F47" s="46" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G47" s="46">
         <v>1</v>
       </c>
       <c r="H47" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="48" spans="1:1026" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="31" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C48"/>
       <c r="D48" s="32" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>245</v>
       </c>
       <c r="H48" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A49" s="31" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D49" s="32" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>245</v>
       </c>
       <c r="F49" s="46" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G49" s="46">
         <v>4</v>
       </c>
       <c r="H49" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="31" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C50"/>
       <c r="D50" s="32" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>248</v>
       </c>
       <c r="F50" s="46" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G50" s="46">
         <v>3</v>
       </c>
       <c r="H50" s="42" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="31" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>26</v>
@@ -6695,24 +6821,24 @@
         <v>70</v>
       </c>
       <c r="D51" s="32" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>245</v>
       </c>
       <c r="F51" s="46" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G51" s="46">
         <v>2</v>
       </c>
       <c r="H51" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="31" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>26</v>
@@ -6721,24 +6847,24 @@
         <v>70</v>
       </c>
       <c r="D52" s="32" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>250</v>
       </c>
       <c r="F52" s="46" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G52" s="46">
         <v>3</v>
       </c>
       <c r="H52" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="31" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>26</v>
@@ -6747,24 +6873,24 @@
         <v>70</v>
       </c>
       <c r="D53" s="32" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>245</v>
       </c>
       <c r="F53" s="46" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G53" s="46">
         <v>1</v>
       </c>
       <c r="H53" s="42" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="31" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>26</v>
@@ -6773,24 +6899,24 @@
         <v>70</v>
       </c>
       <c r="D54" s="32" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>245</v>
       </c>
       <c r="F54" s="46" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G54" s="46">
         <v>1</v>
       </c>
       <c r="H54" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="31" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>98</v>
@@ -6799,18 +6925,18 @@
         <v>70</v>
       </c>
       <c r="D55" s="32" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>245</v>
       </c>
       <c r="H55" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="31" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>26</v>
@@ -6819,24 +6945,24 @@
         <v>70</v>
       </c>
       <c r="D56" s="32" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>245</v>
       </c>
       <c r="F56" s="46" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G56" s="46">
         <v>1</v>
       </c>
       <c r="H56" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="31" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>26</v>
@@ -6845,24 +6971,24 @@
         <v>70</v>
       </c>
       <c r="D57" s="32" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>245</v>
       </c>
       <c r="F57" s="46" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G57" s="46">
         <v>2</v>
       </c>
       <c r="H57" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="31" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>26</v>
@@ -6871,24 +6997,24 @@
         <v>70</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>250</v>
       </c>
       <c r="F58" s="46" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G58" s="46">
         <v>2</v>
       </c>
       <c r="H58" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="31" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>103</v>
@@ -6897,87 +7023,90 @@
         <v>70</v>
       </c>
       <c r="D59" s="32" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>245</v>
       </c>
       <c r="F59" s="46" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G59" s="46">
         <v>3</v>
       </c>
+      <c r="H59" s="42" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="31" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D60" s="32" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>250</v>
       </c>
       <c r="F60" s="46" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G60" s="46">
         <v>3</v>
       </c>
       <c r="H60" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="31" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>103</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D61" s="32" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>248</v>
       </c>
       <c r="H61" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="31" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D62" s="32" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>248</v>
       </c>
       <c r="H62" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="31" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>17</v>
@@ -6986,18 +7115,18 @@
         <v>64</v>
       </c>
       <c r="D63" s="32" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="H63" s="4" t="s">
-        <v>520</v>
+      <c r="H63" s="42" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="31" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>17</v>
@@ -7006,18 +7135,18 @@
         <v>64</v>
       </c>
       <c r="D64" s="32" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="H64" s="4" t="s">
-        <v>333</v>
+      <c r="H64" s="42" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>17</v>
@@ -7026,24 +7155,24 @@
         <v>191</v>
       </c>
       <c r="D65" s="48" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F65" s="46" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G65" s="46">
         <v>1</v>
       </c>
       <c r="H65" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>17</v>
@@ -7052,24 +7181,24 @@
         <v>191</v>
       </c>
       <c r="D66" s="48" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F66" s="46" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G66" s="46">
         <v>1</v>
       </c>
       <c r="H66" s="42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>26</v>
@@ -7078,70 +7207,102 @@
         <v>26</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>245</v>
       </c>
       <c r="F67" s="46" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G67" s="46">
         <v>2</v>
       </c>
       <c r="H67" s="42" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>245</v>
       </c>
       <c r="F68" s="46" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G68" s="46">
         <v>3</v>
       </c>
+      <c r="H68" s="85" t="s">
+        <v>523</v>
+      </c>
     </row>
     <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="B69" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="B69" s="4" t="s">
-        <v>420</v>
-      </c>
       <c r="C69" s="4" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>245</v>
       </c>
       <c r="F69" s="46" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G69" s="46">
         <v>1</v>
       </c>
+      <c r="H69" s="42" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A70" s="85" t="s">
+        <v>533</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D70" s="85" t="s">
+        <v>534</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="F70" s="46" t="s">
+        <v>400</v>
+      </c>
+      <c r="G70" s="46">
+        <v>2</v>
+      </c>
+      <c r="H70" s="85" t="s">
+        <v>536</v>
+      </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D71" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
   </sheetData>
@@ -7174,46 +7335,46 @@
         <v>11</v>
       </c>
       <c r="B1" s="38" t="s">
+        <v>419</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>420</v>
+      </c>
+      <c r="D1" s="50" t="s">
         <v>421</v>
-      </c>
-      <c r="C1" s="50" t="s">
-        <v>422</v>
-      </c>
-      <c r="D1" s="50" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
+        <v>422</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>423</v>
+      </c>
+      <c r="C2" t="s">
         <v>424</v>
-      </c>
-      <c r="B2" s="37" t="s">
-        <v>425</v>
-      </c>
-      <c r="C2" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C3" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
+        <v>427</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>428</v>
+      </c>
+      <c r="C4" t="s">
         <v>429</v>
-      </c>
-      <c r="B4" s="37" t="s">
-        <v>430</v>
-      </c>
-      <c r="C4" t="s">
-        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -7246,34 +7407,34 @@
   <sheetData>
     <row r="1" spans="1:10" s="66" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="66" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B1" s="71" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C1" s="68" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D1" s="68" t="s">
+        <v>512</v>
+      </c>
+      <c r="E1" s="68" t="s">
+        <v>446</v>
+      </c>
+      <c r="F1" s="68" t="s">
+        <v>511</v>
+      </c>
+      <c r="G1" s="68" t="s">
+        <v>447</v>
+      </c>
+      <c r="H1" s="67" t="s">
+        <v>480</v>
+      </c>
+      <c r="I1" s="76" t="s">
         <v>514</v>
       </c>
-      <c r="E1" s="68" t="s">
-        <v>448</v>
-      </c>
-      <c r="F1" s="68" t="s">
+      <c r="J1" s="77" t="s">
         <v>513</v>
-      </c>
-      <c r="G1" s="68" t="s">
-        <v>449</v>
-      </c>
-      <c r="H1" s="67" t="s">
-        <v>482</v>
-      </c>
-      <c r="I1" s="76" t="s">
-        <v>516</v>
-      </c>
-      <c r="J1" s="77" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -7281,7 +7442,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="74" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C2" s="53"/>
       <c r="F2" s="53"/>
@@ -7293,22 +7454,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="62" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C3" s="54" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D3" s="54" t="b">
         <v>1</v>
       </c>
       <c r="E3" s="54" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="I3" s="80" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="J3" s="81" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7316,19 +7477,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="62" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C4" s="55" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D4" s="55" t="b">
         <v>0</v>
       </c>
       <c r="I4" s="80" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="J4" s="81" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7336,19 +7497,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="62" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C5" s="55" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D5" s="55" t="b">
         <v>0</v>
       </c>
       <c r="I5" s="82" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="J5" s="81" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7356,19 +7517,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="62" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C6" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D6" s="55" t="b">
         <v>0</v>
       </c>
       <c r="I6" s="80" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="J6" s="81" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7376,19 +7537,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="62" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C7" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D7" s="55" t="b">
         <v>0</v>
       </c>
       <c r="I7" s="80" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="J7" s="81" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7396,19 +7557,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="62" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C8" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D8" s="55" t="b">
         <v>0</v>
       </c>
       <c r="I8" s="80" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="J8" s="81" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="66" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7416,7 +7577,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="73" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C9" s="58"/>
       <c r="D9" s="58" t="b">
@@ -7427,10 +7588,10 @@
       <c r="G9" s="59"/>
       <c r="H9" s="69"/>
       <c r="I9" s="83" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="J9" s="84" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -7438,13 +7599,13 @@
         <v>0</v>
       </c>
       <c r="B10" s="74" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C10" s="53"/>
       <c r="D10" s="54"/>
       <c r="F10" s="53"/>
       <c r="H10" s="60" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="J10" s="52"/>
     </row>
@@ -7453,19 +7614,19 @@
         <v>1</v>
       </c>
       <c r="B11" s="62" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C11" s="55" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D11" s="55" t="b">
         <v>0</v>
       </c>
       <c r="E11" s="54" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="F11" s="54" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="J11" s="52"/>
     </row>
@@ -7474,10 +7635,10 @@
         <v>2</v>
       </c>
       <c r="B12" s="62" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C12" s="55" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D12" s="55" t="b">
         <v>0</v>
@@ -7489,10 +7650,10 @@
         <v>3</v>
       </c>
       <c r="B13" s="62" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C13" s="55" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D13" s="55" t="b">
         <v>0</v>
@@ -7504,10 +7665,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="62" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C14" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D14" s="55" t="b">
         <v>0</v>
@@ -7519,10 +7680,10 @@
         <v>5</v>
       </c>
       <c r="B15" s="62" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C15" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D15" s="55" t="b">
         <v>0</v>
@@ -7534,10 +7695,10 @@
         <v>6</v>
       </c>
       <c r="B16" s="62" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C16" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D16" s="55" t="b">
         <v>0</v>
@@ -7548,7 +7709,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="73" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C17" s="58"/>
       <c r="D17" s="58" t="b">
@@ -7565,7 +7726,7 @@
         <v>0</v>
       </c>
       <c r="B18" s="74" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C18" s="53"/>
       <c r="D18" s="54"/>
@@ -7576,19 +7737,19 @@
         <v>1</v>
       </c>
       <c r="B19" s="62" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C19" s="55" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D19" s="55" t="b">
         <v>0</v>
       </c>
       <c r="F19" s="54" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G19" s="54" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7596,16 +7757,16 @@
         <v>2</v>
       </c>
       <c r="B20" s="62" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C20" s="56" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D20" s="54" t="b">
         <v>1</v>
       </c>
       <c r="E20" s="54" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7613,10 +7774,10 @@
         <v>3</v>
       </c>
       <c r="B21" s="62" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C21" s="55" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D21" s="55" t="b">
         <v>0</v>
@@ -7627,10 +7788,10 @@
         <v>4</v>
       </c>
       <c r="B22" s="62" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C22" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D22" s="55" t="b">
         <v>0</v>
@@ -7641,10 +7802,10 @@
         <v>5</v>
       </c>
       <c r="B23" s="62" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C23" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D23" s="55" t="b">
         <v>0</v>
@@ -7655,10 +7816,10 @@
         <v>6</v>
       </c>
       <c r="B24" s="62" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C24" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D24" s="55" t="b">
         <v>0</v>
@@ -7669,16 +7830,16 @@
         <v>7</v>
       </c>
       <c r="B25" s="73" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C25" s="64" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D25" s="59" t="b">
         <v>1</v>
       </c>
       <c r="E25" s="59" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="F25" s="59"/>
       <c r="G25" s="59"/>
@@ -7690,7 +7851,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="74" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C26" s="53"/>
       <c r="D26" s="54"/>
@@ -7701,19 +7862,19 @@
         <v>1</v>
       </c>
       <c r="B27" s="62" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C27" s="55" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D27" s="55" t="b">
         <v>0</v>
       </c>
       <c r="F27" s="54" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G27" s="54" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7721,19 +7882,19 @@
         <v>2</v>
       </c>
       <c r="B28" s="62" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C28" s="55" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D28" s="55" t="b">
         <v>0</v>
       </c>
       <c r="E28" s="54" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F28" s="54" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7741,10 +7902,10 @@
         <v>3</v>
       </c>
       <c r="B29" s="62" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C29" s="55" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D29" s="55" t="b">
         <v>0</v>
@@ -7755,10 +7916,10 @@
         <v>4</v>
       </c>
       <c r="B30" s="62" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C30" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D30" s="55" t="b">
         <v>0</v>
@@ -7769,10 +7930,10 @@
         <v>5</v>
       </c>
       <c r="B31" s="62" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C31" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D31" s="55" t="b">
         <v>0</v>
@@ -7783,10 +7944,10 @@
         <v>6</v>
       </c>
       <c r="B32" s="62" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C32" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D32" s="55" t="b">
         <v>0</v>
@@ -7797,10 +7958,10 @@
         <v>7</v>
       </c>
       <c r="B33" s="73" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C33" s="58" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D33" s="58" t="b">
         <v>0</v>
@@ -7816,7 +7977,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="74" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C34" s="53"/>
       <c r="D34" s="54"/>
@@ -7827,19 +7988,19 @@
         <v>1</v>
       </c>
       <c r="B35" s="62" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C35" s="55" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D35" s="55" t="b">
         <v>0</v>
       </c>
       <c r="F35" s="54" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G35" s="54" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7847,22 +8008,22 @@
         <v>2</v>
       </c>
       <c r="B36" s="62" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C36" s="56" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D36" s="54" t="b">
         <v>1</v>
       </c>
       <c r="E36" s="54" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F36" s="54" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="G36" s="54" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7870,19 +8031,19 @@
         <v>3</v>
       </c>
       <c r="B37" s="62" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C37" s="55" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D37" s="55" t="b">
         <v>0</v>
       </c>
       <c r="E37" s="54" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="G37" s="54" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7890,10 +8051,10 @@
         <v>4</v>
       </c>
       <c r="B38" s="62" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C38" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D38" s="55" t="b">
         <v>0</v>
@@ -7904,10 +8065,10 @@
         <v>5</v>
       </c>
       <c r="B39" s="62" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C39" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D39" s="55" t="b">
         <v>0</v>
@@ -7918,10 +8079,10 @@
         <v>6</v>
       </c>
       <c r="B40" s="62" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C40" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D40" s="55" t="b">
         <v>0</v>
@@ -7932,16 +8093,16 @@
         <v>7</v>
       </c>
       <c r="B41" s="73" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C41" s="64" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D41" s="59" t="b">
         <v>1</v>
       </c>
       <c r="E41" s="59" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="F41" s="59"/>
       <c r="G41" s="59"/>
@@ -7953,7 +8114,7 @@
         <v>0</v>
       </c>
       <c r="B42" s="74" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C42" s="53"/>
       <c r="D42" s="54"/>
@@ -7964,19 +8125,19 @@
         <v>1</v>
       </c>
       <c r="B43" s="62" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C43" s="55" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D43" s="55" t="b">
         <v>0</v>
       </c>
       <c r="F43" s="54" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G43" s="54" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7984,19 +8145,19 @@
         <v>2</v>
       </c>
       <c r="B44" s="62" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C44" s="56" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D44" s="54" t="b">
         <v>1</v>
       </c>
       <c r="E44" s="54" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F44" s="54" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8004,16 +8165,16 @@
         <v>3</v>
       </c>
       <c r="B45" s="62" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C45" s="56" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D45" s="54" t="b">
         <v>1</v>
       </c>
       <c r="E45" s="54" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8021,10 +8182,10 @@
         <v>4</v>
       </c>
       <c r="B46" s="62" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C46" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D46" s="55" t="b">
         <v>0</v>
@@ -8035,10 +8196,10 @@
         <v>5</v>
       </c>
       <c r="B47" s="62" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C47" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D47" s="55" t="b">
         <v>0</v>
@@ -8049,10 +8210,10 @@
         <v>6</v>
       </c>
       <c r="B48" s="62" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C48" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D48" s="55" t="b">
         <v>0</v>
@@ -8063,16 +8224,16 @@
         <v>7</v>
       </c>
       <c r="B49" s="73" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C49" s="64" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D49" s="59" t="b">
         <v>1</v>
       </c>
       <c r="E49" s="59" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="F49" s="59"/>
       <c r="G49" s="59"/>
@@ -8084,7 +8245,7 @@
         <v>0</v>
       </c>
       <c r="B50" s="74" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C50" s="53"/>
       <c r="D50" s="54"/>
@@ -8095,19 +8256,19 @@
         <v>1</v>
       </c>
       <c r="B51" s="62" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C51" s="55" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D51" s="55" t="b">
         <v>0</v>
       </c>
       <c r="F51" s="54" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G51" s="54" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8115,19 +8276,19 @@
         <v>2</v>
       </c>
       <c r="B52" s="62" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C52" s="55" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D52" s="55" t="b">
         <v>0</v>
       </c>
       <c r="E52" s="54" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F52" s="54" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8135,19 +8296,19 @@
         <v>3</v>
       </c>
       <c r="B53" s="62" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C53" s="56" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D53" s="54" t="b">
         <v>1</v>
       </c>
       <c r="E53" s="54" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F53" s="54" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8155,16 +8316,16 @@
         <v>4</v>
       </c>
       <c r="B54" s="62" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C54" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D54" s="55" t="b">
         <v>0</v>
       </c>
       <c r="F54" s="54" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8172,16 +8333,16 @@
         <v>5</v>
       </c>
       <c r="B55" s="62" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C55" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D55" s="55" t="b">
         <v>0</v>
       </c>
       <c r="F55" s="54" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8189,16 +8350,16 @@
         <v>6</v>
       </c>
       <c r="B56" s="62" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C56" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D56" s="55" t="b">
         <v>0</v>
       </c>
       <c r="F56" s="54" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="57" spans="1:10" s="66" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8206,10 +8367,10 @@
         <v>7</v>
       </c>
       <c r="B57" s="73" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C57" s="58" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D57" s="58" t="b">
         <v>0</v>
@@ -8225,7 +8386,7 @@
         <v>0</v>
       </c>
       <c r="B58" s="74" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C58" s="53"/>
       <c r="D58" s="54"/>
@@ -8236,22 +8397,22 @@
         <v>1</v>
       </c>
       <c r="B59" s="62" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C59" s="56" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D59" s="56" t="b">
         <v>1</v>
       </c>
       <c r="E59" s="54" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="F59" s="54" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G59" s="54" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8259,17 +8420,17 @@
         <v>2</v>
       </c>
       <c r="B60" s="62" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C60" s="55"/>
       <c r="D60" s="55" t="b">
         <v>0</v>
       </c>
       <c r="E60" s="54" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F60" s="54" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8277,17 +8438,17 @@
         <v>3</v>
       </c>
       <c r="B61" s="62" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C61" s="55"/>
       <c r="D61" s="55" t="b">
         <v>0</v>
       </c>
       <c r="F61" s="54" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="G61" s="54" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8295,22 +8456,22 @@
         <v>4</v>
       </c>
       <c r="B62" s="62" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C62" s="56" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D62" s="54" t="b">
         <v>1</v>
       </c>
       <c r="E62" s="54" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F62" s="54" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="G62" s="54" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8318,22 +8479,22 @@
         <v>5</v>
       </c>
       <c r="B63" s="62" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C63" s="56" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D63" s="54" t="b">
         <v>1</v>
       </c>
       <c r="E63" s="54" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="F63" s="54" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="G63" s="54" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8341,22 +8502,22 @@
         <v>6</v>
       </c>
       <c r="B64" s="62" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C64" s="56" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D64" s="54" t="b">
         <v>1</v>
       </c>
       <c r="E64" s="54" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="F64" s="54" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G64" s="54" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="65" spans="1:10" s="66" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8364,16 +8525,16 @@
         <v>7</v>
       </c>
       <c r="B65" s="73" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C65" s="64" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D65" s="59" t="b">
         <v>1</v>
       </c>
       <c r="E65" s="59" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F65" s="59"/>
       <c r="G65" s="59"/>
@@ -8385,7 +8546,7 @@
         <v>0</v>
       </c>
       <c r="B66" s="75" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C66" s="53"/>
       <c r="D66" s="54" t="b">
@@ -8398,19 +8559,19 @@
         <v>1</v>
       </c>
       <c r="B67" s="62" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C67" s="56" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D67" s="56" t="b">
         <v>1</v>
       </c>
       <c r="F67" s="54" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G67" s="54" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8418,14 +8579,14 @@
         <v>2</v>
       </c>
       <c r="B68" s="62" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C68" s="55"/>
       <c r="D68" s="55" t="b">
         <v>0</v>
       </c>
       <c r="F68" s="54" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8433,17 +8594,17 @@
         <v>3</v>
       </c>
       <c r="B69" s="62" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C69" s="55"/>
       <c r="D69" s="55" t="b">
         <v>0</v>
       </c>
       <c r="F69" s="54" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="G69" s="54" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8451,22 +8612,22 @@
         <v>4</v>
       </c>
       <c r="B70" s="62" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C70" s="56" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D70" s="54" t="b">
         <v>1</v>
       </c>
       <c r="E70" s="54" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F70" s="54" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="G70" s="54" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8474,22 +8635,22 @@
         <v>5</v>
       </c>
       <c r="B71" s="62" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C71" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D71" s="55" t="b">
         <v>0</v>
       </c>
       <c r="E71" s="54" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F71" s="54" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="G71" s="54" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8497,22 +8658,22 @@
         <v>6</v>
       </c>
       <c r="B72" s="62" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C72" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D72" s="55" t="b">
         <v>0</v>
       </c>
       <c r="E72" s="54" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F72" s="54" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G72" s="54" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="73" spans="1:10" s="66" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8520,16 +8681,16 @@
         <v>7</v>
       </c>
       <c r="B73" s="73" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C73" s="64" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D73" s="59" t="b">
         <v>1</v>
       </c>
       <c r="E73" s="59" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F73" s="59"/>
       <c r="G73" s="59"/>
@@ -8541,7 +8702,7 @@
         <v>0</v>
       </c>
       <c r="B74" s="75" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C74" s="53"/>
       <c r="F74" s="53"/>
@@ -8552,19 +8713,19 @@
         <v>1</v>
       </c>
       <c r="B75" s="62" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C75" s="56" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D75" s="56" t="b">
         <v>1</v>
       </c>
       <c r="F75" s="54" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G75" s="54" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8572,14 +8733,14 @@
         <v>2</v>
       </c>
       <c r="B76" s="62" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C76" s="55"/>
       <c r="D76" s="55" t="b">
         <v>0</v>
       </c>
       <c r="F76" s="54" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8587,17 +8748,17 @@
         <v>3</v>
       </c>
       <c r="B77" s="62" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C77" s="55"/>
       <c r="D77" s="55" t="b">
         <v>0</v>
       </c>
       <c r="F77" s="54" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="G77" s="54" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8605,22 +8766,22 @@
         <v>4</v>
       </c>
       <c r="B78" s="62" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C78" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D78" s="55" t="b">
         <v>0</v>
       </c>
       <c r="E78" s="54" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="F78" s="54" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="G78" s="54" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8628,22 +8789,22 @@
         <v>5</v>
       </c>
       <c r="B79" s="62" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C79" s="56" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D79" s="54" t="b">
         <v>1</v>
       </c>
       <c r="E79" s="54" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F79" s="54" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="G79" s="54" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8651,22 +8812,22 @@
         <v>6</v>
       </c>
       <c r="B80" s="62" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C80" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D80" s="55" t="b">
         <v>0</v>
       </c>
       <c r="E80" s="54" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="F80" s="54" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G80" s="54" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="81" spans="1:10" s="66" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8674,16 +8835,16 @@
         <v>7</v>
       </c>
       <c r="B81" s="73" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C81" s="64" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D81" s="59" t="b">
         <v>1</v>
       </c>
       <c r="E81" s="59" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F81" s="59"/>
       <c r="G81" s="59"/>
@@ -8695,7 +8856,7 @@
         <v>0</v>
       </c>
       <c r="B82" s="75" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C82" s="53"/>
       <c r="D82" s="54" t="b">
@@ -8708,19 +8869,19 @@
         <v>1</v>
       </c>
       <c r="B83" s="62" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C83" s="56" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D83" s="56" t="b">
         <v>1</v>
       </c>
       <c r="F83" s="54" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G83" s="54" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8728,14 +8889,14 @@
         <v>2</v>
       </c>
       <c r="B84" s="62" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C84" s="55"/>
       <c r="D84" s="55" t="b">
         <v>0</v>
       </c>
       <c r="F84" s="54" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8743,17 +8904,17 @@
         <v>3</v>
       </c>
       <c r="B85" s="62" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C85" s="55"/>
       <c r="D85" s="55" t="b">
         <v>0</v>
       </c>
       <c r="F85" s="54" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="G85" s="54" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8761,22 +8922,22 @@
         <v>4</v>
       </c>
       <c r="B86" s="62" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C86" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D86" s="55" t="b">
         <v>0</v>
       </c>
       <c r="E86" s="54" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="F86" s="54" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="G86" s="54" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8784,22 +8945,22 @@
         <v>5</v>
       </c>
       <c r="B87" s="62" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C87" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D87" s="55" t="b">
         <v>0</v>
       </c>
       <c r="E87" s="54" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="F87" s="54" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="G87" s="54" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8807,22 +8968,22 @@
         <v>6</v>
       </c>
       <c r="B88" s="62" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C88" s="56" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D88" s="54" t="b">
         <v>1</v>
       </c>
       <c r="E88" s="54" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F88" s="54" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G88" s="54" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="89" spans="1:10" s="66" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8830,16 +8991,16 @@
         <v>7</v>
       </c>
       <c r="B89" s="73" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C89" s="64" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D89" s="59" t="b">
         <v>1</v>
       </c>
       <c r="E89" s="59" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F89" s="59"/>
       <c r="G89" s="59"/>
@@ -8851,7 +9012,7 @@
         <v>0</v>
       </c>
       <c r="B90" s="75" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C90" s="53"/>
       <c r="D90" s="54" t="b">
@@ -8864,17 +9025,17 @@
         <v>1</v>
       </c>
       <c r="B91" s="62" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C91" s="57"/>
       <c r="D91" s="55" t="b">
         <v>0</v>
       </c>
       <c r="F91" s="54" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G91" s="54" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8882,14 +9043,14 @@
         <v>2</v>
       </c>
       <c r="B92" s="62" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C92" s="55"/>
       <c r="D92" s="55" t="b">
         <v>0</v>
       </c>
       <c r="F92" s="54" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8897,17 +9058,17 @@
         <v>3</v>
       </c>
       <c r="B93" s="62" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C93" s="55"/>
       <c r="D93" s="55" t="b">
         <v>0</v>
       </c>
       <c r="F93" s="54" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="G93" s="54" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8915,19 +9076,19 @@
         <v>4</v>
       </c>
       <c r="B94" s="62" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C94" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D94" s="55" t="b">
         <v>0</v>
       </c>
       <c r="F94" s="54" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G94" s="54" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8935,19 +9096,19 @@
         <v>5</v>
       </c>
       <c r="B95" s="62" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C95" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D95" s="55" t="b">
         <v>0</v>
       </c>
       <c r="F95" s="54" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="G95" s="54" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="96" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8955,19 +9116,19 @@
         <v>6</v>
       </c>
       <c r="B96" s="62" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C96" s="55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D96" s="55" t="b">
         <v>0</v>
       </c>
       <c r="F96" s="54" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="G96" s="54" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="97" spans="1:10" s="66" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -8975,19 +9136,19 @@
         <v>7</v>
       </c>
       <c r="B97" s="73" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C97" s="64" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D97" s="59" t="b">
         <v>1</v>
       </c>
       <c r="E97" s="59" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="F97" s="59" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="G97" s="59"/>
       <c r="H97" s="69"/>

</xml_diff>